<commit_message>
Tweaked_gaussian_sigma to 15 not 5
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Medium_Diads.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Medium_Diads.xlsx
@@ -708,97 +708,106 @@
         <v>36</v>
       </c>
       <c r="C2">
-        <v>103.5025689618885</v>
+        <v>103.5024783007825</v>
       </c>
       <c r="D2">
-        <v>1284.782388925229</v>
+        <v>1284.782172258474</v>
       </c>
       <c r="E2">
-        <v>2025.930543005324</v>
+        <v>2018.398940646917</v>
       </c>
       <c r="F2">
-        <v>1284.782438927729</v>
+        <v>1284.782322265974</v>
       </c>
       <c r="G2">
-        <v>6199.386713251325</v>
+        <v>5980.317313515023</v>
       </c>
       <c r="H2">
-        <v>1.18163776167961</v>
+        <v>1.184297945649272</v>
       </c>
       <c r="I2">
-        <v>6.174037294366258</v>
+        <v>4.062692183154739</v>
       </c>
       <c r="J2">
-        <v>0.554125426592036</v>
+        <v>0.4807357664803823</v>
       </c>
       <c r="K2">
-        <v>2.363275523359219</v>
+        <v>2.368595891298543</v>
       </c>
       <c r="L2" t="s">
         <v>70</v>
       </c>
       <c r="M2">
-        <v>1388.284957887117</v>
+        <v>1388.284850569257</v>
       </c>
       <c r="N2">
-        <v>4090.369929815822</v>
+        <v>4090.075344637342</v>
       </c>
       <c r="O2">
-        <v>1388.285007889617</v>
+        <v>1388.284800566757</v>
       </c>
       <c r="P2">
-        <v>9750.408856825492</v>
+        <v>9746.715099738554</v>
       </c>
       <c r="Q2">
-        <v>0.918253107009929</v>
+        <v>0.9183656625332973</v>
       </c>
       <c r="S2">
-        <v>5.933789614380768</v>
+        <v>5.26573787120255</v>
       </c>
       <c r="T2">
-        <v>0.5696802703821771</v>
+        <v>0.5686677646039512</v>
       </c>
       <c r="U2">
-        <v>1.836506214019858</v>
+        <v>1.836731325066595</v>
       </c>
       <c r="V2" t="s">
         <v>70</v>
       </c>
       <c r="W2">
-        <v>1264.759344556284</v>
+        <v>1264.769962759428</v>
       </c>
       <c r="X2">
-        <v>1123.966751022198</v>
+        <v>884.1918482706973</v>
       </c>
       <c r="Y2">
-        <v>1.985875150178413</v>
+        <v>1.654749619324631</v>
       </c>
       <c r="Z2">
-        <v>1409.687721872736</v>
+        <v>1409.686545952824</v>
       </c>
       <c r="AA2">
-        <v>1418.834832621418</v>
+        <v>1303.090060850297</v>
       </c>
       <c r="AB2">
-        <v>1.321391357850652</v>
+        <v>1.308510756802162</v>
       </c>
       <c r="AC2">
-        <v>1370.216263100838</v>
+        <v>1370.209319478406</v>
       </c>
       <c r="AD2">
-        <v>82.36124522318464</v>
+        <v>129.6283599249383</v>
       </c>
       <c r="AE2">
-        <v>0.4571501310278908</v>
+        <v>0.4571469641258965</v>
       </c>
       <c r="AF2">
-        <v>1381.067099035949</v>
+        <v>1388.864509793172</v>
       </c>
       <c r="AG2">
-        <v>857.6410667081138</v>
+        <v>1010.935773428285</v>
       </c>
       <c r="AH2">
-        <v>18.28600524111686</v>
+        <v>22.85749005022513</v>
+      </c>
+      <c r="AI2">
+        <v>1277.815715001517</v>
+      </c>
+      <c r="AJ2">
+        <v>854.9114794925182</v>
+      </c>
+      <c r="AK2">
+        <v>25.3312231309645</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -809,97 +818,106 @@
         <v>37</v>
       </c>
       <c r="C3">
-        <v>103.2408701534448</v>
+        <v>103.241203730686</v>
       </c>
       <c r="D3">
-        <v>1285.256598341661</v>
+        <v>1285.25618374382</v>
       </c>
       <c r="E3">
-        <v>1317.576469414435</v>
+        <v>1313.440205282461</v>
       </c>
       <c r="F3">
-        <v>1285.256648344161</v>
+        <v>1285.25623374632</v>
       </c>
       <c r="G3">
-        <v>3642.84329220333</v>
+        <v>3540.956695190708</v>
       </c>
       <c r="H3">
-        <v>1.069496423063685</v>
+        <v>1.072004796490421</v>
       </c>
       <c r="I3">
-        <v>5.158609223504361</v>
+        <v>4.269687861419299</v>
       </c>
       <c r="J3">
-        <v>0.5487698923278731</v>
+        <v>0.4895914501038657</v>
       </c>
       <c r="K3">
-        <v>2.13899284612737</v>
+        <v>2.144009592980841</v>
       </c>
       <c r="L3" t="s">
         <v>70</v>
       </c>
       <c r="M3">
-        <v>1388.497468495106</v>
+        <v>1388.497387474506</v>
       </c>
       <c r="N3">
-        <v>2608.966087165342</v>
+        <v>2609.134269858496</v>
       </c>
       <c r="O3">
-        <v>1388.497518497606</v>
+        <v>1388.497437477006</v>
       </c>
       <c r="P3">
-        <v>5592.732052043096</v>
+        <v>5597.58836885159</v>
       </c>
       <c r="Q3">
-        <v>0.8356942731022868</v>
+        <v>0.8357192953623533</v>
       </c>
       <c r="S3">
-        <v>4.64872007332885</v>
+        <v>4.441071720393375</v>
       </c>
       <c r="T3">
-        <v>0.5364802009744351</v>
+        <v>0.5379926699161535</v>
       </c>
       <c r="U3">
-        <v>1.671388546204574</v>
+        <v>1.671438590724707</v>
       </c>
       <c r="V3" t="s">
         <v>70</v>
       </c>
       <c r="W3">
-        <v>1265.210453470486</v>
+        <v>1265.225774860759</v>
       </c>
       <c r="X3">
-        <v>598.5488697718421</v>
+        <v>513.631957010207</v>
       </c>
       <c r="Y3">
-        <v>1.408205573925847</v>
+        <v>1.210758891212964</v>
       </c>
       <c r="Z3">
-        <v>1409.879972757741</v>
+        <v>1409.880142364874</v>
       </c>
       <c r="AA3">
-        <v>790.7253007324841</v>
+        <v>768.7364721983182</v>
       </c>
       <c r="AB3">
-        <v>1.018607256598498</v>
+        <v>1.015749198909018</v>
       </c>
       <c r="AC3">
-        <v>1370.328853839304</v>
+        <v>1370.311758300202</v>
       </c>
       <c r="AD3">
-        <v>59.10450208884415</v>
+        <v>71.55440107125425</v>
       </c>
       <c r="AE3">
-        <v>0.4165642773717119</v>
+        <v>0.4165587314187538</v>
       </c>
       <c r="AF3">
-        <v>1381.586904090171</v>
+        <v>1383.188233320925</v>
       </c>
       <c r="AG3">
-        <v>388.4006046616925</v>
+        <v>435.9559525320709</v>
       </c>
       <c r="AH3">
-        <v>16.66257109626212</v>
+        <v>20.82822862117945</v>
+      </c>
+      <c r="AI3">
+        <v>1278.358859035381</v>
+      </c>
+      <c r="AJ3">
+        <v>432.9793051810363</v>
+      </c>
+      <c r="AK3">
+        <v>26.64900151121823</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -910,97 +928,106 @@
         <v>38</v>
       </c>
       <c r="C4">
-        <v>103.7099875279018</v>
+        <v>103.7097849548909</v>
       </c>
       <c r="D4">
-        <v>1284.33869652025</v>
+        <v>1284.338721072538</v>
       </c>
       <c r="E4">
-        <v>922.5388884150183</v>
+        <v>921.2151674959711</v>
       </c>
       <c r="F4">
-        <v>1284.33874652275</v>
+        <v>1284.338771075038</v>
       </c>
       <c r="G4">
-        <v>2796.780946138135</v>
+        <v>2758.859907721517</v>
       </c>
       <c r="H4">
-        <v>1.148573355523057</v>
+        <v>1.149512800233293</v>
       </c>
       <c r="I4">
-        <v>2.149858991618257</v>
+        <v>1.976053998305405</v>
       </c>
       <c r="J4">
-        <v>0.6017597200607285</v>
+        <v>0.5750597548879123</v>
       </c>
       <c r="K4">
-        <v>2.297146711046114</v>
+        <v>2.299025600466587</v>
       </c>
       <c r="L4" t="s">
         <v>70</v>
       </c>
       <c r="M4">
-        <v>1388.048684048152</v>
+        <v>1388.048606032429</v>
       </c>
       <c r="N4">
-        <v>1856.707327568972</v>
+        <v>1856.907118355426</v>
       </c>
       <c r="O4">
-        <v>1388.048734050652</v>
+        <v>1388.048556029929</v>
       </c>
       <c r="P4">
-        <v>4492.531272381981</v>
+        <v>4498.770285811575</v>
       </c>
       <c r="Q4">
-        <v>0.9147651333746794</v>
+        <v>0.9147956328216451</v>
       </c>
       <c r="S4">
-        <v>2.910074067197035</v>
+        <v>2.674451765487926</v>
       </c>
       <c r="T4">
-        <v>0.6180914248070061</v>
+        <v>0.6204730671817161</v>
       </c>
       <c r="U4">
-        <v>1.829530266749359</v>
+        <v>1.82959126564329</v>
       </c>
       <c r="V4" t="s">
         <v>70</v>
       </c>
       <c r="W4">
-        <v>1264.206593043167</v>
+        <v>1264.204531009733</v>
       </c>
       <c r="X4">
-        <v>396.1825940116273</v>
+        <v>355.8514983518411</v>
       </c>
       <c r="Y4">
-        <v>2.043592888209226</v>
+        <v>1.848851249111544</v>
       </c>
       <c r="Z4">
-        <v>1409.435170719134</v>
+        <v>1409.435604835722</v>
       </c>
       <c r="AA4">
-        <v>522.47794692862</v>
+        <v>482.9231483694317</v>
       </c>
       <c r="AB4">
-        <v>1.522163713814284</v>
+        <v>1.47595477144973</v>
       </c>
       <c r="AC4">
-        <v>1370.222927306514</v>
+        <v>1370.215427675166</v>
       </c>
       <c r="AD4">
-        <v>37.62549301579845</v>
+        <v>59.21913710024698</v>
       </c>
       <c r="AE4">
-        <v>0.4561119863336153</v>
+        <v>0.4561112168908973</v>
       </c>
       <c r="AF4">
-        <v>1381.069031312506</v>
+        <v>1385.718866628749</v>
       </c>
       <c r="AG4">
-        <v>438.2423513853706</v>
+        <v>485.3411417411267</v>
       </c>
       <c r="AH4">
-        <v>18.24447945334965</v>
+        <v>22.80562769192313</v>
+      </c>
+      <c r="AI4">
+        <v>1277.272514005475</v>
+      </c>
+      <c r="AJ4">
+        <v>126.2131343824071</v>
+      </c>
+      <c r="AK4">
+        <v>20.30337238308007</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -1011,97 +1038,106 @@
         <v>39</v>
       </c>
       <c r="C5">
-        <v>104.3060271332999</v>
+        <v>104.3058897395076</v>
       </c>
       <c r="D5">
-        <v>1283.014098975203</v>
+        <v>1283.01415126552</v>
       </c>
       <c r="E5">
-        <v>3855.511898196052</v>
+        <v>3843.550907239086</v>
       </c>
       <c r="F5">
-        <v>1283.014148977703</v>
+        <v>1283.01420126802</v>
       </c>
       <c r="G5">
-        <v>12127.95159996322</v>
+        <v>11738.34486599075</v>
       </c>
       <c r="H5">
-        <v>1.133723206924789</v>
+        <v>1.134837012651443</v>
       </c>
       <c r="I5">
-        <v>8.872396576918739</v>
+        <v>4.735342690926224</v>
       </c>
       <c r="J5">
-        <v>0.7247845442082594</v>
+        <v>0.6660075012197993</v>
       </c>
       <c r="K5">
-        <v>2.267446413849577</v>
+        <v>2.269674025302885</v>
       </c>
       <c r="L5" t="s">
         <v>70</v>
       </c>
       <c r="M5">
-        <v>1387.320126108503</v>
+        <v>1387.320141010028</v>
       </c>
       <c r="N5">
-        <v>7643.360015025801</v>
+        <v>7644.197260719631</v>
       </c>
       <c r="O5">
-        <v>1387.320176111003</v>
+        <v>1387.320091007527</v>
       </c>
       <c r="P5">
-        <v>20249.28831936628</v>
+        <v>20273.34139890141</v>
       </c>
       <c r="Q5">
-        <v>0.9750231309121666</v>
+        <v>0.9750071341058354</v>
       </c>
       <c r="S5">
-        <v>7.102088517422658</v>
+        <v>6.417918385283629</v>
       </c>
       <c r="T5">
-        <v>0.6858244159488549</v>
+        <v>0.6878981216539291</v>
       </c>
       <c r="U5">
-        <v>1.950046261824333</v>
+        <v>1.950014268211671</v>
       </c>
       <c r="V5" t="s">
         <v>70</v>
       </c>
       <c r="W5">
-        <v>1262.990788630961</v>
+        <v>1262.921740277488</v>
       </c>
       <c r="X5">
-        <v>1865.106852057118</v>
+        <v>1334.23832032686</v>
       </c>
       <c r="Y5">
-        <v>3.216774848055126</v>
+        <v>2.347241584824356</v>
       </c>
       <c r="Z5">
-        <v>1408.695696838017</v>
+        <v>1408.694666792349</v>
       </c>
       <c r="AA5">
-        <v>2130.185016069041</v>
+        <v>2052.297819122209</v>
       </c>
       <c r="AB5">
-        <v>2.11707261529676</v>
+        <v>2.101959562081314</v>
       </c>
       <c r="AC5">
-        <v>1369.676470450547</v>
+        <v>1369.671894320785</v>
       </c>
       <c r="AD5">
-        <v>143.9840049404786</v>
+        <v>226.6181337309631</v>
       </c>
       <c r="AE5">
-        <v>0.4859899320463625</v>
+        <v>0.485989624035731</v>
       </c>
       <c r="AF5">
-        <v>1383.032666221383</v>
+        <v>1385.102514204258</v>
       </c>
       <c r="AG5">
-        <v>2042.561816307338</v>
+        <v>2029.148160961093</v>
       </c>
       <c r="AH5">
-        <v>19.03225120073381</v>
+        <v>20.05639204536351</v>
+      </c>
+      <c r="AI5">
+        <v>1279.740772591193</v>
+      </c>
+      <c r="AJ5">
+        <v>1401.000507597325</v>
+      </c>
+      <c r="AK5">
+        <v>21.61710556870263</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1112,97 +1148,106 @@
         <v>40</v>
       </c>
       <c r="C6">
-        <v>104.2506500451982</v>
+        <v>104.2504798746418</v>
       </c>
       <c r="D6">
-        <v>1283.138802697714</v>
+        <v>1283.138864066844</v>
       </c>
       <c r="E6">
-        <v>3192.10368582654</v>
+        <v>3182.483939699866</v>
       </c>
       <c r="F6">
-        <v>1283.138852700215</v>
+        <v>1283.138914069344</v>
       </c>
       <c r="G6">
-        <v>10152.57710760084</v>
+        <v>9826.782049396796</v>
       </c>
       <c r="H6">
-        <v>1.166999541924315</v>
+        <v>1.167995820163469</v>
       </c>
       <c r="I6">
-        <v>7.152845904294082</v>
+        <v>4.426803885308346</v>
       </c>
       <c r="J6">
-        <v>0.681626636669165</v>
+        <v>0.6217960666678791</v>
       </c>
       <c r="K6">
-        <v>2.33399908384863</v>
+        <v>2.335991640326937</v>
       </c>
       <c r="L6" t="s">
         <v>70</v>
       </c>
       <c r="M6">
-        <v>1387.389452742913</v>
+        <v>1387.389343941486</v>
       </c>
       <c r="N6">
-        <v>6474.677688250504</v>
+        <v>6475.454388598406</v>
       </c>
       <c r="O6">
-        <v>1387.389502745413</v>
+        <v>1387.389393943986</v>
       </c>
       <c r="P6">
-        <v>17102.14601231299</v>
+        <v>17124.98970236774</v>
       </c>
       <c r="Q6">
-        <v>0.9641187744220386</v>
+        <v>0.9641105596980557</v>
       </c>
       <c r="S6">
-        <v>5.794216514871439</v>
+        <v>5.210615402469444</v>
       </c>
       <c r="T6">
-        <v>0.7040099915112425</v>
+        <v>0.7063006132273106</v>
       </c>
       <c r="U6">
-        <v>1.928237548844077</v>
+        <v>1.928221119396111</v>
       </c>
       <c r="V6" t="s">
         <v>70</v>
       </c>
       <c r="W6">
-        <v>1263.128287369341</v>
+        <v>1263.072175943932</v>
       </c>
       <c r="X6">
-        <v>1497.859148991304</v>
+        <v>1123.833410494608</v>
       </c>
       <c r="Y6">
-        <v>3.031434524901154</v>
+        <v>2.310619860981791</v>
       </c>
       <c r="Z6">
-        <v>1408.763931974687</v>
+        <v>1408.765875043263</v>
       </c>
       <c r="AA6">
-        <v>1868.957711181531</v>
+        <v>1821.463001202329</v>
       </c>
       <c r="AB6">
-        <v>2.095882684314504</v>
+        <v>2.050546655578875</v>
       </c>
       <c r="AC6">
-        <v>1369.752564041607</v>
+        <v>1369.725886882306</v>
       </c>
       <c r="AD6">
-        <v>135.8368053080717</v>
+        <v>212.7279713052085</v>
       </c>
       <c r="AE6">
-        <v>0.4807221701503044</v>
+        <v>0.4807219130162296</v>
       </c>
       <c r="AF6">
-        <v>1380.707117451341</v>
+        <v>1382.774668879995</v>
       </c>
       <c r="AG6">
-        <v>1481.413683857086</v>
+        <v>1446.699273817374</v>
       </c>
       <c r="AH6">
-        <v>18.02987466387137</v>
+        <v>19.39488655960258</v>
+      </c>
+      <c r="AI6">
+        <v>1280.870351408255</v>
+      </c>
+      <c r="AJ6">
+        <v>1044.074236624445</v>
+      </c>
+      <c r="AK6">
+        <v>20.0706244144023</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -1213,97 +1258,106 @@
         <v>41</v>
       </c>
       <c r="C7">
-        <v>104.0261008035116</v>
+        <v>104.0258394810348</v>
       </c>
       <c r="D7">
-        <v>1283.619935291661</v>
+        <v>1283.619982895231</v>
       </c>
       <c r="E7">
-        <v>3209.207185750962</v>
+        <v>3198.615580589591</v>
       </c>
       <c r="F7">
-        <v>1283.619985294162</v>
+        <v>1283.620132902732</v>
       </c>
       <c r="G7">
-        <v>10496.96196234382</v>
+        <v>10144.49670587649</v>
       </c>
       <c r="H7">
-        <v>1.22607805986422</v>
+        <v>1.22773004064868</v>
       </c>
       <c r="I7">
-        <v>6.968231223748575</v>
+        <v>3.498183215279531</v>
       </c>
       <c r="J7">
-        <v>0.6292488603298091</v>
+        <v>0.5640158350157751</v>
       </c>
       <c r="K7">
-        <v>2.45215611972844</v>
+        <v>2.455460081297359</v>
       </c>
       <c r="L7" t="s">
         <v>70</v>
       </c>
       <c r="M7">
-        <v>1387.646036095173</v>
+        <v>1387.645922381266</v>
       </c>
       <c r="N7">
-        <v>6595.495883792571</v>
+        <v>6596.248834847829</v>
       </c>
       <c r="O7">
-        <v>1387.646086097673</v>
+        <v>1387.645972383767</v>
       </c>
       <c r="P7">
-        <v>17036.91433347062</v>
+        <v>17059.08781255781</v>
       </c>
       <c r="Q7">
-        <v>0.9696603206985176</v>
+        <v>0.9696539966807418</v>
       </c>
       <c r="S7">
-        <v>6.704021322960319</v>
+        <v>6.162703870379673</v>
       </c>
       <c r="T7">
-        <v>0.6359338686722541</v>
+        <v>0.6382401269637302</v>
       </c>
       <c r="U7">
-        <v>1.939320641397035</v>
+        <v>1.939307993361484</v>
       </c>
       <c r="V7" t="s">
         <v>70</v>
       </c>
       <c r="W7">
-        <v>1263.585882120312</v>
+        <v>1263.554614989503</v>
       </c>
       <c r="X7">
-        <v>1555.250404510655</v>
+        <v>1124.28994648788</v>
       </c>
       <c r="Y7">
-        <v>2.836405752640114</v>
+        <v>2.085702172638559</v>
       </c>
       <c r="Z7">
-        <v>1409.064939307804</v>
+        <v>1409.066120157815</v>
       </c>
       <c r="AA7">
-        <v>1797.893994932811</v>
+        <v>1728.104617489085</v>
       </c>
       <c r="AB7">
-        <v>1.819326499801938</v>
+        <v>1.784273261137982</v>
       </c>
       <c r="AC7">
-        <v>1369.866821418466</v>
+        <v>1369.811826208155</v>
       </c>
       <c r="AD7">
-        <v>137.0218405710265</v>
+        <v>209.4466927251703</v>
       </c>
       <c r="AE7">
-        <v>0.483348950995418</v>
+        <v>0.4833479077639835</v>
       </c>
       <c r="AF7">
-        <v>1381.604655967008</v>
+        <v>1384.15220257645</v>
       </c>
       <c r="AG7">
-        <v>1548.049141069473</v>
+        <v>1553.76770654053</v>
       </c>
       <c r="AH7">
-        <v>18.26458515501248</v>
+        <v>20.06169556624405</v>
+      </c>
+      <c r="AI7">
+        <v>1278.673484509746</v>
+      </c>
+      <c r="AJ7">
+        <v>1227.685595445894</v>
+      </c>
+      <c r="AK7">
+        <v>22.54762723332253</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -1314,97 +1368,106 @@
         <v>42</v>
       </c>
       <c r="C8">
-        <v>103.9609886880908</v>
+        <v>103.9608143288494</v>
       </c>
       <c r="D8">
-        <v>1283.770208587817</v>
+        <v>1283.770186710841</v>
       </c>
       <c r="E8">
-        <v>2948.602509224464</v>
+        <v>2939.228698271468</v>
       </c>
       <c r="F8">
-        <v>1283.770258590317</v>
+        <v>1283.770336718341</v>
       </c>
       <c r="G8">
-        <v>9635.715006266639</v>
+        <v>9333.508586768445</v>
       </c>
       <c r="H8">
-        <v>1.235464364053505</v>
+        <v>1.237347830323499</v>
       </c>
       <c r="I8">
-        <v>5.928189262917473</v>
+        <v>2.79971205979286</v>
       </c>
       <c r="J8">
-        <v>0.6078943201575746</v>
+        <v>0.5459720181244645</v>
       </c>
       <c r="K8">
-        <v>2.470928728107009</v>
+        <v>2.474695660646997</v>
       </c>
       <c r="L8" t="s">
         <v>70</v>
       </c>
       <c r="M8">
-        <v>1387.731197275908</v>
+        <v>1387.731101044691</v>
       </c>
       <c r="N8">
-        <v>6076.290864013416</v>
+        <v>6077.169824362888</v>
       </c>
       <c r="O8">
-        <v>1387.731247278408</v>
+        <v>1387.731151047191</v>
       </c>
       <c r="P8">
-        <v>15601.74545969024</v>
+        <v>15625.44969886349</v>
       </c>
       <c r="Q8">
-        <v>0.9678311722689541</v>
+        <v>0.9677959294644471</v>
       </c>
       <c r="S8">
-        <v>6.550207316371936</v>
+        <v>5.945522271392369</v>
       </c>
       <c r="T8">
-        <v>0.6260202304851048</v>
+        <v>0.628778589156616</v>
       </c>
       <c r="U8">
-        <v>1.935662344537908</v>
+        <v>1.935591858928894</v>
       </c>
       <c r="V8" t="s">
         <v>70</v>
       </c>
       <c r="W8">
-        <v>1263.740894691031</v>
+        <v>1263.719839918262</v>
       </c>
       <c r="X8">
-        <v>1402.08490823713</v>
+        <v>1034.585738307424</v>
       </c>
       <c r="Y8">
-        <v>2.738354435184113</v>
+        <v>2.058926607601635</v>
       </c>
       <c r="Z8">
-        <v>1409.164324327029</v>
+        <v>1409.164174491246</v>
       </c>
       <c r="AA8">
-        <v>1635.649251609585</v>
+        <v>1582.120112329646</v>
       </c>
       <c r="AB8">
-        <v>1.710196487615742</v>
+        <v>1.683111846455375</v>
       </c>
       <c r="AC8">
-        <v>1369.902330680147</v>
+        <v>1369.82228382959</v>
       </c>
       <c r="AD8">
-        <v>117.6166219925424</v>
+        <v>185.118177598445</v>
       </c>
       <c r="AE8">
-        <v>0.4821085795261653</v>
+        <v>0.4821085697721401</v>
       </c>
       <c r="AF8">
-        <v>1382.495213991876</v>
+        <v>1384.936342243457</v>
       </c>
       <c r="AG8">
-        <v>1519.449357206128</v>
+        <v>1512.189719754705</v>
       </c>
       <c r="AH8">
-        <v>19.28004406973114</v>
+        <v>20.92219162897494</v>
+      </c>
+      <c r="AI8">
+        <v>1278.098156586957</v>
+      </c>
+      <c r="AJ8">
+        <v>1072.402720903121</v>
+      </c>
+      <c r="AK8">
+        <v>23.12412444985227</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -1415,97 +1478,106 @@
         <v>43</v>
       </c>
       <c r="C9">
-        <v>103.8722973410058</v>
+        <v>103.8721178978426</v>
       </c>
       <c r="D9">
-        <v>1283.955865057428</v>
+        <v>1283.955837607395</v>
       </c>
       <c r="E9">
-        <v>2397.431322178775</v>
+        <v>2389.825409531364</v>
       </c>
       <c r="F9">
-        <v>1283.955915059928</v>
+        <v>1283.955987614896</v>
       </c>
       <c r="G9">
-        <v>7860.986761498461</v>
+        <v>7617.001462314839</v>
       </c>
       <c r="H9">
-        <v>1.243544288116456</v>
+        <v>1.245507991580291</v>
       </c>
       <c r="I9">
-        <v>5.021999120214767</v>
+        <v>2.715942756242247</v>
       </c>
       <c r="J9">
-        <v>0.5999532925072359</v>
+        <v>0.5383397482313288</v>
       </c>
       <c r="K9">
-        <v>2.487088576232912</v>
+        <v>2.491015983160582</v>
       </c>
       <c r="L9" t="s">
         <v>70</v>
       </c>
       <c r="M9">
-        <v>1387.828162398434</v>
+        <v>1387.828055510238</v>
       </c>
       <c r="N9">
-        <v>4953.441424910835</v>
+        <v>4954.248378664242</v>
       </c>
       <c r="O9">
-        <v>1387.828212400934</v>
+        <v>1387.828105512738</v>
       </c>
       <c r="P9">
-        <v>12616.36236221711</v>
+        <v>12638.19344592967</v>
       </c>
       <c r="Q9">
-        <v>0.9625894389478331</v>
+        <v>0.9625556516540861</v>
       </c>
       <c r="S9">
-        <v>5.385645212180648</v>
+        <v>5.021804043684627</v>
       </c>
       <c r="T9">
-        <v>0.6187268264329916</v>
+        <v>0.6218593870041802</v>
       </c>
       <c r="U9">
-        <v>1.925178877895666</v>
+        <v>1.925111303308172</v>
       </c>
       <c r="V9" t="s">
         <v>70</v>
       </c>
       <c r="W9">
-        <v>1263.952299812286</v>
+        <v>1263.953449475129</v>
       </c>
       <c r="X9">
-        <v>1132.449631833486</v>
+        <v>827.4068150950312</v>
       </c>
       <c r="Y9">
-        <v>2.669096555037808</v>
+        <v>1.983839837723862</v>
       </c>
       <c r="Z9">
-        <v>1409.227116375052</v>
+        <v>1409.22826488335</v>
       </c>
       <c r="AA9">
-        <v>1325.427157122384</v>
+        <v>1283.505032388621</v>
       </c>
       <c r="AB9">
-        <v>1.629288018792084</v>
+        <v>1.582671591780085</v>
       </c>
       <c r="AC9">
-        <v>1369.978698809441</v>
+        <v>1370.05114608459</v>
       </c>
       <c r="AD9">
-        <v>100.285146464421</v>
+        <v>152.8894569602154</v>
       </c>
       <c r="AE9">
-        <v>0.4795094301013614</v>
+        <v>0.4795093710834263</v>
       </c>
       <c r="AF9">
-        <v>1381.998547094443</v>
+        <v>1384.605524383677</v>
       </c>
       <c r="AG9">
-        <v>1174.028532308689</v>
+        <v>1182.664618999205</v>
       </c>
       <c r="AH9">
-        <v>19.1803772009248</v>
+        <v>21.51749288234376</v>
+      </c>
+      <c r="AI9">
+        <v>1276.891507981919</v>
+      </c>
+      <c r="AJ9">
+        <v>879.4415304878179</v>
+      </c>
+      <c r="AK9">
+        <v>23.25254915719977</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -1516,97 +1588,106 @@
         <v>44</v>
       </c>
       <c r="C10">
-        <v>103.7653722891787</v>
+        <v>103.765300165076</v>
       </c>
       <c r="D10">
-        <v>1284.202769855721</v>
+        <v>1284.202585994414</v>
       </c>
       <c r="E10">
-        <v>2099.513856336334</v>
+        <v>2092.64408228188</v>
       </c>
       <c r="F10">
-        <v>1284.202819858221</v>
+        <v>1284.202736001915</v>
       </c>
       <c r="G10">
-        <v>6755.619966651094</v>
+        <v>6542.198237642884</v>
       </c>
       <c r="H10">
-        <v>1.230297023613359</v>
+        <v>1.23248249834218</v>
       </c>
       <c r="I10">
-        <v>5.039787623157244</v>
+        <v>3.057808898585026</v>
       </c>
       <c r="J10">
-        <v>0.5790388356243121</v>
+        <v>0.515194513742334</v>
       </c>
       <c r="K10">
-        <v>2.460594047226718</v>
+        <v>2.46496499668436</v>
       </c>
       <c r="L10" t="s">
         <v>70</v>
       </c>
       <c r="M10">
-        <v>1387.9681421449</v>
+        <v>1387.968086169491</v>
       </c>
       <c r="N10">
-        <v>4291.007471114089</v>
+        <v>4291.594559304483</v>
       </c>
       <c r="O10">
-        <v>1387.9681921474</v>
+        <v>1387.968036166991</v>
       </c>
       <c r="P10">
-        <v>10710.06709933581</v>
+        <v>10726.77331592671</v>
       </c>
       <c r="Q10">
-        <v>0.9486814543627063</v>
+        <v>0.9486746387666813</v>
       </c>
       <c r="S10">
-        <v>5.575023616495497</v>
+        <v>4.950767948786703</v>
       </c>
       <c r="T10">
-        <v>0.6036192141734393</v>
+        <v>0.6064139701009563</v>
       </c>
       <c r="U10">
-        <v>1.897362908725413</v>
+        <v>1.897349277533363</v>
       </c>
       <c r="V10" t="s">
         <v>70</v>
       </c>
       <c r="W10">
-        <v>1264.162073594684</v>
+        <v>1264.169444827622</v>
       </c>
       <c r="X10">
-        <v>930.6986702229433</v>
+        <v>689.160663506977</v>
       </c>
       <c r="Y10">
-        <v>2.300680232656277</v>
+        <v>1.795241573600231</v>
       </c>
       <c r="Z10">
-        <v>1409.403695502454</v>
+        <v>1409.402161042292</v>
       </c>
       <c r="AA10">
-        <v>1144.753573324406</v>
+        <v>1064.270619891727</v>
       </c>
       <c r="AB10">
-        <v>1.546950334693985</v>
+        <v>1.517191931284933</v>
       </c>
       <c r="AC10">
-        <v>1370.105900714638</v>
+        <v>1370.135130037444</v>
       </c>
       <c r="AD10">
-        <v>90.95286711259013</v>
+        <v>143.1511722440306</v>
       </c>
       <c r="AE10">
-        <v>0.4727749587328476</v>
+        <v>0.4727755114364375</v>
       </c>
       <c r="AF10">
-        <v>1381.057649092364</v>
+        <v>1385.796926751513</v>
       </c>
       <c r="AG10">
-        <v>947.4984317390167</v>
+        <v>1020.436747933544</v>
       </c>
       <c r="AH10">
-        <v>18.91099834931403</v>
+        <v>23.13745438635959</v>
+      </c>
+      <c r="AI10">
+        <v>1277.272516585797</v>
+      </c>
+      <c r="AJ10">
+        <v>761.4828300030192</v>
+      </c>
+      <c r="AK10">
+        <v>23.33414073286034</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -1617,97 +1698,106 @@
         <v>45</v>
       </c>
       <c r="C11">
-        <v>103.6685044393637</v>
+        <v>103.6685285315198</v>
       </c>
       <c r="D11">
-        <v>1284.419462899673</v>
+        <v>1284.419177167122</v>
       </c>
       <c r="E11">
-        <v>1872.823500404936</v>
+        <v>1865.985647369261</v>
       </c>
       <c r="F11">
-        <v>1284.419512902173</v>
+        <v>1284.419327174622</v>
       </c>
       <c r="G11">
-        <v>5888.636100031392</v>
+        <v>5681.14741975534</v>
       </c>
       <c r="H11">
-        <v>1.20499571769612</v>
+        <v>1.207459250445543</v>
       </c>
       <c r="I11">
-        <v>5.457535625401506</v>
+        <v>3.04569638483334</v>
       </c>
       <c r="J11">
-        <v>0.5732465027856082</v>
+        <v>0.5012555333631965</v>
       </c>
       <c r="K11">
-        <v>2.40999143539224</v>
+        <v>2.414918500891085</v>
       </c>
       <c r="L11" t="s">
         <v>70</v>
       </c>
       <c r="M11">
-        <v>1388.087967339036</v>
+        <v>1388.087905708642</v>
       </c>
       <c r="N11">
-        <v>3826.890288596453</v>
+        <v>3827.26181384214</v>
       </c>
       <c r="O11">
-        <v>1388.088017341536</v>
+        <v>1388.087855706142</v>
       </c>
       <c r="P11">
-        <v>9270.400406736069</v>
+        <v>9281.768904936946</v>
       </c>
       <c r="Q11">
-        <v>0.9275925297890572</v>
+        <v>0.9276102085919685</v>
       </c>
       <c r="S11">
-        <v>5.062781452212374</v>
+        <v>4.583681225782867</v>
       </c>
       <c r="T11">
-        <v>0.5847522964541959</v>
+        <v>0.5869222541514714</v>
       </c>
       <c r="U11">
-        <v>1.855185059578114</v>
+        <v>1.855220417183937</v>
       </c>
       <c r="V11" t="s">
         <v>70</v>
       </c>
       <c r="W11">
-        <v>1264.34420014005</v>
+        <v>1264.351665261633</v>
       </c>
       <c r="X11">
-        <v>860.6968304407931</v>
+        <v>627.4312002796938</v>
       </c>
       <c r="Y11">
-        <v>2.279667483211655</v>
+        <v>1.673581186233672</v>
       </c>
       <c r="Z11">
-        <v>1409.477686091423</v>
+        <v>1409.476083319527</v>
       </c>
       <c r="AA11">
-        <v>989.9279339607142</v>
+        <v>909.0470823440295</v>
       </c>
       <c r="AB11">
-        <v>1.483229619308736</v>
+        <v>1.468360153730507</v>
       </c>
       <c r="AC11">
-        <v>1370.153329272597</v>
+        <v>1370.166253403246</v>
       </c>
       <c r="AD11">
-        <v>72.14016588431608</v>
+        <v>113.542262963693</v>
       </c>
       <c r="AE11">
-        <v>0.4624834354461316</v>
+        <v>0.4624842750062863</v>
       </c>
       <c r="AF11">
-        <v>1381.055776631848</v>
+        <v>1386.066025228307</v>
       </c>
       <c r="AG11">
-        <v>799.393734294102</v>
+        <v>881.1121675198656</v>
       </c>
       <c r="AH11">
-        <v>18.0914504669856</v>
+        <v>22.50118858696616</v>
+      </c>
+      <c r="AI11">
+        <v>1277.272514051486</v>
+      </c>
+      <c r="AJ11">
+        <v>779.6599362360623</v>
+      </c>
+      <c r="AK11">
+        <v>24.42276353936427</v>
       </c>
     </row>
     <row r="12" spans="1:37">
@@ -1718,97 +1808,106 @@
         <v>46</v>
       </c>
       <c r="C12">
-        <v>103.600032236709</v>
+        <v>103.6001418639703</v>
       </c>
       <c r="D12">
-        <v>1284.569067650163</v>
+        <v>1284.568829779816</v>
       </c>
       <c r="E12">
-        <v>2596.54120906659</v>
+        <v>2589.208754617643</v>
       </c>
       <c r="F12">
-        <v>1284.569117652663</v>
+        <v>1284.568879782316</v>
       </c>
       <c r="G12">
-        <v>7917.262545926441</v>
+        <v>7710.639814300486</v>
       </c>
       <c r="H12">
-        <v>1.15795708577287</v>
+        <v>1.1600246682448</v>
       </c>
       <c r="I12">
-        <v>7.055884855661122</v>
+        <v>4.845378303957913</v>
       </c>
       <c r="J12">
-        <v>0.59595215502037</v>
+        <v>0.5431709619835757</v>
       </c>
       <c r="K12">
-        <v>2.315914171545739</v>
+        <v>2.320049336489601</v>
       </c>
       <c r="L12" t="s">
         <v>70</v>
       </c>
       <c r="M12">
-        <v>1388.169099886872</v>
+        <v>1388.168971643786</v>
       </c>
       <c r="N12">
-        <v>5248.259159128937</v>
+        <v>5249.141141965775</v>
       </c>
       <c r="O12">
-        <v>1388.169149889372</v>
+        <v>1388.169021646286</v>
       </c>
       <c r="P12">
-        <v>12470.87205137317</v>
+        <v>12494.7354458831</v>
       </c>
       <c r="Q12">
-        <v>0.9063630101600593</v>
+        <v>0.9063531345468943</v>
       </c>
       <c r="S12">
-        <v>7.327568262383606</v>
+        <v>6.704238681710057</v>
       </c>
       <c r="T12">
-        <v>0.5936278681637729</v>
+        <v>0.5970787275664307</v>
       </c>
       <c r="U12">
-        <v>1.812726020320119</v>
+        <v>1.812706269093789</v>
       </c>
       <c r="V12" t="s">
         <v>70</v>
       </c>
       <c r="W12">
-        <v>1264.458667643739</v>
+        <v>1264.474989551325</v>
       </c>
       <c r="X12">
-        <v>1112.706842261321</v>
+        <v>874.897865287019</v>
       </c>
       <c r="Y12">
-        <v>2.185948864918933</v>
+        <v>1.728585625129651</v>
       </c>
       <c r="Z12">
-        <v>1409.569670851406</v>
+        <v>1409.57127267474</v>
       </c>
       <c r="AA12">
-        <v>1330.672083814933</v>
+        <v>1271.107782242019</v>
       </c>
       <c r="AB12">
-        <v>1.373326659865822</v>
+        <v>1.317587563959992</v>
       </c>
       <c r="AC12">
-        <v>1370.160646691855</v>
+        <v>1370.170328785164</v>
       </c>
       <c r="AD12">
-        <v>111.8394034355986</v>
+        <v>174.729456533551</v>
       </c>
       <c r="AE12">
-        <v>0.4517302373503267</v>
+        <v>0.4517253368335039</v>
       </c>
       <c r="AF12">
-        <v>1381.054688557143</v>
+        <v>1385.085331958195</v>
       </c>
       <c r="AG12">
-        <v>1012.412835577029</v>
+        <v>1072.250870530101</v>
       </c>
       <c r="AH12">
-        <v>18.06920949397663</v>
+        <v>22.58652585234532</v>
+      </c>
+      <c r="AI12">
+        <v>1277.815715791181</v>
+      </c>
+      <c r="AJ12">
+        <v>833.4264750840827</v>
+      </c>
+      <c r="AK12">
+        <v>25.75142770882319</v>
       </c>
     </row>
     <row r="13" spans="1:37">
@@ -1819,97 +1918,106 @@
         <v>47</v>
       </c>
       <c r="C13">
-        <v>103.5463829613607</v>
+        <v>103.5464523439414</v>
       </c>
       <c r="D13">
-        <v>1284.69004373599</v>
+        <v>1284.689882625671</v>
       </c>
       <c r="E13">
-        <v>2488.932079831929</v>
+        <v>2484.238743698504</v>
       </c>
       <c r="F13">
-        <v>1284.69009373849</v>
+        <v>1284.689932628171</v>
       </c>
       <c r="G13">
-        <v>7369.344431686128</v>
+        <v>7245.748600297708</v>
       </c>
       <c r="H13">
-        <v>1.122558477825553</v>
+        <v>1.124030767858206</v>
       </c>
       <c r="I13">
-        <v>5.935128467005621</v>
+        <v>4.917580607240545</v>
       </c>
       <c r="J13">
-        <v>0.5996841243127965</v>
+        <v>0.565862371716394</v>
       </c>
       <c r="K13">
-        <v>2.245116955651107</v>
+        <v>2.248061535716413</v>
       </c>
       <c r="L13" t="s">
         <v>70</v>
       </c>
       <c r="M13">
-        <v>1388.23642669735</v>
+        <v>1388.236334969612</v>
       </c>
       <c r="N13">
-        <v>4936.987266419704</v>
+        <v>4938.325948963481</v>
       </c>
       <c r="O13">
-        <v>1388.236476699851</v>
+        <v>1388.236384972112</v>
       </c>
       <c r="P13">
-        <v>11445.24723041732</v>
+        <v>11476.06947007039</v>
       </c>
       <c r="Q13">
-        <v>0.887234262359641</v>
+        <v>0.8871354633258662</v>
       </c>
       <c r="S13">
-        <v>6.777523900461879</v>
+        <v>6.522319588412299</v>
       </c>
       <c r="T13">
-        <v>0.5847304027172852</v>
+        <v>0.5898237095572595</v>
       </c>
       <c r="U13">
-        <v>1.774468524719282</v>
+        <v>1.774270926651732</v>
       </c>
       <c r="V13" t="s">
         <v>70</v>
       </c>
       <c r="W13">
-        <v>1264.583921118047</v>
+        <v>1264.58916055485</v>
       </c>
       <c r="X13">
-        <v>933.5311777768709</v>
+        <v>800.6179457469588</v>
       </c>
       <c r="Y13">
-        <v>1.92113248495559</v>
+        <v>1.653103006581944</v>
       </c>
       <c r="Z13">
-        <v>1409.627129321759</v>
+        <v>1409.625464557969</v>
       </c>
       <c r="AA13">
-        <v>1193.904955025007</v>
+        <v>1147.551533887141</v>
       </c>
       <c r="AB13">
-        <v>1.342492514451655</v>
+        <v>1.334094952850222</v>
       </c>
       <c r="AC13">
-        <v>1370.22601292961</v>
+        <v>1370.218698051059</v>
       </c>
       <c r="AD13">
-        <v>94.80425363279934</v>
+        <v>149.2044771580624</v>
       </c>
       <c r="AE13">
-        <v>0.4420583109778212</v>
+        <v>0.4420581893904116</v>
       </c>
       <c r="AF13">
-        <v>1381.054675585953</v>
+        <v>1382.699595946567</v>
       </c>
       <c r="AG13">
-        <v>897.3974634016131</v>
+        <v>927.3392344554044</v>
       </c>
       <c r="AH13">
-        <v>17.68233239189748</v>
+        <v>22.10291825350417</v>
+      </c>
+      <c r="AI13">
+        <v>1277.81571609703</v>
+      </c>
+      <c r="AJ13">
+        <v>485.5771120981301</v>
+      </c>
+      <c r="AK13">
+        <v>24.56395891835728</v>
       </c>
     </row>
     <row r="14" spans="1:37">
@@ -1920,97 +2028,106 @@
         <v>48</v>
       </c>
       <c r="C14">
-        <v>103.5034918947993</v>
+        <v>103.5036587060711</v>
       </c>
       <c r="D14">
-        <v>1284.813953664592</v>
+        <v>1284.813718786922</v>
       </c>
       <c r="E14">
-        <v>2396.63770729631</v>
+        <v>2389.49952335985</v>
       </c>
       <c r="F14">
-        <v>1284.814003667092</v>
+        <v>1284.813768789422</v>
       </c>
       <c r="G14">
-        <v>6948.578259021415</v>
+        <v>6752.460919827642</v>
       </c>
       <c r="H14">
-        <v>1.104122563114895</v>
+        <v>1.106134561230224</v>
       </c>
       <c r="I14">
-        <v>7.023291916626619</v>
+        <v>4.692263700359636</v>
       </c>
       <c r="J14">
-        <v>0.5886747878033973</v>
+        <v>0.5312245086205671</v>
       </c>
       <c r="K14">
-        <v>2.208245126229791</v>
+        <v>2.212269122460448</v>
       </c>
       <c r="L14" t="s">
         <v>70</v>
       </c>
       <c r="M14">
-        <v>1388.317445559392</v>
+        <v>1388.317377492993</v>
       </c>
       <c r="N14">
-        <v>4774.386510834103</v>
+        <v>4775.822229297332</v>
       </c>
       <c r="O14">
-        <v>1388.317495561892</v>
+        <v>1388.317427495493</v>
       </c>
       <c r="P14">
-        <v>10805.31686343743</v>
+        <v>10835.90790773841</v>
       </c>
       <c r="Q14">
-        <v>0.8648191372480848</v>
+        <v>0.8646928472440216</v>
       </c>
       <c r="S14">
-        <v>6.833842091456769</v>
+        <v>6.530824531394795</v>
       </c>
       <c r="T14">
-        <v>0.588496211121876</v>
+        <v>0.5938685082476673</v>
       </c>
       <c r="U14">
-        <v>1.72963827449617</v>
+        <v>1.729385694488043</v>
       </c>
       <c r="V14" t="s">
         <v>70</v>
       </c>
       <c r="W14">
-        <v>1264.723667550817</v>
+        <v>1264.737636826267</v>
       </c>
       <c r="X14">
-        <v>963.9440735418942</v>
+        <v>748.4414489822598</v>
       </c>
       <c r="Y14">
-        <v>1.967086796482732</v>
+        <v>1.538057963355852</v>
       </c>
       <c r="Z14">
-        <v>1409.693222332882</v>
+        <v>1409.69342804502</v>
       </c>
       <c r="AA14">
-        <v>1156.777242235342</v>
+        <v>1131.223264811598</v>
       </c>
       <c r="AB14">
-        <v>1.281664150247978</v>
+        <v>1.255968508137351</v>
       </c>
       <c r="AC14">
-        <v>1370.229055989642</v>
+        <v>1370.22128313084</v>
       </c>
       <c r="AD14">
-        <v>109.8643859911042</v>
+        <v>153.7641002752144</v>
       </c>
       <c r="AE14">
-        <v>0.4306923265739998</v>
+        <v>0.4306894045463142</v>
       </c>
       <c r="AF14">
-        <v>1381.586900000001</v>
+        <v>1381.925017281976</v>
       </c>
       <c r="AG14">
-        <v>829.959438751026</v>
+        <v>862.0530474658885</v>
       </c>
       <c r="AH14">
-        <v>17.22769522305119</v>
+        <v>21.53456432757852</v>
+      </c>
+      <c r="AI14">
+        <v>1277.815715003929</v>
+      </c>
+      <c r="AJ14">
+        <v>828.0810610889044</v>
+      </c>
+      <c r="AK14">
+        <v>26.17301021093211</v>
       </c>
     </row>
     <row r="15" spans="1:37">
@@ -2021,97 +2138,106 @@
         <v>49</v>
       </c>
       <c r="C15">
-        <v>103.4548440391661</v>
+        <v>103.4549012197867</v>
       </c>
       <c r="D15">
-        <v>1284.906259892627</v>
+        <v>1284.906049266056</v>
       </c>
       <c r="E15">
-        <v>2322.718456597142</v>
+        <v>2317.851203272275</v>
       </c>
       <c r="F15">
-        <v>1284.906309895127</v>
+        <v>1284.906099268556</v>
       </c>
       <c r="G15">
-        <v>6526.132407873967</v>
+        <v>6401.873688087589</v>
       </c>
       <c r="H15">
-        <v>1.067755540916005</v>
+        <v>1.06928930436832</v>
       </c>
       <c r="I15">
-        <v>5.890219705262596</v>
+        <v>4.410857820829094</v>
       </c>
       <c r="J15">
-        <v>0.5936232523485446</v>
+        <v>0.5549266505540706</v>
       </c>
       <c r="K15">
-        <v>2.135511081832011</v>
+        <v>2.13857860873664</v>
       </c>
       <c r="L15" t="s">
         <v>70</v>
       </c>
       <c r="M15">
-        <v>1388.361103931793</v>
+        <v>1388.361050490843</v>
       </c>
       <c r="N15">
-        <v>4559.569423564882</v>
+        <v>4559.309183071594</v>
       </c>
       <c r="O15">
-        <v>1388.361153934293</v>
+        <v>1388.361000488343</v>
       </c>
       <c r="P15">
-        <v>10094.98152189347</v>
+        <v>10092.40276561945</v>
       </c>
       <c r="Q15">
-        <v>0.8484283874177407</v>
+        <v>0.84851991828881</v>
       </c>
       <c r="S15">
-        <v>6.468440672023305</v>
+        <v>5.802948212617295</v>
       </c>
       <c r="T15">
-        <v>0.5808516132094964</v>
+        <v>0.5801089842405369</v>
       </c>
       <c r="U15">
-        <v>1.696856774835481</v>
+        <v>1.69703983657762</v>
       </c>
       <c r="V15" t="s">
         <v>70</v>
       </c>
       <c r="W15">
-        <v>1264.769326022992</v>
+        <v>1264.771068487696</v>
       </c>
       <c r="X15">
-        <v>822.0466798974295</v>
+        <v>689.9913847373266</v>
       </c>
       <c r="Y15">
-        <v>1.779579347483372</v>
+        <v>1.514631470411971</v>
       </c>
       <c r="Z15">
-        <v>1409.748660719213</v>
+        <v>1409.75032820025</v>
       </c>
       <c r="AA15">
-        <v>1075.309312327725</v>
+        <v>986.3468385220064</v>
       </c>
       <c r="AB15">
-        <v>1.247854917903752</v>
+        <v>1.21929519332803</v>
       </c>
       <c r="AC15">
-        <v>1370.274560882958</v>
+        <v>1370.257730438828</v>
       </c>
       <c r="AD15">
-        <v>102.45775810827</v>
+        <v>138.7208661872547</v>
       </c>
       <c r="AE15">
-        <v>0.4226448973631609</v>
+        <v>0.4226381358010209</v>
       </c>
       <c r="AF15">
-        <v>1381.587104785057</v>
+        <v>1388.08148227868</v>
       </c>
       <c r="AG15">
-        <v>739.6619068540869</v>
+        <v>863.9848109995163</v>
       </c>
       <c r="AH15">
-        <v>16.90579589452964</v>
+        <v>21.13224710715429</v>
+      </c>
+      <c r="AI15">
+        <v>1277.81571647705</v>
+      </c>
+      <c r="AJ15">
+        <v>543.490557862776</v>
+      </c>
+      <c r="AK15">
+        <v>26.62530718798367</v>
       </c>
     </row>
     <row r="16" spans="1:37">
@@ -2122,100 +2248,109 @@
         <v>50</v>
       </c>
       <c r="C16">
-        <v>103.3935576279146</v>
+        <v>103.3935538256278</v>
       </c>
       <c r="D16">
-        <v>1285.05962683044</v>
+        <v>1285.059607514911</v>
       </c>
       <c r="E16">
-        <v>2325.039090055861</v>
+        <v>2320.331391097652</v>
       </c>
       <c r="F16">
-        <v>1285.05967683294</v>
+        <v>1285.059657517411</v>
       </c>
       <c r="G16">
-        <v>6181.717390185915</v>
+        <v>6077.017547909794</v>
       </c>
       <c r="H16">
-        <v>0.9993714109887689</v>
+        <v>1.000989633308584</v>
       </c>
       <c r="I16">
-        <v>5.469887477634123</v>
+        <v>4.421479004349811</v>
       </c>
       <c r="J16">
-        <v>0.6208387877717153</v>
+        <v>0.5864174171742591</v>
       </c>
       <c r="K16">
-        <v>1.998742821977538</v>
+        <v>2.001979266617168</v>
       </c>
       <c r="L16" t="s">
         <v>70</v>
       </c>
       <c r="M16">
-        <v>1388.453184458355</v>
+        <v>1388.453161340539</v>
       </c>
       <c r="N16">
-        <v>4440.44355935778</v>
+        <v>4439.109443791202</v>
       </c>
       <c r="O16">
-        <v>1388.453234460855</v>
+        <v>1388.453211343039</v>
       </c>
       <c r="P16">
-        <v>9436.963646973287</v>
+        <v>9412.040927199203</v>
       </c>
       <c r="Q16">
-        <v>0.8127820962353964</v>
+        <v>0.8129686562088658</v>
       </c>
       <c r="S16">
-        <v>5.730687065960862</v>
+        <v>6.382141926630983</v>
       </c>
       <c r="T16">
-        <v>0.5847918530964276</v>
+        <v>0.5794136861826706</v>
       </c>
       <c r="U16">
-        <v>1.625564192470793</v>
+        <v>1.625937312417732</v>
       </c>
       <c r="V16" t="s">
         <v>70</v>
       </c>
       <c r="W16">
-        <v>1264.968585334458</v>
+        <v>1264.970186773187</v>
       </c>
       <c r="X16">
-        <v>772.342421748625</v>
+        <v>661.0061713514564</v>
       </c>
       <c r="Y16">
-        <v>1.643655145189853</v>
+        <v>1.436127669217389</v>
       </c>
       <c r="Z16">
-        <v>1409.845435452521</v>
+        <v>1409.847238883013</v>
       </c>
       <c r="AA16">
-        <v>1033.033781228501</v>
+        <v>981.0585034406249</v>
       </c>
       <c r="AB16">
-        <v>1.17315569188696</v>
+        <v>1.161577966766453</v>
       </c>
       <c r="AC16">
-        <v>1370.316477635146</v>
+        <v>1369.186467641471</v>
       </c>
       <c r="AD16">
-        <v>101.4702278177562</v>
+        <v>149.0454395356566</v>
       </c>
       <c r="AE16">
-        <v>0.4052224880260806</v>
+        <v>0.06119998719054073</v>
       </c>
       <c r="AF16">
-        <v>1381.586900000004</v>
+        <v>1381.5869000052</v>
       </c>
       <c r="AG16">
-        <v>615.5591271429884</v>
+        <v>856.5406484982387</v>
       </c>
       <c r="AH16">
-        <v>16.20889952105988</v>
+        <v>20.26111000939225</v>
+      </c>
+      <c r="AI16">
+        <v>1277.815716852729</v>
+      </c>
+      <c r="AJ16">
+        <v>454.6448400315055</v>
+      </c>
+      <c r="AK16">
+        <v>24.92131575635062</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:37">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -2223,100 +2358,109 @@
         <v>51</v>
       </c>
       <c r="C17">
-        <v>103.3651452401311</v>
+        <v>103.3653344538889</v>
       </c>
       <c r="D17">
-        <v>1285.121697504421</v>
+        <v>1285.121607943055</v>
       </c>
       <c r="E17">
-        <v>2585.029256994835</v>
+        <v>2578.210606275994</v>
       </c>
       <c r="F17">
-        <v>1285.121747506921</v>
+        <v>1285.121657945555</v>
       </c>
       <c r="G17">
-        <v>6752.727603830856</v>
+        <v>6604.809086835231</v>
       </c>
       <c r="H17">
-        <v>0.9865807372535207</v>
+        <v>0.9887095475327121</v>
       </c>
       <c r="I17">
-        <v>6.756613689661127</v>
+        <v>5.059870419149132</v>
       </c>
       <c r="J17">
-        <v>0.6089755688339125</v>
+        <v>0.5638390466970179</v>
       </c>
       <c r="K17">
-        <v>1.973161474507041</v>
+        <v>1.977419095065424</v>
       </c>
       <c r="L17" t="s">
         <v>70</v>
       </c>
       <c r="M17">
-        <v>1388.486942749553</v>
+        <v>1388.487042401944</v>
       </c>
       <c r="N17">
-        <v>4876.984525473892</v>
+        <v>4877.864077842917</v>
       </c>
       <c r="O17">
-        <v>1388.486892747052</v>
+        <v>1388.486992399444</v>
       </c>
       <c r="P17">
-        <v>10213.85381892693</v>
+        <v>10235.83875094609</v>
       </c>
       <c r="Q17">
-        <v>0.8114586352689492</v>
+        <v>0.8114734776138857</v>
       </c>
       <c r="S17">
-        <v>9.465041484124926</v>
+        <v>8.473038660456002</v>
       </c>
       <c r="T17">
-        <v>0.5576916350717993</v>
+        <v>0.5615262952595559</v>
       </c>
       <c r="U17">
-        <v>1.622917270537898</v>
+        <v>1.622946955227771</v>
       </c>
       <c r="V17" t="s">
         <v>70</v>
       </c>
       <c r="W17">
-        <v>1265.004938080015</v>
+        <v>1265.007352539703</v>
       </c>
       <c r="X17">
-        <v>862.6088845832733</v>
+        <v>711.9993659722729</v>
       </c>
       <c r="Y17">
-        <v>1.636279595468475</v>
+        <v>1.351308294887548</v>
       </c>
       <c r="Z17">
-        <v>1409.845605988493</v>
+        <v>1409.840749396793</v>
       </c>
       <c r="AA17">
-        <v>877.9840747209914</v>
+        <v>868.0377372275917</v>
       </c>
       <c r="AB17">
-        <v>1.121160692480326</v>
+        <v>1.123595841681791</v>
       </c>
       <c r="AC17">
-        <v>1370.33454265225</v>
+        <v>1370.303098246682</v>
       </c>
       <c r="AD17">
-        <v>111.0987450849537</v>
+        <v>133.2469192687425</v>
       </c>
       <c r="AE17">
-        <v>0.4043032217178208</v>
+        <v>0.4042989344568853</v>
       </c>
       <c r="AF17">
-        <v>1395.586717276705</v>
+        <v>1395.58689992772</v>
       </c>
       <c r="AG17">
-        <v>1202.978030291562</v>
+        <v>1337.154801212871</v>
       </c>
       <c r="AH17">
-        <v>16.17212882824779</v>
+        <v>20.21515493084511</v>
+      </c>
+      <c r="AI17">
+        <v>1278.358859006803</v>
+      </c>
+      <c r="AJ17">
+        <v>635.3265284211584</v>
+      </c>
+      <c r="AK17">
+        <v>24.60271282245623</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:37">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -2324,100 +2468,109 @@
         <v>52</v>
       </c>
       <c r="C18">
-        <v>103.2707881740471</v>
+        <v>103.2707072435846</v>
       </c>
       <c r="D18">
-        <v>1285.368031407907</v>
+        <v>1285.368072011206</v>
       </c>
       <c r="E18">
-        <v>2450.572947496967</v>
+        <v>2445.405207038837</v>
       </c>
       <c r="F18">
-        <v>1285.368081410407</v>
+        <v>1285.368122013706</v>
       </c>
       <c r="G18">
-        <v>5879.034797035802</v>
+        <v>5768.670079349027</v>
       </c>
       <c r="H18">
-        <v>0.9086935911530621</v>
+        <v>0.9101048631580447</v>
       </c>
       <c r="I18">
-        <v>5.358859371696196</v>
+        <v>4.097992888851596</v>
       </c>
       <c r="J18">
-        <v>0.601517047674736</v>
+        <v>0.5631913695807881</v>
       </c>
       <c r="K18">
-        <v>1.817387182306124</v>
+        <v>1.820209726316089</v>
       </c>
       <c r="L18" t="s">
         <v>70</v>
       </c>
       <c r="M18">
-        <v>1388.638819581954</v>
+        <v>1388.638779254791</v>
       </c>
       <c r="N18">
-        <v>4535.95327445139</v>
+        <v>4536.084327093931</v>
       </c>
       <c r="O18">
-        <v>1388.638869584454</v>
+        <v>1388.638829257291</v>
       </c>
       <c r="P18">
-        <v>8933.577642953991</v>
+        <v>8937.804460737494</v>
       </c>
       <c r="Q18">
-        <v>0.7612468950120763</v>
+        <v>0.7612729365716503</v>
       </c>
       <c r="S18">
-        <v>5.220804649569674</v>
+        <v>5.005272864731561</v>
       </c>
       <c r="T18">
-        <v>0.5557114786450956</v>
+        <v>0.5564826785444538</v>
       </c>
       <c r="U18">
-        <v>1.522493790024153</v>
+        <v>1.522545873143301</v>
       </c>
       <c r="V18" t="s">
         <v>70</v>
       </c>
       <c r="W18">
-        <v>1265.245955960716</v>
+        <v>1265.250110125112</v>
       </c>
       <c r="X18">
-        <v>744.3279350291813</v>
+        <v>635.8168343889045</v>
       </c>
       <c r="Y18">
-        <v>1.437533805390741</v>
+        <v>1.228489493643669</v>
       </c>
       <c r="Z18">
-        <v>1410.0022814075</v>
+        <v>1410.002680567491</v>
       </c>
       <c r="AA18">
-        <v>967.1972232559417</v>
+        <v>945.2288034098709</v>
       </c>
       <c r="AB18">
-        <v>1.032626834663987</v>
+        <v>1.028217733251187</v>
       </c>
       <c r="AC18">
-        <v>1370.580896414545</v>
+        <v>1370.359008836545</v>
       </c>
       <c r="AD18">
-        <v>101.2233573195221</v>
+        <v>108.8346296454825</v>
       </c>
       <c r="AE18">
-        <v>0.3799225997219037</v>
+        <v>0.3799225922185184</v>
       </c>
       <c r="AF18">
-        <v>1381.586900000006</v>
+        <v>1381.5869</v>
       </c>
       <c r="AG18">
-        <v>436.6766112993326</v>
+        <v>502.2400977515393</v>
       </c>
       <c r="AH18">
-        <v>15.19690398889287</v>
+        <v>18.99612961092713</v>
+      </c>
+      <c r="AI18">
+        <v>1278.358859016664</v>
+      </c>
+      <c r="AJ18">
+        <v>476.4075254448958</v>
+      </c>
+      <c r="AK18">
+        <v>22.67345278907516</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:37">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -2425,100 +2578,109 @@
         <v>53</v>
       </c>
       <c r="C19">
-        <v>103.1903672620506</v>
+        <v>103.1902752280726</v>
       </c>
       <c r="D19">
-        <v>1285.554098593069</v>
+        <v>1285.554156947959</v>
       </c>
       <c r="E19">
-        <v>2261.605354752287</v>
+        <v>2257.707048423372</v>
       </c>
       <c r="F19">
-        <v>1285.554148595569</v>
+        <v>1285.554206950459</v>
       </c>
       <c r="G19">
-        <v>5032.758329058962</v>
+        <v>4962.645365942993</v>
       </c>
       <c r="H19">
-        <v>0.8440672643162637</v>
+        <v>0.8453287111745613</v>
       </c>
       <c r="I19">
-        <v>4.165196780136003</v>
+        <v>3.586639988247118</v>
       </c>
       <c r="J19">
-        <v>0.5978462110811092</v>
+        <v>0.5689187132459403</v>
       </c>
       <c r="K19">
-        <v>1.688134528632527</v>
+        <v>1.690657422349123</v>
       </c>
       <c r="L19" t="s">
         <v>70</v>
       </c>
       <c r="M19">
-        <v>1388.74446585512</v>
+        <v>1388.744432176032</v>
       </c>
       <c r="N19">
-        <v>4071.362247802999</v>
+        <v>4071.624806099137</v>
       </c>
       <c r="O19">
-        <v>1388.74451585762</v>
+        <v>1388.744482178532</v>
       </c>
       <c r="P19">
-        <v>7650.49898296584</v>
+        <v>7656.067973677981</v>
       </c>
       <c r="Q19">
-        <v>0.7353565930543221</v>
+        <v>0.7353566045748773</v>
       </c>
       <c r="S19">
-        <v>4.465816475782313</v>
+        <v>4.13585206023327</v>
       </c>
       <c r="T19">
-        <v>0.5233741243655273</v>
+        <v>0.5246994502240523</v>
       </c>
       <c r="U19">
-        <v>1.470713186108644</v>
+        <v>1.470713209149755</v>
       </c>
       <c r="V19" t="s">
         <v>70</v>
       </c>
       <c r="W19">
-        <v>1265.417623921856</v>
+        <v>1265.417275783665</v>
       </c>
       <c r="X19">
-        <v>634.577664763335</v>
+        <v>570.8372673988931</v>
       </c>
       <c r="Y19">
-        <v>1.259809510223814</v>
+        <v>1.13577883542481</v>
       </c>
       <c r="Z19">
-        <v>1410.075174622546</v>
+        <v>1410.075624170385</v>
       </c>
       <c r="AA19">
-        <v>804.176133496725</v>
+        <v>788.7850368186675</v>
       </c>
       <c r="AB19">
-        <v>0.9556802779002791</v>
+        <v>0.9530563232047351</v>
       </c>
       <c r="AC19">
-        <v>1370.647885088767</v>
+        <v>1370.664389369633</v>
       </c>
       <c r="AD19">
-        <v>85.17573906054466</v>
+        <v>104.339086896669</v>
       </c>
       <c r="AE19">
-        <v>0.3667307148241742</v>
+        <v>0.3667312188891979</v>
       </c>
       <c r="AF19">
-        <v>1381.5869</v>
+        <v>1381.586900064072</v>
       </c>
       <c r="AG19">
-        <v>348.2646934708653</v>
+        <v>387.7617338271237</v>
       </c>
       <c r="AH19">
-        <v>14.66929973054157</v>
+        <v>18.33662152732966</v>
+      </c>
+      <c r="AI19">
+        <v>1278.358859000062</v>
+      </c>
+      <c r="AJ19">
+        <v>298.4206276870534</v>
+      </c>
+      <c r="AK19">
+        <v>21.06195625549128</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
+    <row r="20" spans="1:37">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -2526,100 +2688,109 @@
         <v>54</v>
       </c>
       <c r="C20">
-        <v>103.125359848875</v>
+        <v>103.1251887762685</v>
       </c>
       <c r="D20">
-        <v>1285.703612919761</v>
+        <v>1285.70374950788</v>
       </c>
       <c r="E20">
-        <v>2058.913713875982</v>
+        <v>2056.450151889917</v>
       </c>
       <c r="F20">
-        <v>1285.703662922261</v>
+        <v>1285.70379951038</v>
       </c>
       <c r="G20">
-        <v>4389.947780244084</v>
+        <v>4348.996829215022</v>
       </c>
       <c r="H20">
-        <v>0.8204537277004733</v>
+        <v>0.8213634349756128</v>
       </c>
       <c r="I20">
-        <v>3.882004018219325</v>
+        <v>3.577867444550539</v>
       </c>
       <c r="J20">
-        <v>0.5614796904039859</v>
+        <v>0.5416675720191627</v>
       </c>
       <c r="K20">
-        <v>1.640907455400947</v>
+        <v>1.642726869951226</v>
       </c>
       <c r="L20" t="s">
         <v>70</v>
       </c>
       <c r="M20">
-        <v>1388.828972768636</v>
+        <v>1388.828938284148</v>
       </c>
       <c r="N20">
-        <v>3711.967936003738</v>
+        <v>3712.262558219285</v>
       </c>
       <c r="O20">
-        <v>1388.829022771136</v>
+        <v>1388.828988286648</v>
       </c>
       <c r="P20">
-        <v>6727.3675363496</v>
+        <v>6732.154854390022</v>
       </c>
       <c r="Q20">
-        <v>0.7111424524148574</v>
+        <v>0.7111185716481389</v>
       </c>
       <c r="S20">
-        <v>4.307663410697703</v>
+        <v>4.015901994905707</v>
       </c>
       <c r="T20">
-        <v>0.5158240217688459</v>
+        <v>0.5171791548826378</v>
       </c>
       <c r="U20">
-        <v>1.422284904829715</v>
+        <v>1.422237143296278</v>
       </c>
       <c r="V20" t="s">
         <v>70</v>
       </c>
       <c r="W20">
-        <v>1265.546931190931</v>
+        <v>1265.547577265206</v>
       </c>
       <c r="X20">
-        <v>528.7854942269412</v>
+        <v>493.0141181749876</v>
       </c>
       <c r="Y20">
-        <v>1.197237404988811</v>
+        <v>1.117972761555069</v>
       </c>
       <c r="Z20">
-        <v>1410.088249658834</v>
+        <v>1410.088538889702</v>
       </c>
       <c r="AA20">
-        <v>712.8943627926876</v>
+        <v>701.6673548093507</v>
       </c>
       <c r="AB20">
-        <v>0.8718403306434289</v>
+        <v>0.8707404336828392</v>
       </c>
       <c r="AC20">
-        <v>1370.654677164219</v>
+        <v>1370.672711908545</v>
       </c>
       <c r="AD20">
-        <v>67.15301638840373</v>
+        <v>86.97620911689005</v>
       </c>
       <c r="AE20">
-        <v>0.3544095426778784</v>
+        <v>0.3544063493837731</v>
       </c>
       <c r="AF20">
-        <v>1381.586902010486</v>
+        <v>1381.586900000003</v>
       </c>
       <c r="AG20">
-        <v>277.9955373173109</v>
+        <v>306.5743888483058</v>
       </c>
       <c r="AH20">
-        <v>14.1763819383146</v>
+        <v>17.72047838675017</v>
+      </c>
+      <c r="AI20">
+        <v>1278.90194581624</v>
+      </c>
+      <c r="AJ20">
+        <v>172.3149099733864</v>
+      </c>
+      <c r="AK20">
+        <v>20.47465611914883</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
+    <row r="21" spans="1:37">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -2627,100 +2798,109 @@
         <v>55</v>
       </c>
       <c r="C21">
-        <v>103.0191955998012</v>
+        <v>103.0191669801502</v>
       </c>
       <c r="D21">
-        <v>1285.956363308928</v>
+        <v>1285.956354326193</v>
       </c>
       <c r="E21">
-        <v>7081.385004971848</v>
+        <v>7072.240536108265</v>
       </c>
       <c r="F21">
-        <v>1285.956413311428</v>
+        <v>1285.956404328693</v>
       </c>
       <c r="G21">
-        <v>13792.92769118485</v>
+        <v>13611.72273658324</v>
       </c>
       <c r="H21">
-        <v>0.7649367902568475</v>
+        <v>0.7655484217397355</v>
       </c>
       <c r="I21">
-        <v>11.69547081992733</v>
+        <v>9.629930360719355</v>
       </c>
       <c r="J21">
-        <v>0.5089884390766628</v>
+        <v>0.4813718789443406</v>
       </c>
       <c r="K21">
-        <v>1.529873580513695</v>
+        <v>1.531096843479471</v>
       </c>
       <c r="L21" t="s">
         <v>70</v>
       </c>
       <c r="M21">
-        <v>1388.975558908729</v>
+        <v>1388.975521306343</v>
       </c>
       <c r="N21">
-        <v>12155.77337058851</v>
+        <v>12156.47647761266</v>
       </c>
       <c r="O21">
-        <v>1388.975608911229</v>
+        <v>1388.975571308843</v>
       </c>
       <c r="P21">
-        <v>20585.95822422618</v>
+        <v>20599.19360021237</v>
       </c>
       <c r="Q21">
-        <v>0.6796258902452902</v>
+        <v>0.6796230880206973</v>
       </c>
       <c r="S21">
-        <v>13.45430180042643</v>
+        <v>12.21723643617569</v>
       </c>
       <c r="T21">
-        <v>0.4563579840226657</v>
+        <v>0.4575775224975633</v>
       </c>
       <c r="U21">
-        <v>1.35925178049058</v>
+        <v>1.359246176041395</v>
       </c>
       <c r="V21" t="s">
         <v>70</v>
       </c>
       <c r="W21">
-        <v>1265.749878312873</v>
+        <v>1265.749565637645</v>
       </c>
       <c r="X21">
-        <v>1646.326890994239</v>
+        <v>1487.536774756166</v>
       </c>
       <c r="Y21">
-        <v>0.9933448086103405</v>
+        <v>0.9317484435665958</v>
       </c>
       <c r="Z21">
-        <v>1410.265684743453</v>
+        <v>1410.266050671942</v>
       </c>
       <c r="AA21">
-        <v>2242.979221039282</v>
+        <v>2213.185968178697</v>
       </c>
       <c r="AB21">
-        <v>0.833631467722281</v>
+        <v>0.8326754190265163</v>
       </c>
       <c r="AC21">
-        <v>1370.709346271989</v>
+        <v>1370.712353696467</v>
       </c>
       <c r="AD21">
-        <v>239.7265158213338</v>
+        <v>308.2480921473848</v>
       </c>
       <c r="AE21">
-        <v>0.3391199056341206</v>
+        <v>0.3391194354809396</v>
       </c>
       <c r="AF21">
-        <v>1382.119088977215</v>
+        <v>1382.119077</v>
       </c>
       <c r="AG21">
-        <v>761.4034305262641</v>
+        <v>837.4614354936155</v>
       </c>
       <c r="AH21">
-        <v>13.5647962254391</v>
+        <v>16.95599903709542</v>
+      </c>
+      <c r="AI21">
+        <v>1278.901945000001</v>
+      </c>
+      <c r="AJ21">
+        <v>787.4342240927331</v>
+      </c>
+      <c r="AK21">
+        <v>19.10228181831076</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
+    <row r="22" spans="1:37">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2728,100 +2908,109 @@
         <v>56</v>
       </c>
       <c r="C22">
-        <v>102.9778720933273</v>
+        <v>102.9778132244155</v>
       </c>
       <c r="D22">
-        <v>1286.056143669417</v>
+        <v>1286.056102633331</v>
       </c>
       <c r="E22">
-        <v>6193.434356868668</v>
+        <v>6187.861395111239</v>
       </c>
       <c r="F22">
-        <v>1286.056193671917</v>
+        <v>1286.056152635831</v>
       </c>
       <c r="G22">
-        <v>11516.32514306246</v>
+        <v>11430.85922490465</v>
       </c>
       <c r="H22">
-        <v>0.7365539073258756</v>
+        <v>0.7371406529304015</v>
       </c>
       <c r="I22">
-        <v>8.063911998280423</v>
+        <v>7.613391263420052</v>
       </c>
       <c r="J22">
-        <v>0.4865237316719924</v>
+        <v>0.4703193267449124</v>
       </c>
       <c r="K22">
-        <v>1.473107814651751</v>
+        <v>1.474281305860803</v>
       </c>
       <c r="L22" t="s">
         <v>70</v>
       </c>
       <c r="M22">
-        <v>1389.034015762744</v>
+        <v>1389.034015862747</v>
       </c>
       <c r="N22">
-        <v>10285.11989728798</v>
+        <v>10285.21694995341</v>
       </c>
       <c r="O22">
-        <v>1389.034065765244</v>
+        <v>1389.033965860247</v>
       </c>
       <c r="P22">
-        <v>17061.5836779786</v>
+        <v>17064.0310967537</v>
       </c>
       <c r="Q22">
-        <v>0.6723088197354977</v>
+        <v>0.6723198347325456</v>
       </c>
       <c r="S22">
-        <v>11.40316343408969</v>
+        <v>10.73610516296675</v>
       </c>
       <c r="T22">
-        <v>0.4294799715374555</v>
+        <v>0.4296872442166246</v>
       </c>
       <c r="U22">
-        <v>1.344617639470995</v>
+        <v>1.344639669465091</v>
       </c>
       <c r="V22" t="s">
         <v>70</v>
       </c>
       <c r="W22">
-        <v>1265.842995383226</v>
+        <v>1265.842954827534</v>
       </c>
       <c r="X22">
-        <v>1330.732675242365</v>
+        <v>1247.063651310059</v>
       </c>
       <c r="Y22">
-        <v>0.9234990868890975</v>
+        <v>0.9084822947248079</v>
       </c>
       <c r="Z22">
-        <v>1410.32569439429</v>
+        <v>1410.326731953533</v>
       </c>
       <c r="AA22">
-        <v>1838.941443339333</v>
+        <v>1733.649097946407</v>
       </c>
       <c r="AB22">
-        <v>0.7955402372553034</v>
+        <v>0.7938184376059781</v>
       </c>
       <c r="AC22">
-        <v>1370.737064962382</v>
+        <v>1370.734990901279</v>
       </c>
       <c r="AD22">
-        <v>204.9155614373019</v>
+        <v>284.6716182264918</v>
       </c>
       <c r="AE22">
-        <v>0.3357104179016078</v>
+        <v>0.3357034207221342</v>
       </c>
       <c r="AF22">
-        <v>1382.119077005259</v>
+        <v>1396.119077</v>
       </c>
       <c r="AG22">
-        <v>544.2200089725548</v>
+        <v>637.0335257515837</v>
       </c>
       <c r="AH22">
-        <v>13.42841671620555</v>
+        <v>16.78551965935237</v>
+      </c>
+      <c r="AI22">
+        <v>1278.901945000001</v>
+      </c>
+      <c r="AJ22">
+        <v>366.5473853726332</v>
+      </c>
+      <c r="AK22">
+        <v>18.39071171379168</v>
       </c>
     </row>
-    <row r="23" spans="1:34">
+    <row r="23" spans="1:37">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -2829,100 +3018,109 @@
         <v>57</v>
       </c>
       <c r="C23">
-        <v>102.9512281011653</v>
+        <v>102.9517482435906</v>
       </c>
       <c r="D23">
-        <v>1286.136941609204</v>
+        <v>1286.136961046252</v>
       </c>
       <c r="E23">
-        <v>4882.922514682432</v>
+        <v>4879.719266682373</v>
       </c>
       <c r="F23">
-        <v>1286.136991611704</v>
+        <v>1286.137011048752</v>
       </c>
       <c r="G23">
-        <v>8767.236526183855</v>
+        <v>8729.290973074494</v>
       </c>
       <c r="H23">
-        <v>0.71173089166152</v>
+        <v>0.7122443961501892</v>
       </c>
       <c r="I23">
-        <v>7.962379195232214</v>
+        <v>7.800185155777428</v>
       </c>
       <c r="J23">
-        <v>0.484631133469041</v>
+        <v>0.4748158964100658</v>
       </c>
       <c r="K23">
-        <v>1.42346178332304</v>
+        <v>1.424488792300378</v>
       </c>
       <c r="L23" t="s">
         <v>70</v>
       </c>
       <c r="M23">
-        <v>1389.08836972037</v>
+        <v>1389.088709289842</v>
       </c>
       <c r="N23">
-        <v>7905.171866881334</v>
+        <v>7902.467785685674</v>
       </c>
       <c r="O23">
-        <v>1389.088219712869</v>
+        <v>1389.088759292342</v>
       </c>
       <c r="P23">
-        <v>12671.79619223748</v>
+        <v>12703.2971120527</v>
       </c>
       <c r="Q23">
-        <v>0.6561153539367683</v>
+        <v>0.6573650476858113</v>
       </c>
       <c r="S23">
-        <v>10.31814768338209</v>
+        <v>8.48390627532722</v>
       </c>
       <c r="T23">
-        <v>0.4067764305762054</v>
+        <v>0.4048337271724332</v>
       </c>
       <c r="U23">
-        <v>1.312230707873537</v>
+        <v>1.314730095371623</v>
       </c>
       <c r="V23" t="s">
         <v>70</v>
       </c>
       <c r="W23">
-        <v>1265.913181805897</v>
+        <v>1265.912651666856</v>
       </c>
       <c r="X23">
-        <v>1017.925031510029</v>
+        <v>981.117398298597</v>
       </c>
       <c r="Y23">
-        <v>0.90521933061365</v>
+        <v>0.8954686846887614</v>
       </c>
       <c r="Z23">
-        <v>1410.376247040679</v>
+        <v>1410.376890706118</v>
       </c>
       <c r="AA23">
-        <v>1408.310005879851</v>
+        <v>1376.255424194667</v>
       </c>
       <c r="AB23">
-        <v>0.7801932588410797</v>
+        <v>0.7796665017358365</v>
       </c>
       <c r="AC23">
-        <v>1370.726860322883</v>
+        <v>1370.727073208254</v>
       </c>
       <c r="AD23">
-        <v>144.4283808053086</v>
+        <v>193.0325314639768</v>
       </c>
       <c r="AE23">
-        <v>0.3283598978634956</v>
+        <v>0.3283571741232323</v>
       </c>
       <c r="AF23">
-        <v>1389.819539216186</v>
+        <v>1382.119077</v>
       </c>
       <c r="AG23">
-        <v>117.5518282610824</v>
+        <v>417.721549740717</v>
       </c>
       <c r="AH23">
-        <v>1.970159387182876</v>
+        <v>16.41801472185887</v>
+      </c>
+      <c r="AI23">
+        <v>1278.901945003676</v>
+      </c>
+      <c r="AJ23">
+        <v>158.7039200442109</v>
+      </c>
+      <c r="AK23">
+        <v>17.76627212087253</v>
       </c>
     </row>
-    <row r="24" spans="1:34">
+    <row r="24" spans="1:37">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -2930,100 +3128,109 @@
         <v>58</v>
       </c>
       <c r="C24">
-        <v>102.919051026762</v>
+        <v>102.9201447363628</v>
       </c>
       <c r="D24">
-        <v>1286.225653034865</v>
+        <v>1286.225656051569</v>
       </c>
       <c r="E24">
-        <v>4277.162111741199</v>
+        <v>4277.028181582102</v>
       </c>
       <c r="F24">
-        <v>1286.225703037365</v>
+        <v>1286.225706054069</v>
       </c>
       <c r="G24">
-        <v>7359.67510553917</v>
+        <v>7358.147732708598</v>
       </c>
       <c r="H24">
-        <v>0.6899213636373237</v>
+        <v>0.6899451214300998</v>
       </c>
       <c r="I24">
-        <v>6.92675718025102</v>
+        <v>6.92463495754702</v>
       </c>
       <c r="J24">
-        <v>0.4544741432907445</v>
+        <v>0.4539979161720071</v>
       </c>
       <c r="K24">
-        <v>1.379842727274647</v>
+        <v>1.3798902428602</v>
       </c>
       <c r="L24" t="s">
         <v>70</v>
       </c>
       <c r="M24">
-        <v>1389.145104081628</v>
+        <v>1389.145800787932</v>
       </c>
       <c r="N24">
-        <v>6781.108127561045</v>
+        <v>6782.945025791491</v>
       </c>
       <c r="O24">
-        <v>1389.144754064127</v>
+        <v>1389.145850790432</v>
       </c>
       <c r="P24">
-        <v>10483.58407322541</v>
+        <v>10687.12398826688</v>
       </c>
       <c r="Q24">
-        <v>0.6481189062499462</v>
+        <v>0.6507056515868868</v>
       </c>
       <c r="S24">
-        <v>8.41162700007138</v>
+        <v>7.343329184685644</v>
       </c>
       <c r="T24">
-        <v>0.3528543811457042</v>
+        <v>0.3772504386883369</v>
       </c>
       <c r="U24">
-        <v>1.296237812499892</v>
+        <v>1.301411303173774</v>
       </c>
       <c r="V24" t="s">
         <v>70</v>
       </c>
       <c r="W24">
-        <v>1266.012028974179</v>
+        <v>1266.012013492207</v>
       </c>
       <c r="X24">
-        <v>831.0298140526728</v>
+        <v>830.4732468316478</v>
       </c>
       <c r="Y24">
-        <v>0.8185991099754172</v>
+        <v>0.8185615150547877</v>
       </c>
       <c r="Z24">
-        <v>1410.420235965225</v>
+        <v>1410.420618353765</v>
       </c>
       <c r="AA24">
-        <v>1171.903694235983</v>
+        <v>1150.673473359937</v>
       </c>
       <c r="AB24">
-        <v>0.7478079659526882</v>
+        <v>0.7477363594970271</v>
       </c>
       <c r="AC24">
-        <v>1370.785682917096</v>
+        <v>1370.771397684028</v>
       </c>
       <c r="AD24">
-        <v>139.7376494789321</v>
+        <v>165.358340484935</v>
       </c>
       <c r="AE24">
-        <v>0.3250663175070017</v>
+        <v>0.32506470183717</v>
       </c>
       <c r="AF24">
-        <v>1389.78558015269</v>
+        <v>1382.119077</v>
       </c>
       <c r="AG24">
-        <v>241.9966723425673</v>
+        <v>267.1566131763556</v>
       </c>
       <c r="AH24">
-        <v>1.950397905048703</v>
+        <v>16.25331551890926</v>
+      </c>
+      <c r="AI24">
+        <v>1293.415378761506</v>
+      </c>
+      <c r="AJ24">
+        <v>6.253405311368098</v>
+      </c>
+      <c r="AK24">
+        <v>17.22342374131281</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:37">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -3031,100 +3238,109 @@
         <v>59</v>
       </c>
       <c r="C25">
-        <v>102.8851114821828</v>
+        <v>102.885510157377</v>
       </c>
       <c r="D25">
-        <v>1286.307952356643</v>
+        <v>1286.307955037097</v>
       </c>
       <c r="E25">
-        <v>3730.036675876071</v>
+        <v>3729.946000349129</v>
       </c>
       <c r="F25">
-        <v>1286.308002359143</v>
+        <v>1286.308005039597</v>
       </c>
       <c r="G25">
-        <v>6286.535018390293</v>
+        <v>6285.210039430156</v>
       </c>
       <c r="H25">
-        <v>0.6896632270554484</v>
+        <v>0.6896779105685856</v>
       </c>
       <c r="I25">
-        <v>5.95800773496336</v>
+        <v>5.956319977531034</v>
       </c>
       <c r="J25">
-        <v>0.3999685287428566</v>
+        <v>0.3994927954523566</v>
       </c>
       <c r="K25">
-        <v>1.379326454110897</v>
+        <v>1.379355821137171</v>
       </c>
       <c r="L25" t="s">
         <v>70</v>
       </c>
       <c r="M25">
-        <v>1389.193263848826</v>
+        <v>1389.193465194474</v>
       </c>
       <c r="N25">
-        <v>5902.493767433258</v>
+        <v>5902.302519261482</v>
       </c>
       <c r="O25">
-        <v>1389.193113841326</v>
+        <v>1389.193515196974</v>
       </c>
       <c r="P25">
-        <v>9057.418024363742</v>
+        <v>9087.718800358285</v>
       </c>
       <c r="Q25">
-        <v>0.6340725782889254</v>
+        <v>0.6347244412366301</v>
       </c>
       <c r="S25">
-        <v>7.484232959689152</v>
+        <v>6.975738202138834</v>
       </c>
       <c r="T25">
-        <v>0.378198560930521</v>
+        <v>0.3811484273599627</v>
       </c>
       <c r="U25">
-        <v>1.268145156577851</v>
+        <v>1.26944888247326</v>
       </c>
       <c r="V25" t="s">
         <v>70</v>
       </c>
       <c r="W25">
-        <v>1266.049704205592</v>
+        <v>1266.04969473916</v>
       </c>
       <c r="X25">
-        <v>708.7319186278969</v>
+        <v>708.2748791133473</v>
       </c>
       <c r="Y25">
-        <v>0.7479094686638177</v>
+        <v>0.7479082687313071</v>
       </c>
       <c r="Z25">
-        <v>1410.4663124883</v>
+        <v>1410.466375658101</v>
       </c>
       <c r="AA25">
-        <v>981.9985143270674</v>
+        <v>973.7093237056291</v>
       </c>
       <c r="AB25">
-        <v>0.6784451308514597</v>
+        <v>0.6785826134074892</v>
       </c>
       <c r="AC25">
-        <v>1370.809193055841</v>
+        <v>1370.784145278321</v>
       </c>
       <c r="AD25">
-        <v>119.9866934498272</v>
+        <v>141.99294907661</v>
       </c>
       <c r="AE25">
-        <v>0.3170779008820681</v>
+        <v>0.3170750321892484</v>
       </c>
       <c r="AF25">
-        <v>1390.119851155811</v>
+        <v>1382.119077000001</v>
       </c>
       <c r="AG25">
-        <v>55.72640233047765</v>
+        <v>129.3534075472842</v>
       </c>
       <c r="AH25">
-        <v>1.902467405292833</v>
+        <v>15.85391092422577</v>
+      </c>
+      <c r="AI25">
+        <v>1293.444716505453</v>
+      </c>
+      <c r="AJ25">
+        <v>5.600020709877732</v>
+      </c>
+      <c r="AK25">
+        <v>17.22421924123349</v>
       </c>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:37">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -3132,100 +3348,109 @@
         <v>60</v>
       </c>
       <c r="C26">
-        <v>102.8590991927979</v>
+        <v>102.8591426406306</v>
       </c>
       <c r="D26">
-        <v>1286.380005975821</v>
+        <v>1286.380041201693</v>
       </c>
       <c r="E26">
-        <v>3195.521515535806</v>
+        <v>3194.933006645435</v>
       </c>
       <c r="F26">
-        <v>1286.380055978321</v>
+        <v>1286.380091204193</v>
       </c>
       <c r="G26">
-        <v>5186.596172914073</v>
+        <v>5175.876621498763</v>
       </c>
       <c r="H26">
-        <v>0.6687517782128921</v>
+        <v>0.6688266513871959</v>
       </c>
       <c r="I26">
-        <v>6.138484627973001</v>
+        <v>6.096149002292435</v>
       </c>
       <c r="J26">
-        <v>0.3813100470067965</v>
+        <v>0.3767448491483635</v>
       </c>
       <c r="K26">
-        <v>1.337503556425784</v>
+        <v>1.337653302774392</v>
       </c>
       <c r="L26" t="s">
         <v>70</v>
       </c>
       <c r="M26">
-        <v>1389.239205173619</v>
+        <v>1389.239283847323</v>
       </c>
       <c r="N26">
-        <v>4935.909727746068</v>
+        <v>4935.937693211805</v>
       </c>
       <c r="O26">
-        <v>1389.239155171119</v>
+        <v>1389.239233844823</v>
       </c>
       <c r="P26">
-        <v>7433.353628503502</v>
+        <v>7438.685378570683</v>
       </c>
       <c r="Q26">
-        <v>0.6213676179597226</v>
+        <v>0.6214821502022263</v>
       </c>
       <c r="S26">
-        <v>6.196685385902443</v>
+        <v>6.165630963539456</v>
       </c>
       <c r="T26">
-        <v>0.3782781156540145</v>
+        <v>0.3790312792850333</v>
       </c>
       <c r="U26">
-        <v>1.242735235919445</v>
+        <v>1.242964300404453</v>
       </c>
       <c r="V26" t="s">
         <v>70</v>
       </c>
       <c r="W26">
-        <v>1266.148666818761</v>
+        <v>1266.148896620929</v>
       </c>
       <c r="X26">
-        <v>584.6003374861918</v>
+        <v>574.5617442670721</v>
       </c>
       <c r="Y26">
-        <v>0.7721033323347626</v>
+        <v>0.7704798353294184</v>
       </c>
       <c r="Z26">
-        <v>1410.506348919504</v>
+        <v>1410.506359139955</v>
       </c>
       <c r="AA26">
-        <v>796.4237762883058</v>
+        <v>795.3749671308361</v>
       </c>
       <c r="AB26">
-        <v>0.6611704837879567</v>
+        <v>0.6612972238582869</v>
       </c>
       <c r="AC26">
-        <v>1370.818943751671</v>
+        <v>1371.137305812034</v>
       </c>
       <c r="AD26">
-        <v>84.18816429483502</v>
+        <v>96.55936063585924</v>
       </c>
       <c r="AE26">
-        <v>0.3104798841170232</v>
+        <v>0.3104799724638496</v>
       </c>
       <c r="AF26">
-        <v>1390.212497860455</v>
+        <v>1382.119077</v>
       </c>
       <c r="AG26">
-        <v>8.619998780015772</v>
+        <v>16.03700240237901</v>
       </c>
       <c r="AH26">
-        <v>1.862883271054004</v>
+        <v>15.52399862321339</v>
+      </c>
+      <c r="AI26">
+        <v>1279.4449741955</v>
+      </c>
+      <c r="AJ26">
+        <v>47.37694268065144</v>
+      </c>
+      <c r="AK26">
+        <v>16.70629908342694</v>
       </c>
     </row>
-    <row r="27" spans="1:34">
+    <row r="27" spans="1:37">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -3233,100 +3458,109 @@
         <v>61</v>
       </c>
       <c r="C27">
-        <v>102.8330140513744</v>
+        <v>102.8338521942269</v>
       </c>
       <c r="D27">
-        <v>1286.448210372344</v>
+        <v>1286.448210259634</v>
       </c>
       <c r="E27">
-        <v>2444.588544919373</v>
+        <v>2444.545508791241</v>
       </c>
       <c r="F27">
-        <v>1286.448260374844</v>
+        <v>1286.448260262134</v>
       </c>
       <c r="G27">
-        <v>3858.038096691865</v>
+        <v>3857.216862162943</v>
       </c>
       <c r="H27">
-        <v>0.6592551159314366</v>
+        <v>0.6592617548503852</v>
       </c>
       <c r="I27">
-        <v>4.487961754645116</v>
+        <v>4.495489942641665</v>
       </c>
       <c r="J27">
-        <v>0.3435901527710629</v>
+        <v>0.3431140419584963</v>
       </c>
       <c r="K27">
-        <v>1.318510231862873</v>
+        <v>1.31852350970077</v>
       </c>
       <c r="L27" t="s">
         <v>70</v>
       </c>
       <c r="M27">
-        <v>1389.281524438719</v>
+        <v>1389.282162458861</v>
       </c>
       <c r="N27">
-        <v>3852.176651715336</v>
+        <v>3855.79395897339</v>
       </c>
       <c r="O27">
-        <v>1389.281274426218</v>
+        <v>1389.282112456361</v>
       </c>
       <c r="P27">
-        <v>5570.181722202121</v>
+        <v>5644.329816840092</v>
       </c>
       <c r="Q27">
-        <v>0.6098568113547875</v>
+        <v>0.6103908045350632</v>
       </c>
       <c r="S27">
-        <v>5.004583049391286</v>
+        <v>4.92094430532785</v>
       </c>
       <c r="T27">
-        <v>0.3264143185175707</v>
+        <v>0.3486011367305651</v>
       </c>
       <c r="U27">
-        <v>1.219713622709575</v>
+        <v>1.220781609070126</v>
       </c>
       <c r="V27" t="s">
         <v>70</v>
       </c>
       <c r="W27">
-        <v>1266.173732546312</v>
+        <v>1266.173778554489</v>
       </c>
       <c r="X27">
-        <v>409.4393138380261</v>
+        <v>408.6535803261495</v>
       </c>
       <c r="Y27">
-        <v>0.7778550011986873</v>
+        <v>0.7778837951171459</v>
       </c>
       <c r="Z27">
-        <v>1410.547424856317</v>
+        <v>1410.547390246229</v>
       </c>
       <c r="AA27">
-        <v>590.5277250104713</v>
+        <v>588.5535497351424</v>
       </c>
       <c r="AB27">
-        <v>0.6660375244125994</v>
+        <v>0.6662970238375208</v>
       </c>
       <c r="AC27">
-        <v>1370.844216115541</v>
+        <v>1370.792137775551</v>
       </c>
       <c r="AD27">
-        <v>59.0058170113154</v>
+        <v>79.01452910676652</v>
       </c>
       <c r="AE27">
-        <v>0.3049066328635975</v>
+        <v>0.3049073568567074</v>
       </c>
       <c r="AF27">
-        <v>1390.19529625062</v>
+        <v>1396.086750259635</v>
       </c>
       <c r="AG27">
-        <v>68.40439912649229</v>
+        <v>6.196667480000345</v>
       </c>
       <c r="AH27">
-        <v>1.829439797183273</v>
+        <v>15.2401899151037</v>
+      </c>
+      <c r="AI27">
+        <v>1279.448357748417</v>
+      </c>
+      <c r="AJ27">
+        <v>3.67333384324506</v>
+      </c>
+      <c r="AK27">
+        <v>16.46397178556865</v>
       </c>
     </row>
-    <row r="28" spans="1:34">
+    <row r="28" spans="1:37">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -3334,100 +3568,109 @@
         <v>62</v>
       </c>
       <c r="C28">
-        <v>102.8106755392253</v>
+        <v>102.8111819234791</v>
       </c>
       <c r="D28">
-        <v>1286.490998295702</v>
+        <v>1286.491071198229</v>
       </c>
       <c r="E28">
-        <v>2228.792232682761</v>
+        <v>2228.724542367189</v>
       </c>
       <c r="F28">
-        <v>1286.491048298202</v>
+        <v>1286.491021195729</v>
       </c>
       <c r="G28">
-        <v>3464.030430033019</v>
+        <v>3462.780398888111</v>
       </c>
       <c r="H28">
-        <v>0.6522095114673016</v>
+        <v>0.6522208597694967</v>
       </c>
       <c r="I28">
-        <v>4.22308817657717</v>
+        <v>4.239512778819704</v>
       </c>
       <c r="J28">
-        <v>0.3309566932358205</v>
+        <v>0.3301461050094627</v>
       </c>
       <c r="K28">
-        <v>1.304419022934603</v>
+        <v>1.304441719538993</v>
       </c>
       <c r="L28" t="s">
         <v>70</v>
       </c>
       <c r="M28">
-        <v>1389.301873844928</v>
+        <v>1389.302253121708</v>
       </c>
       <c r="N28">
-        <v>3456.481701868185</v>
+        <v>3458.606874108311</v>
       </c>
       <c r="O28">
-        <v>1389.301723837427</v>
+        <v>1389.302203119208</v>
       </c>
       <c r="P28">
-        <v>4977.590376156973</v>
+        <v>5017.352877340106</v>
       </c>
       <c r="Q28">
-        <v>0.60949525787934</v>
+        <v>0.6097655016904719</v>
       </c>
       <c r="S28">
-        <v>4.857893653807684</v>
+        <v>4.850580865391025</v>
       </c>
       <c r="T28">
-        <v>0.3129041481960479</v>
+        <v>0.3264516730235098</v>
       </c>
       <c r="U28">
-        <v>1.21899051575868</v>
+        <v>1.219531003380944</v>
       </c>
       <c r="V28" t="s">
         <v>70</v>
       </c>
       <c r="W28">
-        <v>1266.233089314268</v>
+        <v>1266.233088873261</v>
       </c>
       <c r="X28">
-        <v>361.2297732389313</v>
+        <v>361.2219834581911</v>
       </c>
       <c r="Y28">
-        <v>0.7684774641865586</v>
+        <v>0.7685114667606923</v>
       </c>
       <c r="Z28">
-        <v>1410.569606232373</v>
+        <v>1410.569600281344</v>
       </c>
       <c r="AA28">
-        <v>539.9623797824365</v>
+        <v>539.2156395133782</v>
       </c>
       <c r="AB28">
-        <v>0.606705497974409</v>
+        <v>0.6069379761197972</v>
       </c>
       <c r="AC28">
-        <v>1370.819294976424</v>
+        <v>1370.802217043543</v>
       </c>
       <c r="AD28">
-        <v>73.0783304474283</v>
+        <v>81.20099665847738</v>
       </c>
       <c r="AE28">
-        <v>0.3045498351419623</v>
+        <v>0.3045484292657096</v>
       </c>
       <c r="AF28">
-        <v>1390.205939062379</v>
+        <v>1382.120731050799</v>
       </c>
       <c r="AG28">
-        <v>37.03408228300173</v>
+        <v>6.12666626000034</v>
       </c>
       <c r="AH28">
-        <v>1.8272990621135</v>
+        <v>15.22723271333104</v>
+      </c>
+      <c r="AI28">
+        <v>1293.006222365252</v>
+      </c>
+      <c r="AJ28">
+        <v>3.333333740034013</v>
+      </c>
+      <c r="AK28">
+        <v>6.675951690474317</v>
       </c>
     </row>
-    <row r="29" spans="1:34">
+    <row r="29" spans="1:37">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -3435,100 +3678,109 @@
         <v>63</v>
       </c>
       <c r="C29">
-        <v>102.8074540595214</v>
+        <v>102.807544042834</v>
       </c>
       <c r="D29">
-        <v>1286.514203679813</v>
+        <v>1286.51419963736</v>
       </c>
       <c r="E29">
-        <v>2008.914204525501</v>
+        <v>2008.868576334886</v>
       </c>
       <c r="F29">
-        <v>1286.514253682313</v>
+        <v>1286.51424963986</v>
       </c>
       <c r="G29">
-        <v>3122.915372749056</v>
+        <v>3122.193152174541</v>
       </c>
       <c r="H29">
-        <v>0.6526553093024455</v>
+        <v>0.6526672364534671</v>
       </c>
       <c r="I29">
-        <v>4.204922172261536</v>
+        <v>4.213209383733347</v>
       </c>
       <c r="J29">
-        <v>0.3296167345397992</v>
+        <v>0.3290836986304686</v>
       </c>
       <c r="K29">
-        <v>1.305310618604891</v>
+        <v>1.305334472906934</v>
       </c>
       <c r="L29" t="s">
         <v>70</v>
       </c>
       <c r="M29">
-        <v>1389.321757744335</v>
+        <v>1389.321843685194</v>
       </c>
       <c r="N29">
-        <v>3159.601421864544</v>
+        <v>3159.851735533242</v>
       </c>
       <c r="O29">
-        <v>1389.321707741835</v>
+        <v>1389.321793682694</v>
       </c>
       <c r="P29">
-        <v>4525.805911131346</v>
+        <v>4530.402441423998</v>
       </c>
       <c r="Q29">
-        <v>0.6011623253419275</v>
+        <v>0.6012025865532689</v>
       </c>
       <c r="S29">
-        <v>4.667441735679418</v>
+        <v>4.730319940684018</v>
       </c>
       <c r="T29">
-        <v>0.3313875885993361</v>
+        <v>0.3330618763955572</v>
       </c>
       <c r="U29">
-        <v>1.202324650683855</v>
+        <v>1.202405173106538</v>
       </c>
       <c r="V29" t="s">
         <v>70</v>
       </c>
       <c r="W29">
-        <v>1266.227170452153</v>
+        <v>1266.227162220108</v>
       </c>
       <c r="X29">
-        <v>333.7030297286241</v>
+        <v>333.4598613775185</v>
       </c>
       <c r="Y29">
-        <v>0.7484521116453239</v>
+        <v>0.7484668860410986</v>
       </c>
       <c r="Z29">
-        <v>1410.567799178647</v>
+        <v>1410.567803262081</v>
       </c>
       <c r="AA29">
-        <v>476.6873449056368</v>
+        <v>476.3519852308297</v>
       </c>
       <c r="AB29">
-        <v>0.6421950224917871</v>
+        <v>0.6422985817734113</v>
       </c>
       <c r="AC29">
-        <v>1370.793263455517</v>
+        <v>1371.115327777997</v>
       </c>
       <c r="AD29">
-        <v>61.4746639573999</v>
+        <v>57.10170585244833</v>
       </c>
       <c r="AE29">
-        <v>0.3002645152523816</v>
+        <v>0.3002637807533339</v>
       </c>
       <c r="AF29">
-        <v>1390.48969818163</v>
+        <v>1382.126918494953</v>
       </c>
       <c r="AG29">
-        <v>5.35667029591713</v>
+        <v>5.356666870000296</v>
       </c>
       <c r="AH29">
-        <v>1.801587396970348</v>
+        <v>15.01316893083252</v>
+      </c>
+      <c r="AI29">
+        <v>1293.444945581967</v>
+      </c>
+      <c r="AJ29">
+        <v>3.126666262992906</v>
+      </c>
+      <c r="AK29">
+        <v>16.29793743505674</v>
       </c>
     </row>
-    <row r="30" spans="1:34">
+    <row r="30" spans="1:37">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -3536,100 +3788,109 @@
         <v>64</v>
       </c>
       <c r="C30">
-        <v>102.8039526065052</v>
+        <v>102.8042071581879</v>
       </c>
       <c r="D30">
-        <v>1286.536097814129</v>
+        <v>1286.536000071309</v>
       </c>
       <c r="E30">
-        <v>1867.858413859518</v>
+        <v>1865.966017632548</v>
       </c>
       <c r="F30">
-        <v>1286.536147816629</v>
+        <v>1286.535950068808</v>
       </c>
       <c r="G30">
-        <v>2833.776069082804</v>
+        <v>2804.76912399759</v>
       </c>
       <c r="H30">
-        <v>0.6438403563183082</v>
+        <v>0.6443640444583525</v>
       </c>
       <c r="I30">
-        <v>4.78210932414124</v>
+        <v>4.940838896153801</v>
       </c>
       <c r="J30">
-        <v>0.2996397599779582</v>
+        <v>0.2754892892152043</v>
       </c>
       <c r="K30">
-        <v>1.287680712636616</v>
+        <v>1.288728088916705</v>
       </c>
       <c r="L30" t="s">
         <v>70</v>
       </c>
       <c r="M30">
-        <v>1389.340150425634</v>
+        <v>1389.340207229496</v>
       </c>
       <c r="N30">
-        <v>2912.44048892475</v>
+        <v>2912.64171656537</v>
       </c>
       <c r="O30">
-        <v>1389.340100423134</v>
+        <v>1389.340157226996</v>
       </c>
       <c r="P30">
-        <v>4091.984321131485</v>
+        <v>4096.482976645813</v>
       </c>
       <c r="Q30">
-        <v>0.59566462117568</v>
+        <v>0.5957371079248025</v>
       </c>
       <c r="S30">
-        <v>3.711916810701452</v>
+        <v>3.718549048814805</v>
       </c>
       <c r="T30">
-        <v>0.3033214991574682</v>
+        <v>0.3049646819555763</v>
       </c>
       <c r="U30">
-        <v>1.19132924235136</v>
+        <v>1.191474215849605</v>
       </c>
       <c r="V30" t="s">
         <v>70</v>
       </c>
       <c r="W30">
-        <v>1266.272881853919</v>
+        <v>1266.272679094143</v>
       </c>
       <c r="X30">
-        <v>314.2117085119229</v>
+        <v>305.6445961995115</v>
       </c>
       <c r="Y30">
-        <v>0.6964666436946143</v>
+        <v>0.6949371025937966</v>
       </c>
       <c r="Z30">
-        <v>1410.586483285438</v>
+        <v>1410.586498214726</v>
       </c>
       <c r="AA30">
-        <v>420.088558655803</v>
+        <v>419.7641799129782</v>
       </c>
       <c r="AB30">
-        <v>0.6301249900284742</v>
+        <v>0.6302457983438781</v>
       </c>
       <c r="AC30">
-        <v>1371.160730198868</v>
+        <v>1371.164454949497</v>
       </c>
       <c r="AD30">
-        <v>52.83367705558074</v>
+        <v>54.26496962000803</v>
       </c>
       <c r="AE30">
-        <v>0.2975395679732885</v>
+        <v>0.29753952309746</v>
       </c>
       <c r="AF30">
-        <v>1389.978008724147</v>
+        <v>1382.122976950466</v>
       </c>
       <c r="AG30">
-        <v>5.026667591335293</v>
+        <v>5.02666748000028</v>
       </c>
       <c r="AH30">
-        <v>1.785237407839778</v>
+        <v>14.87685135305244</v>
+      </c>
+      <c r="AI30">
+        <v>1293.444973994145</v>
+      </c>
+      <c r="AJ30">
+        <v>124.8439276784139</v>
+      </c>
+      <c r="AK30">
+        <v>16.08442405428351</v>
       </c>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:37">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -3637,100 +3898,109 @@
         <v>65</v>
       </c>
       <c r="C31">
-        <v>102.7771549213526</v>
+        <v>102.7772285692772</v>
       </c>
       <c r="D31">
-        <v>1286.565614092087</v>
+        <v>1286.565611801179</v>
       </c>
       <c r="E31">
-        <v>1583.912281281004</v>
+        <v>1583.864684543118</v>
       </c>
       <c r="F31">
-        <v>1286.565664094587</v>
+        <v>1286.565661803679</v>
       </c>
       <c r="G31">
-        <v>2353.181674154757</v>
+        <v>2352.569050375168</v>
       </c>
       <c r="H31">
-        <v>0.6309334075551256</v>
+        <v>0.6309513066634059</v>
       </c>
       <c r="I31">
-        <v>3.409036472528213</v>
+        <v>3.413060496520722</v>
       </c>
       <c r="J31">
-        <v>0.2976732085389794</v>
+        <v>0.2970538647294006</v>
       </c>
       <c r="K31">
-        <v>1.261866815110251</v>
+        <v>1.261902613326812</v>
       </c>
       <c r="L31" t="s">
         <v>70</v>
       </c>
       <c r="M31">
-        <v>1389.34286901844</v>
+        <v>1389.342940375456</v>
       </c>
       <c r="N31">
-        <v>2496.304250107215</v>
+        <v>2496.483487183542</v>
       </c>
       <c r="O31">
-        <v>1389.34281901594</v>
+        <v>1389.342890372956</v>
       </c>
       <c r="P31">
-        <v>3475.658623432715</v>
+        <v>3479.006923694167</v>
       </c>
       <c r="Q31">
-        <v>0.5867404667393311</v>
+        <v>0.5867880673485513</v>
       </c>
       <c r="S31">
-        <v>4.143861069791602</v>
+        <v>4.141285090056682</v>
       </c>
       <c r="T31">
-        <v>0.3200072061184527</v>
+        <v>0.3215288071153884</v>
       </c>
       <c r="U31">
-        <v>1.173480933478662</v>
+        <v>1.173576134697103</v>
       </c>
       <c r="V31" t="s">
         <v>70</v>
       </c>
       <c r="W31">
-        <v>1266.288328367928</v>
+        <v>1266.288335077386</v>
       </c>
       <c r="X31">
-        <v>260.4105054434503</v>
+        <v>259.9049369542465</v>
       </c>
       <c r="Y31">
-        <v>0.6834500396475989</v>
+        <v>0.683330201107119</v>
       </c>
       <c r="Z31">
-        <v>1410.617125967737</v>
+        <v>1410.617138983688</v>
       </c>
       <c r="AA31">
-        <v>364.085279018369</v>
+        <v>363.8353141494953</v>
       </c>
       <c r="AB31">
-        <v>0.6192954469362103</v>
+        <v>0.6194218091352323</v>
       </c>
       <c r="AC31">
-        <v>1371.167598403236</v>
+        <v>1371.184255196041</v>
       </c>
       <c r="AD31">
-        <v>40.98313942511325</v>
+        <v>45.40091710128078</v>
       </c>
       <c r="AE31">
-        <v>0.2930373748562188</v>
+        <v>0.293038184021251</v>
       </c>
       <c r="AF31">
-        <v>1390.380486262239</v>
+        <v>1382.125227141049</v>
       </c>
       <c r="AG31">
-        <v>3.946666262027783</v>
+        <v>3.946666260000218</v>
       </c>
       <c r="AH31">
-        <v>1.758275875049561</v>
+        <v>14.65134495160179</v>
+      </c>
+      <c r="AI31">
+        <v>1279.451065156078</v>
+      </c>
+      <c r="AJ31">
+        <v>2.653332592961221</v>
+      </c>
+      <c r="AK31">
+        <v>15.75951499737055</v>
       </c>
     </row>
-    <row r="32" spans="1:34">
+    <row r="32" spans="1:37">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -3738,100 +4008,109 @@
         <v>66</v>
       </c>
       <c r="C32">
-        <v>102.7805346452121</v>
+        <v>102.7813601111325</v>
       </c>
       <c r="D32">
-        <v>1286.584352825957</v>
+        <v>1286.584348235206</v>
       </c>
       <c r="E32">
-        <v>1310.050215853997</v>
+        <v>1310.005413624454</v>
       </c>
       <c r="F32">
-        <v>1286.584402828457</v>
+        <v>1286.584398237706</v>
       </c>
       <c r="G32">
-        <v>1945.273342552923</v>
+        <v>1944.772811874042</v>
       </c>
       <c r="H32">
-        <v>0.638152155805543</v>
+        <v>0.6381761678543481</v>
       </c>
       <c r="I32">
-        <v>2.870364897494821</v>
+        <v>2.875128372389924</v>
       </c>
       <c r="J32">
-        <v>0.2639881935208652</v>
+        <v>0.2633498119905987</v>
       </c>
       <c r="K32">
-        <v>1.276304311611086</v>
+        <v>1.276352335708696</v>
       </c>
       <c r="L32" t="s">
         <v>70</v>
       </c>
       <c r="M32">
-        <v>1389.36518748617</v>
+        <v>1389.365808351339</v>
       </c>
       <c r="N32">
-        <v>2064.500912142702</v>
+        <v>2068.474749286894</v>
       </c>
       <c r="O32">
-        <v>1389.364937473669</v>
+        <v>1389.365758348839</v>
       </c>
       <c r="P32">
-        <v>2801.007463963373</v>
+        <v>2858.114173362447</v>
       </c>
       <c r="Q32">
-        <v>0.5893830739149604</v>
+        <v>0.5896595412274436</v>
       </c>
       <c r="S32">
-        <v>2.89242556272526</v>
+        <v>2.930726314114268</v>
       </c>
       <c r="T32">
-        <v>0.2477880222093624</v>
+        <v>0.2840148363227043</v>
       </c>
       <c r="U32">
-        <v>1.178766147829921</v>
+        <v>1.179319082454887</v>
       </c>
       <c r="V32" t="s">
         <v>70</v>
       </c>
       <c r="W32">
-        <v>1266.315188939658</v>
+        <v>1266.31473042184</v>
       </c>
       <c r="X32">
-        <v>191.0164000710911</v>
+        <v>190.6097334015723</v>
       </c>
       <c r="Y32">
-        <v>0.7148878138603743</v>
+        <v>0.7148697402570848</v>
       </c>
       <c r="Z32">
-        <v>1410.613457841766</v>
+        <v>1410.613514845817</v>
       </c>
       <c r="AA32">
-        <v>293.0949451680685</v>
+        <v>291.8870836986122</v>
       </c>
       <c r="AB32">
-        <v>0.6045588776895386</v>
+        <v>0.60526840391162</v>
       </c>
       <c r="AC32">
-        <v>1370.823607890383</v>
+        <v>1371.185991745583</v>
       </c>
       <c r="AD32">
-        <v>39.65687671494177</v>
+        <v>42.34211465245085</v>
       </c>
       <c r="AE32">
-        <v>0.2944793646990267</v>
+        <v>0.2944758136565972</v>
       </c>
       <c r="AF32">
-        <v>1390.135729191089</v>
+        <v>1396.10643127472</v>
       </c>
       <c r="AG32">
-        <v>50.73887182449522</v>
+        <v>3.400000000000189</v>
       </c>
       <c r="AH32">
-        <v>1.766876424315585</v>
+        <v>14.72388432113223</v>
+      </c>
+      <c r="AI32">
+        <v>1279.44727389341</v>
+      </c>
+      <c r="AJ32">
+        <v>2.100000003515599</v>
+      </c>
+      <c r="AK32">
+        <v>15.93522113345558</v>
       </c>
     </row>
-    <row r="33" spans="1:34">
+    <row r="33" spans="1:37">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -3839,100 +4118,109 @@
         <v>67</v>
       </c>
       <c r="C33">
-        <v>102.7713412065482</v>
+        <v>102.7713398518249</v>
       </c>
       <c r="D33">
-        <v>1286.598046778287</v>
+        <v>1286.598044469672</v>
       </c>
       <c r="E33">
-        <v>1088.256538252867</v>
+        <v>1088.216683083583</v>
       </c>
       <c r="F33">
-        <v>1286.598096780787</v>
+        <v>1286.598094472172</v>
       </c>
       <c r="G33">
-        <v>1595.734126571619</v>
+        <v>1595.304759366684</v>
       </c>
       <c r="H33">
-        <v>0.6327017709503497</v>
+        <v>0.6327267822575772</v>
       </c>
       <c r="I33">
-        <v>2.771010839254505</v>
+        <v>2.775462627186402</v>
       </c>
       <c r="J33">
-        <v>0.2526010498836068</v>
+        <v>0.2519328485732725</v>
       </c>
       <c r="K33">
-        <v>1.265403541900699</v>
+        <v>1.265453564515154</v>
       </c>
       <c r="L33" t="s">
         <v>70</v>
       </c>
       <c r="M33">
-        <v>1389.369487989835</v>
+        <v>1389.369484326497</v>
       </c>
       <c r="N33">
-        <v>1733.793783626194</v>
+        <v>1733.957536393506</v>
       </c>
       <c r="O33">
-        <v>1389.369437987335</v>
+        <v>1389.369434323997</v>
       </c>
       <c r="P33">
-        <v>2392.739475623455</v>
+        <v>2393.60311126731</v>
       </c>
       <c r="Q33">
-        <v>0.5953419197786604</v>
+        <v>0.595248826369152</v>
       </c>
       <c r="S33">
-        <v>2.832078939604849</v>
+        <v>3.073379085011418</v>
       </c>
       <c r="T33">
-        <v>0.2534046998056544</v>
+        <v>0.2545499874272787</v>
       </c>
       <c r="U33">
-        <v>1.190683839557321</v>
+        <v>1.190497652738304</v>
       </c>
       <c r="V33" t="s">
         <v>70</v>
       </c>
       <c r="W33">
-        <v>1266.305772161574</v>
+        <v>1266.30577410924</v>
       </c>
       <c r="X33">
-        <v>159.1159350407097</v>
+        <v>158.7700036648057</v>
       </c>
       <c r="Y33">
-        <v>0.691769019102132</v>
+        <v>0.6918087597000544</v>
       </c>
       <c r="Z33">
-        <v>1410.596971456873</v>
+        <v>1410.596969628088</v>
       </c>
       <c r="AA33">
-        <v>239.6120461331453</v>
+        <v>239.4697732723918</v>
       </c>
       <c r="AB33">
-        <v>0.6034397199771269</v>
+        <v>0.603395683560995</v>
       </c>
       <c r="AC33">
-        <v>1370.838551666827</v>
+        <v>1372.279143866829</v>
       </c>
       <c r="AD33">
-        <v>33.24626346222346</v>
+        <v>25.74117358324341</v>
       </c>
       <c r="AE33">
-        <v>0.2973296907058455</v>
+        <v>0.06707769081172879</v>
       </c>
       <c r="AF33">
-        <v>1390.378539159779</v>
+        <v>1396.119052657059</v>
       </c>
       <c r="AG33">
-        <v>2.927999268000164</v>
+        <v>2.928014686635279</v>
       </c>
       <c r="AH33">
-        <v>11.83687684254998</v>
+        <v>14.86647759703322</v>
+      </c>
+      <c r="AI33">
+        <v>1279.491169799146</v>
+      </c>
+      <c r="AJ33">
+        <v>1.812000732075966</v>
+      </c>
+      <c r="AK33">
+        <v>15.80436866677322</v>
       </c>
     </row>
-    <row r="34" spans="1:34">
+    <row r="34" spans="1:37">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -3940,100 +4228,109 @@
         <v>68</v>
       </c>
       <c r="C34">
-        <v>102.768920631629</v>
+        <v>102.7690025152999</v>
       </c>
       <c r="D34">
-        <v>1286.609900207412</v>
+        <v>1286.609984993699</v>
       </c>
       <c r="E34">
-        <v>1029.254318875583</v>
+        <v>1029.188775113476</v>
       </c>
       <c r="F34">
-        <v>1286.609950209912</v>
+        <v>1286.609934991199</v>
       </c>
       <c r="G34">
-        <v>1500.313327263367</v>
+        <v>1499.647802438984</v>
       </c>
       <c r="H34">
-        <v>0.6237616531740494</v>
+        <v>0.6238054999275542</v>
       </c>
       <c r="I34">
-        <v>2.522790576415903</v>
+        <v>2.529145271540814</v>
       </c>
       <c r="J34">
-        <v>0.2762455713531488</v>
+        <v>0.2751457006022905</v>
       </c>
       <c r="K34">
-        <v>1.247523306348099</v>
+        <v>1.247610999855108</v>
       </c>
       <c r="L34" t="s">
         <v>70</v>
       </c>
       <c r="M34">
-        <v>1389.378920844041</v>
+        <v>1389.378887503998</v>
       </c>
       <c r="N34">
-        <v>1591.937755554214</v>
+        <v>1592.050150224253</v>
       </c>
       <c r="O34">
-        <v>1389.378870841541</v>
+        <v>1389.378937506498</v>
       </c>
       <c r="P34">
-        <v>2179.14259003314</v>
+        <v>2181.236997850418</v>
       </c>
       <c r="Q34">
-        <v>0.5904083205417551</v>
+        <v>0.5904543283158393</v>
       </c>
       <c r="S34">
-        <v>2.510312905566934</v>
+        <v>2.513224899319243</v>
       </c>
       <c r="T34">
-        <v>0.2545370189272815</v>
+        <v>0.2561198419930477</v>
       </c>
       <c r="U34">
-        <v>1.18081664108351</v>
+        <v>1.180908656631679</v>
       </c>
       <c r="V34" t="s">
         <v>70</v>
       </c>
       <c r="W34">
-        <v>1266.332772576304</v>
+        <v>1266.33277362229</v>
       </c>
       <c r="X34">
-        <v>157.9680906150324</v>
+        <v>157.9697643777457</v>
       </c>
       <c r="Y34">
-        <v>0.6127682915586752</v>
+        <v>0.612776123025752</v>
       </c>
       <c r="Z34">
-        <v>1410.623121562817</v>
+        <v>1410.62313548418</v>
       </c>
       <c r="AA34">
-        <v>200.7474923915191</v>
+        <v>200.5800263633021</v>
       </c>
       <c r="AB34">
-        <v>0.6342037441135279</v>
+        <v>0.6343230863785215</v>
       </c>
       <c r="AC34">
-        <v>1371.196176865055</v>
+        <v>1371.208137839467</v>
       </c>
       <c r="AD34">
-        <v>28.73758989782264</v>
+        <v>31.91959846709693</v>
       </c>
       <c r="AE34">
-        <v>0.2949201136066733</v>
+        <v>0.2949163777109329</v>
       </c>
       <c r="AF34">
-        <v>1390.439606556916</v>
+        <v>1382.11915567057</v>
       </c>
       <c r="AG34">
-        <v>2.484129548968456</v>
+        <v>2.484000244000137</v>
       </c>
       <c r="AH34">
-        <v>1.769544521088274</v>
+        <v>14.74599447687163</v>
+      </c>
+      <c r="AI34">
+        <v>1293.398036541638</v>
+      </c>
+      <c r="AJ34">
+        <v>1.780000126033564</v>
+      </c>
+      <c r="AK34">
+        <v>6.233520591337053</v>
       </c>
     </row>
-    <row r="35" spans="1:34">
+    <row r="35" spans="1:37">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -4041,97 +4338,106 @@
         <v>69</v>
       </c>
       <c r="C35">
-        <v>102.7591567312393</v>
+        <v>102.7602675722046</v>
       </c>
       <c r="D35">
-        <v>1286.618255419427</v>
+        <v>1286.618254988405</v>
       </c>
       <c r="E35">
-        <v>869.1145325597366</v>
+        <v>869.080939668228</v>
       </c>
       <c r="F35">
-        <v>1286.618305421927</v>
+        <v>1286.618304990905</v>
       </c>
       <c r="G35">
-        <v>1250.242750661209</v>
+        <v>1249.900778476057</v>
       </c>
       <c r="H35">
-        <v>0.6332231179342097</v>
+        <v>0.6332500362212475</v>
       </c>
       <c r="I35">
-        <v>2.456912130475217</v>
+        <v>2.462031311581896</v>
       </c>
       <c r="J35">
-        <v>0.1951163412968929</v>
+        <v>0.1944171538056184</v>
       </c>
       <c r="K35">
-        <v>1.266446235868419</v>
+        <v>1.266500072442495</v>
       </c>
       <c r="L35" t="s">
         <v>70</v>
       </c>
       <c r="M35">
-        <v>1389.377912175667</v>
+        <v>1389.37852256061</v>
       </c>
       <c r="N35">
-        <v>1386.887650916441</v>
+        <v>1391.09123811041</v>
       </c>
       <c r="O35">
-        <v>1389.377462153166</v>
+        <v>1389.37857256311</v>
       </c>
       <c r="P35">
-        <v>1836.849393633055</v>
+        <v>1895.266022735262</v>
       </c>
       <c r="Q35">
-        <v>0.5830985057719927</v>
+        <v>0.5834845192105496</v>
       </c>
       <c r="S35">
-        <v>2.259547848471676</v>
+        <v>2.279018049892208</v>
       </c>
       <c r="T35">
-        <v>0.2173250849403056</v>
+        <v>0.2739547470164674</v>
       </c>
       <c r="U35">
-        <v>1.166197011543985</v>
+        <v>1.166969038421099</v>
       </c>
       <c r="V35" t="s">
         <v>70</v>
       </c>
       <c r="W35">
-        <v>1266.318666400096</v>
+        <v>1266.318644145231</v>
       </c>
       <c r="X35">
-        <v>122.4810039223934</v>
+        <v>122.208518125967</v>
       </c>
       <c r="Y35">
-        <v>0.6949020374787976</v>
+        <v>0.6949585402962395</v>
       </c>
       <c r="Z35">
-        <v>1410.617729750225</v>
+        <v>1410.617821642817</v>
       </c>
       <c r="AA35">
-        <v>185.7684982865595</v>
+        <v>185.0295198892397</v>
       </c>
       <c r="AB35">
-        <v>0.6081205455923355</v>
+        <v>0.6087707202682061</v>
       </c>
       <c r="AC35">
-        <v>1371.183684888526</v>
+        <v>1371.201131942557</v>
       </c>
       <c r="AD35">
-        <v>25.6267695536324</v>
+        <v>29.22818299593447</v>
       </c>
       <c r="AE35">
-        <v>0.2914075732165767</v>
+        <v>0.2914060989362039</v>
       </c>
       <c r="AF35">
-        <v>1390.06955259625</v>
+        <v>1382.119532352629</v>
       </c>
       <c r="AG35">
-        <v>51.29854307716887</v>
+        <v>2.290006155309677</v>
       </c>
       <c r="AH35">
-        <v>1.748445477915376</v>
+        <v>14.57030589189413</v>
+      </c>
+      <c r="AI35">
+        <v>1279.524278658239</v>
+      </c>
+      <c r="AJ35">
+        <v>1.424000481230938</v>
+      </c>
+      <c r="AK35">
+        <v>15.81759572791232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
peak errors for ne and diadds - nans if not there
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Medium_Diads.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Medium_Diads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>filename</t>
   </si>
@@ -22,9 +22,18 @@
     <t>Splitting</t>
   </si>
   <si>
+    <t>Split_err_abs</t>
+  </si>
+  <si>
+    <t>Split_err_quadrature</t>
+  </si>
+  <si>
     <t>Diad1_Combofit_Cent</t>
   </si>
   <si>
+    <t>Diad1_cent_err</t>
+  </si>
+  <si>
     <t>Diad1_Combofit_Height</t>
   </si>
   <si>
@@ -50,6 +59,9 @@
   </si>
   <si>
     <t>Diad2_Combofit_Cent</t>
+  </si>
+  <si>
+    <t>Diad2_cent_err</t>
   </si>
   <si>
     <t>Diad2_Combofit_Height</t>
@@ -557,13 +569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:41">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,2242 +684,2350 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:41">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2">
-        <v>102.8051327964185</v>
-      </c>
-      <c r="D2">
-        <v>1286.621103908068</v>
-      </c>
-      <c r="E2">
-        <v>224.6095648437857</v>
+        <v>102.8051262264119</v>
       </c>
       <c r="F2">
-        <v>1286.621153910568</v>
+        <v>1286.621110480609</v>
       </c>
       <c r="G2">
-        <v>336.6721216990084</v>
+        <v>0.0102</v>
       </c>
       <c r="H2">
-        <v>0.6334875615034639</v>
+        <v>224.6092870872134</v>
       </c>
       <c r="I2">
-        <v>1.773253724212751</v>
+        <v>1286.621160483109</v>
       </c>
       <c r="J2">
-        <v>0.3111768758221626</v>
+        <v>336.6717722460721</v>
       </c>
       <c r="K2">
-        <v>1.266975123006928</v>
-      </c>
-      <c r="L2" t="s">
-        <v>61</v>
+        <v>0.633489358719682</v>
+      </c>
+      <c r="L2">
+        <v>1.773250077959958</v>
       </c>
       <c r="M2">
-        <v>1389.426336709486</v>
+        <v>0.3111695119442074</v>
       </c>
       <c r="N2">
-        <v>337.3526464967373</v>
-      </c>
-      <c r="O2">
-        <v>1389.426286706986</v>
+        <v>1.266978717439364</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
       </c>
       <c r="P2">
-        <v>474.5748669203644</v>
-      </c>
-      <c r="Q2">
-        <v>0.6039303686360886</v>
+        <v>1389.426336712021</v>
+      </c>
+      <c r="R2">
+        <v>337.3526464252443</v>
       </c>
       <c r="S2">
-        <v>1.60012168039366</v>
+        <v>1389.426286709521</v>
       </c>
       <c r="T2">
-        <v>0.2669154255606911</v>
+        <v>474.5748667817988</v>
       </c>
       <c r="U2">
-        <v>1.207860737272177</v>
-      </c>
-      <c r="V2" t="s">
-        <v>61</v>
+        <v>0.6039303688599593</v>
       </c>
       <c r="W2">
-        <v>1266.277894071709</v>
+        <v>1.60012168758843</v>
       </c>
       <c r="X2">
-        <v>31.9145414207134</v>
+        <v>0.2669154242825329</v>
       </c>
       <c r="Y2">
-        <v>0.5816280647885609</v>
-      </c>
-      <c r="Z2">
-        <v>1410.616237450954</v>
+        <v>1.207860737719919</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
       </c>
       <c r="AA2">
-        <v>29.67155335880512</v>
+        <v>1266.277893990354</v>
       </c>
       <c r="AB2">
-        <v>0.6517629216800432</v>
+        <v>31.91454943563645</v>
+      </c>
+      <c r="AC2">
+        <v>0.5816281463045017</v>
+      </c>
+      <c r="AD2">
+        <v>1410.616237452104</v>
+      </c>
+      <c r="AE2">
+        <v>29.67155334849159</v>
+      </c>
+      <c r="AF2">
+        <v>0.6517629253805296</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:41">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>102.9773628793794</v>
-      </c>
-      <c r="D3">
-        <v>1286.142237992318</v>
-      </c>
-      <c r="E3">
-        <v>920.492420180272</v>
+        <v>102.977379185882</v>
       </c>
       <c r="F3">
-        <v>1286.142287994818</v>
+        <v>1286.142237305786</v>
       </c>
       <c r="G3">
-        <v>1696.320600073124</v>
+        <v>0.00155</v>
       </c>
       <c r="H3">
-        <v>0.721292033514674</v>
+        <v>920.4924086324348</v>
       </c>
       <c r="I3">
-        <v>2.177296538793625</v>
+        <v>1286.142287308286</v>
       </c>
       <c r="J3">
-        <v>0.5175961623109532</v>
+        <v>1696.320589755973</v>
       </c>
       <c r="K3">
-        <v>1.442584067029348</v>
-      </c>
-      <c r="L3" t="s">
-        <v>61</v>
+        <v>0.721292047934459</v>
+      </c>
+      <c r="L3">
+        <v>2.177297269892438</v>
       </c>
       <c r="M3">
-        <v>1389.119700876697</v>
+        <v>0.5175961274162209</v>
       </c>
       <c r="N3">
-        <v>1509.63142689788</v>
-      </c>
-      <c r="O3">
-        <v>1389.119650874197</v>
+        <v>1.442584095868918</v>
+      </c>
+      <c r="O3" t="s">
+        <v>65</v>
       </c>
       <c r="P3">
-        <v>2452.141832282759</v>
-      </c>
-      <c r="Q3">
-        <v>0.6614310349468335</v>
+        <v>1389.119716496668</v>
+      </c>
+      <c r="R3">
+        <v>1509.579403321555</v>
       </c>
       <c r="S3">
-        <v>2.719342610231618</v>
+        <v>1389.119666494168</v>
       </c>
       <c r="T3">
-        <v>0.4130690349299858</v>
+        <v>2451.596265784035</v>
       </c>
       <c r="U3">
-        <v>1.322862069893667</v>
-      </c>
-      <c r="V3" t="s">
-        <v>61</v>
+        <v>0.6614774225610583</v>
       </c>
       <c r="W3">
-        <v>1265.962245344889</v>
+        <v>2.408481938513006</v>
       </c>
       <c r="X3">
-        <v>175.2227354328774</v>
+        <v>0.4123889455891819</v>
       </c>
       <c r="Y3">
-        <v>0.8996650840852876</v>
-      </c>
-      <c r="Z3">
-        <v>1410.402225359817</v>
+        <v>1.322954845122117</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>65</v>
       </c>
       <c r="AA3">
-        <v>224.0719426925021</v>
+        <v>1265.962245354878</v>
       </c>
       <c r="AB3">
-        <v>0.8577996511938711</v>
+        <v>175.2227423467431</v>
       </c>
       <c r="AC3">
-        <v>1372.05082916597</v>
+        <v>0.8996651646593313</v>
       </c>
       <c r="AD3">
-        <v>9.905293335230482</v>
+        <v>1410.402253905768</v>
       </c>
       <c r="AE3">
-        <v>0.3303980192469421</v>
+        <v>223.9012810243753</v>
+      </c>
+      <c r="AF3">
+        <v>0.8579376677918553</v>
+      </c>
+      <c r="AG3">
+        <v>1370.780035001478</v>
+      </c>
+      <c r="AH3">
+        <v>38.1357858046014</v>
+      </c>
+      <c r="AI3">
+        <v>0.3305482852942186</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:41">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>102.941197360678</v>
-      </c>
-      <c r="D4">
-        <v>1286.176034489468</v>
-      </c>
-      <c r="E4">
-        <v>1186.684630577492</v>
+        <v>102.9411904931269</v>
       </c>
       <c r="F4">
-        <v>1286.176084491968</v>
+        <v>1286.176034138752</v>
       </c>
       <c r="G4">
-        <v>2091.849038349718</v>
+        <v>0.00218</v>
       </c>
       <c r="H4">
-        <v>0.7007103613150235</v>
+        <v>1186.684634279051</v>
       </c>
       <c r="I4">
-        <v>3.208753139018645</v>
+        <v>1286.176084141252</v>
       </c>
       <c r="J4">
-        <v>0.4773604831687455</v>
+        <v>2091.849045338558</v>
       </c>
       <c r="K4">
-        <v>1.401420722630047</v>
-      </c>
-      <c r="L4" t="s">
-        <v>61</v>
+        <v>0.7007103571129424</v>
+      </c>
+      <c r="L4">
+        <v>3.208751005882271</v>
       </c>
       <c r="M4">
-        <v>1389.117331855146</v>
+        <v>0.4773604994384979</v>
       </c>
       <c r="N4">
-        <v>1895.843798092352</v>
-      </c>
-      <c r="O4">
-        <v>1389.117281852646</v>
+        <v>1.401420714225885</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
       </c>
       <c r="P4">
-        <v>3009.235486666579</v>
-      </c>
-      <c r="Q4">
-        <v>0.6438958746127023</v>
+        <v>1389.117324636879</v>
+      </c>
+      <c r="R4">
+        <v>1895.839455406573</v>
       </c>
       <c r="S4">
-        <v>3.05359273905546</v>
+        <v>1389.117274634379</v>
       </c>
       <c r="T4">
-        <v>0.4232279063877801</v>
+        <v>3009.188354174909</v>
       </c>
       <c r="U4">
-        <v>1.287791749225405</v>
-      </c>
-      <c r="V4" t="s">
-        <v>61</v>
+        <v>0.6438989544147339</v>
       </c>
       <c r="W4">
-        <v>1265.893517497353</v>
+        <v>3.124580128324887</v>
       </c>
       <c r="X4">
-        <v>264.7138845500049</v>
+        <v>0.4231801819671297</v>
       </c>
       <c r="Y4">
-        <v>0.9312797596004225</v>
-      </c>
-      <c r="Z4">
-        <v>1410.406811990126</v>
+        <v>1.287797908829468</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>65</v>
       </c>
       <c r="AA4">
-        <v>293.3078707532302</v>
+        <v>1265.893517512056</v>
       </c>
       <c r="AB4">
-        <v>0.7383919074714707</v>
+        <v>264.7138679601991</v>
       </c>
       <c r="AC4">
-        <v>1370.691170153234</v>
+        <v>0.9312796677855697</v>
       </c>
       <c r="AD4">
-        <v>38.9174131758708</v>
+        <v>1410.406812152842</v>
       </c>
       <c r="AE4">
-        <v>0.321767031737243</v>
+        <v>293.3029371466725</v>
+      </c>
+      <c r="AF4">
+        <v>0.738396947827581</v>
+      </c>
+      <c r="AG4">
+        <v>1371.198181380825</v>
+      </c>
+      <c r="AH4">
+        <v>38.86397924620814</v>
+      </c>
+      <c r="AI4">
+        <v>0.3217670311761398</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:41">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>102.7988483464787</v>
-      </c>
-      <c r="D5">
-        <v>1286.535171577091</v>
-      </c>
-      <c r="E5">
-        <v>220.4668566145194</v>
+        <v>102.7988371033789</v>
       </c>
       <c r="F5">
-        <v>1286.535221579591</v>
-      </c>
-      <c r="G5">
-        <v>340.9015786163991</v>
+        <v>1286.535186659185</v>
       </c>
       <c r="H5">
-        <v>0.6549803548661346</v>
+        <v>220.4669799005895</v>
       </c>
       <c r="I5">
-        <v>1.469520675634615</v>
+        <v>1286.535236661685</v>
       </c>
       <c r="J5">
-        <v>0.3050755185620552</v>
+        <v>340.9021062057939</v>
       </c>
       <c r="K5">
-        <v>1.309960709732269</v>
-      </c>
-      <c r="L5" t="s">
-        <v>61</v>
+        <v>0.6549797809222929</v>
+      </c>
+      <c r="L5">
+        <v>1.46953971543885</v>
       </c>
       <c r="M5">
-        <v>1389.334119928569</v>
+        <v>0.3050806832093069</v>
       </c>
       <c r="N5">
-        <v>323.7356502422034</v>
-      </c>
-      <c r="O5">
-        <v>1389.334069926069</v>
+        <v>1.309959561844586</v>
+      </c>
+      <c r="O5" t="s">
+        <v>65</v>
       </c>
       <c r="P5">
-        <v>469.0649744330171</v>
-      </c>
-      <c r="Q5">
-        <v>0.6131262978038413</v>
+        <v>1389.334123767564</v>
+      </c>
+      <c r="R5">
+        <v>323.7356851676585</v>
       </c>
       <c r="S5">
-        <v>1.696594512470026</v>
+        <v>1389.334073765064</v>
       </c>
       <c r="T5">
-        <v>0.3076190883320529</v>
+        <v>469.0650905278301</v>
       </c>
       <c r="U5">
-        <v>1.226252595607683</v>
-      </c>
-      <c r="V5" t="s">
-        <v>61</v>
+        <v>0.6131262076564963</v>
       </c>
       <c r="W5">
-        <v>1266.26027022904</v>
+        <v>1.696591719754426</v>
       </c>
       <c r="X5">
-        <v>41.32836032664527</v>
+        <v>0.3076198925420393</v>
       </c>
       <c r="Y5">
-        <v>1.043524539422343</v>
-      </c>
-      <c r="Z5">
-        <v>1410.629047976989</v>
+        <v>1.226252415312993</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>65</v>
       </c>
       <c r="AA5">
-        <v>47.13224273261184</v>
+        <v>1266.260282483029</v>
       </c>
       <c r="AB5">
-        <v>0.4712695706070757</v>
+        <v>41.32702709133547</v>
+      </c>
+      <c r="AC5">
+        <v>1.043574286436232</v>
+      </c>
+      <c r="AD5">
+        <v>1410.629047419488</v>
+      </c>
+      <c r="AE5">
+        <v>47.13234913422648</v>
+      </c>
+      <c r="AF5">
+        <v>0.4712792885736533</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:41">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6">
-        <v>102.7822141992342</v>
-      </c>
-      <c r="D6">
-        <v>1286.576893283737</v>
-      </c>
-      <c r="E6">
-        <v>212.8471844237235</v>
+        <v>102.782184022516</v>
       </c>
       <c r="F6">
-        <v>1286.576943286238</v>
-      </c>
-      <c r="G6">
-        <v>321.7275464265713</v>
+        <v>1286.576922436266</v>
       </c>
       <c r="H6">
-        <v>0.6456013182674454</v>
+        <v>212.8472553217206</v>
       </c>
       <c r="I6">
-        <v>1.906822995797115</v>
+        <v>1286.576972438766</v>
       </c>
       <c r="J6">
-        <v>0.2816478002688294</v>
+        <v>321.7276811283846</v>
       </c>
       <c r="K6">
-        <v>1.291202636534891</v>
-      </c>
-      <c r="L6" t="s">
-        <v>61</v>
+        <v>0.645601118220876</v>
+      </c>
+      <c r="L6">
+        <v>1.906805452887065</v>
       </c>
       <c r="M6">
-        <v>1389.359157485472</v>
+        <v>0.2816489157379291</v>
       </c>
       <c r="N6">
-        <v>326.0697837515762</v>
-      </c>
-      <c r="O6">
-        <v>1389.359157485472</v>
+        <v>1.291202236441752</v>
+      </c>
+      <c r="O6" t="s">
+        <v>65</v>
       </c>
       <c r="P6">
-        <v>437.8395530301093</v>
-      </c>
-      <c r="Q6">
-        <v>0.5974604741175547</v>
+        <v>1389.359156461282</v>
+      </c>
+      <c r="R6">
+        <v>326.0697986552468</v>
       </c>
       <c r="S6">
-        <v>1.901323688952621</v>
+        <v>1389.359156461282</v>
       </c>
       <c r="T6">
-        <v>0.1636316492523814</v>
+        <v>437.8395592172536</v>
       </c>
       <c r="U6">
-        <v>1.194920948235109</v>
-      </c>
-      <c r="V6" t="s">
-        <v>61</v>
+        <v>0.5974604161073844</v>
       </c>
       <c r="W6">
-        <v>1266.266090195165</v>
+        <v>1.901324066872183</v>
       </c>
       <c r="X6">
-        <v>37.56387187894458</v>
+        <v>0.1636318417913954</v>
       </c>
       <c r="Y6">
-        <v>0.6810094220841747</v>
-      </c>
-      <c r="Z6">
-        <v>1410.5838376193</v>
+        <v>1.194920832214769</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>65</v>
       </c>
       <c r="AA6">
-        <v>41.39469431468907</v>
+        <v>1266.266090067799</v>
       </c>
       <c r="AB6">
-        <v>0.6275779853898689</v>
+        <v>37.56392333611879</v>
+      </c>
+      <c r="AC6">
+        <v>0.6810107663658919</v>
+      </c>
+      <c r="AD6">
+        <v>1410.583837617139</v>
+      </c>
+      <c r="AE6">
+        <v>41.39469400661506</v>
+      </c>
+      <c r="AF6">
+        <v>0.6275779776486956</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:41">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C7">
-        <v>102.9753967288952</v>
-      </c>
-      <c r="D7">
-        <v>1286.103313582453</v>
-      </c>
-      <c r="E7">
-        <v>896.2525474751169</v>
+        <v>102.9753628956444</v>
       </c>
       <c r="F7">
-        <v>1286.103363584953</v>
-      </c>
-      <c r="G7">
-        <v>1639.448020717831</v>
+        <v>1286.103334474685</v>
       </c>
       <c r="H7">
-        <v>0.7329134281005496</v>
+        <v>896.2535036600909</v>
       </c>
       <c r="I7">
-        <v>2.028079917875056</v>
+        <v>1286.103384477185</v>
       </c>
       <c r="J7">
-        <v>0.4564158282433977</v>
+        <v>1639.450099033515</v>
       </c>
       <c r="K7">
-        <v>1.465826856201099</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
+        <v>0.7329119370511813</v>
+      </c>
+      <c r="L7">
+        <v>2.02806965606898</v>
       </c>
       <c r="M7">
-        <v>1389.078810316348</v>
+        <v>0.4564217403284296</v>
       </c>
       <c r="N7">
-        <v>1459.879669106917</v>
-      </c>
-      <c r="O7">
-        <v>1389.078760313848</v>
+        <v>1.465823874102363</v>
+      </c>
+      <c r="O7" t="s">
+        <v>65</v>
       </c>
       <c r="P7">
-        <v>2397.938301148521</v>
-      </c>
-      <c r="Q7">
-        <v>0.6625615057485711</v>
+        <v>1389.078797375329</v>
+      </c>
+      <c r="R7">
+        <v>1459.880697154655</v>
       </c>
       <c r="S7">
-        <v>2.150972324791249</v>
+        <v>1389.078747372829</v>
       </c>
       <c r="T7">
-        <v>0.4383625252308709</v>
+        <v>2397.939941069175</v>
       </c>
       <c r="U7">
-        <v>1.325123011497142</v>
-      </c>
-      <c r="V7" t="s">
-        <v>61</v>
+        <v>0.6625605956250965</v>
       </c>
       <c r="W7">
-        <v>1265.877697806367</v>
+        <v>2.150878361716104</v>
       </c>
       <c r="X7">
-        <v>171.4239382341091</v>
+        <v>0.4383661301312429</v>
       </c>
       <c r="Y7">
-        <v>0.9314475358862666</v>
-      </c>
-      <c r="Z7">
-        <v>1410.362999101218</v>
+        <v>1.325121191250193</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>65</v>
       </c>
       <c r="AA7">
-        <v>213.9624927739542</v>
+        <v>1265.877697763392</v>
       </c>
       <c r="AB7">
-        <v>0.7878570247636757</v>
+        <v>171.4237483733937</v>
       </c>
       <c r="AC7">
-        <v>1370.79740063136</v>
+        <v>0.9314460393823989</v>
       </c>
       <c r="AD7">
-        <v>28.52619354570651</v>
+        <v>1410.362999109011</v>
       </c>
       <c r="AE7">
-        <v>0.3310843762346936</v>
+        <v>213.9624725536328</v>
+      </c>
+      <c r="AF7">
+        <v>0.7878570022211167</v>
+      </c>
+      <c r="AG7">
+        <v>1370.797400474069</v>
+      </c>
+      <c r="AH7">
+        <v>28.52619844494455</v>
+      </c>
+      <c r="AI7">
+        <v>0.3310841147380467</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:41">
       <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C8">
-        <v>102.9470049142617</v>
-      </c>
-      <c r="D8">
-        <v>1286.145916891238</v>
-      </c>
-      <c r="E8">
-        <v>533.1729626495795</v>
+        <v>102.9470062375822</v>
       </c>
       <c r="F8">
-        <v>1286.145966893738</v>
-      </c>
-      <c r="G8">
-        <v>952.3507826533868</v>
+        <v>1286.145917245345</v>
       </c>
       <c r="H8">
-        <v>0.7296824986365448</v>
+        <v>533.1729638665158</v>
       </c>
       <c r="I8">
-        <v>1.975333645539415</v>
+        <v>1286.145967247845</v>
       </c>
       <c r="J8">
-        <v>0.4045213607449668</v>
+        <v>952.3507878896918</v>
       </c>
       <c r="K8">
-        <v>1.45936499727309</v>
-      </c>
-      <c r="L8" t="s">
-        <v>61</v>
+        <v>0.7296824962101843</v>
+      </c>
+      <c r="L8">
+        <v>1.975335828945617</v>
       </c>
       <c r="M8">
-        <v>1389.0930218105</v>
+        <v>0.4045213783871919</v>
       </c>
       <c r="N8">
-        <v>881.7126840541914</v>
-      </c>
-      <c r="O8">
-        <v>1389.092971808</v>
+        <v>1.459364992420369</v>
+      </c>
+      <c r="O8" t="s">
+        <v>65</v>
       </c>
       <c r="P8">
-        <v>1408.301188988288</v>
+        <v>1389.093023487927</v>
       </c>
       <c r="Q8">
-        <v>0.6445366290487803</v>
+        <v>0.00239</v>
+      </c>
+      <c r="R8">
+        <v>881.7104109585813</v>
       </c>
       <c r="S8">
-        <v>2.316100793083602</v>
+        <v>1389.092973485427</v>
       </c>
       <c r="T8">
-        <v>0.4372408592725923</v>
+        <v>1408.278260105434</v>
       </c>
       <c r="U8">
-        <v>1.289073258097561</v>
-      </c>
-      <c r="V8" t="s">
-        <v>61</v>
+        <v>0.6445401465653127</v>
       </c>
       <c r="W8">
-        <v>1265.889704663218</v>
+        <v>2.330519543285114</v>
       </c>
       <c r="X8">
-        <v>96.08361525871923</v>
+        <v>0.4371904608548771</v>
       </c>
       <c r="Y8">
-        <v>0.7312227659071487</v>
-      </c>
-      <c r="Z8">
-        <v>1410.415967472505</v>
+        <v>1.289080293130625</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>65</v>
       </c>
       <c r="AA8">
-        <v>122.9148779153306</v>
+        <v>1265.889704663077</v>
       </c>
       <c r="AB8">
-        <v>0.7367479309668697</v>
+        <v>96.08361579541474</v>
       </c>
       <c r="AC8">
-        <v>1370.813663324735</v>
+        <v>0.7312227776355612</v>
       </c>
       <c r="AD8">
-        <v>21.15289848868478</v>
+        <v>1410.415967401254</v>
       </c>
       <c r="AE8">
-        <v>0.3221032297840681</v>
+        <v>122.9114117632236</v>
+      </c>
+      <c r="AF8">
+        <v>0.7367565985914748</v>
+      </c>
+      <c r="AG8">
+        <v>1371.125107870915</v>
+      </c>
+      <c r="AH8">
+        <v>21.15284669706393</v>
+      </c>
+      <c r="AI8">
+        <v>0.3221032388999725</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:41">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>102.8162849112632</v>
-      </c>
-      <c r="D9">
-        <v>1286.343266797184</v>
-      </c>
-      <c r="E9">
-        <v>242.3293973742767</v>
+        <v>102.8162844541048</v>
       </c>
       <c r="F9">
-        <v>1286.343316799684</v>
+        <v>1286.343267465442</v>
       </c>
       <c r="G9">
-        <v>376.8360348321216</v>
+        <v>0.00526</v>
       </c>
       <c r="H9">
-        <v>0.6845724658097078</v>
+        <v>242.3293911527297</v>
       </c>
       <c r="I9">
-        <v>1.834991306176284</v>
+        <v>1286.343317467942</v>
       </c>
       <c r="J9">
-        <v>0.1949800896543405</v>
+        <v>376.8360384983733</v>
       </c>
       <c r="K9">
-        <v>1.369144931619416</v>
-      </c>
-      <c r="L9" t="s">
-        <v>61</v>
+        <v>0.6845725019348934</v>
+      </c>
+      <c r="L9">
+        <v>1.834990727366698</v>
       </c>
       <c r="M9">
-        <v>1389.159601710948</v>
+        <v>0.1949800377035091</v>
       </c>
       <c r="N9">
-        <v>369.5528597445702</v>
-      </c>
-      <c r="O9">
-        <v>1389.159601710948</v>
+        <v>1.369145003869787</v>
+      </c>
+      <c r="O9" t="s">
+        <v>65</v>
       </c>
       <c r="P9">
-        <v>535.6093785487344</v>
-      </c>
-      <c r="Q9">
-        <v>0.6173737915215406</v>
+        <v>1389.159601922047</v>
+      </c>
+      <c r="R9">
+        <v>369.552860876786</v>
       </c>
       <c r="S9">
-        <v>1.709877838097372</v>
+        <v>1389.159601922047</v>
       </c>
       <c r="T9">
-        <v>0.2889596547451765</v>
+        <v>535.6093869739776</v>
       </c>
       <c r="U9">
-        <v>1.234747583043081</v>
-      </c>
-      <c r="V9" t="s">
-        <v>61</v>
+        <v>0.6173737890091212</v>
       </c>
       <c r="W9">
-        <v>1266.092933634534</v>
+        <v>1.709878256674886</v>
       </c>
       <c r="X9">
-        <v>35.61084492571671</v>
+        <v>0.2889597018295515</v>
       </c>
       <c r="Y9">
-        <v>0.6664840574414921</v>
-      </c>
-      <c r="Z9">
-        <v>1410.383516711816</v>
+        <v>1.234747578018242</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>65</v>
       </c>
       <c r="AA9">
-        <v>36.70089385257007</v>
+        <v>1266.092934001882</v>
       </c>
       <c r="AB9">
-        <v>0.7005593354293703</v>
+        <v>35.61078195539379</v>
+      </c>
+      <c r="AC9">
+        <v>0.6664856042552408</v>
+      </c>
+      <c r="AD9">
+        <v>1410.38351671132</v>
+      </c>
+      <c r="AE9">
+        <v>36.70089377136598</v>
+      </c>
+      <c r="AF9">
+        <v>0.7005593340725396</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:41">
       <c r="A10" s="1">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10">
-        <v>102.8256676062556</v>
-      </c>
-      <c r="D10">
-        <v>1286.49725687143</v>
-      </c>
-      <c r="E10">
-        <v>445.3245632427923</v>
+        <v>102.825669543839</v>
       </c>
       <c r="F10">
-        <v>1286.49730687393</v>
-      </c>
-      <c r="G10">
-        <v>691.9152305829003</v>
+        <v>1286.497254643279</v>
       </c>
       <c r="H10">
-        <v>0.6637935802010833</v>
+        <v>445.32457671345</v>
       </c>
       <c r="I10">
-        <v>2.538396999939414</v>
+        <v>1286.497304645779</v>
       </c>
       <c r="J10">
-        <v>0.2808882371198119</v>
+        <v>691.9151787245454</v>
       </c>
       <c r="K10">
-        <v>1.327587160402167</v>
-      </c>
-      <c r="L10" t="s">
-        <v>61</v>
+        <v>0.6637935241262416</v>
+      </c>
+      <c r="L10">
+        <v>2.538390861102536</v>
       </c>
       <c r="M10">
-        <v>1389.323024482686</v>
+        <v>0.2808881787322722</v>
       </c>
       <c r="N10">
-        <v>685.1523042870402</v>
-      </c>
-      <c r="O10">
-        <v>1389.322974480186</v>
+        <v>1.327587048252483</v>
+      </c>
+      <c r="O10" t="s">
+        <v>65</v>
       </c>
       <c r="P10">
-        <v>996.5042687751529</v>
+        <v>1389.323024192118</v>
       </c>
       <c r="Q10">
-        <v>0.6148132362949696</v>
+        <v>0.0027</v>
+      </c>
+      <c r="R10">
+        <v>685.1522989133298</v>
       </c>
       <c r="S10">
-        <v>2.450160621889088</v>
+        <v>1389.322974189618</v>
       </c>
       <c r="T10">
-        <v>0.3104723430601229</v>
+        <v>996.5042669820286</v>
       </c>
       <c r="U10">
-        <v>1.229626472589939</v>
-      </c>
-      <c r="V10" t="s">
-        <v>61</v>
+        <v>0.6148132443534273</v>
       </c>
       <c r="W10">
-        <v>1266.257825993446</v>
+        <v>2.450158671928495</v>
       </c>
       <c r="X10">
-        <v>79.16349521259367</v>
+        <v>0.3104723243471091</v>
       </c>
       <c r="Y10">
-        <v>0.7282596136499765</v>
-      </c>
-      <c r="Z10">
-        <v>1410.524745331823</v>
+        <v>1.229626488706855</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>65</v>
       </c>
       <c r="AA10">
-        <v>84.5405918570309</v>
+        <v>1266.257825990973</v>
       </c>
       <c r="AB10">
-        <v>0.6356355005463731</v>
+        <v>79.16349728156347</v>
       </c>
       <c r="AC10">
-        <v>1371.320587582452</v>
+        <v>0.7282595759466393</v>
       </c>
       <c r="AD10">
-        <v>14.46072187168822</v>
+        <v>1410.524745331725</v>
       </c>
       <c r="AE10">
-        <v>0.3071240262808056</v>
+        <v>84.54059136004084</v>
+      </c>
+      <c r="AF10">
+        <v>0.6356355019024439</v>
+      </c>
+      <c r="AG10">
+        <v>1371.320589012113</v>
+      </c>
+      <c r="AH10">
+        <v>14.46084089688989</v>
+      </c>
+      <c r="AI10">
+        <v>0.3071388647385409</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:41">
       <c r="A11" s="1">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C11">
-        <v>102.8839773525358</v>
-      </c>
-      <c r="D11">
-        <v>1286.211853515998</v>
-      </c>
-      <c r="E11">
-        <v>670.6703104532046</v>
+        <v>102.8839614952153</v>
       </c>
       <c r="F11">
-        <v>1286.211903518498</v>
+        <v>1286.211853429656</v>
       </c>
       <c r="G11">
-        <v>1112.211286001372</v>
+        <v>0.00207</v>
       </c>
       <c r="H11">
-        <v>0.6717628123928286</v>
+        <v>670.6702827679284</v>
       </c>
       <c r="I11">
-        <v>2.1890121940446</v>
+        <v>1286.211903432156</v>
       </c>
       <c r="J11">
-        <v>0.4272433527498082</v>
+        <v>1112.211241168339</v>
       </c>
       <c r="K11">
-        <v>1.343525624785657</v>
-      </c>
-      <c r="L11" t="s">
-        <v>61</v>
+        <v>0.6717628704541425</v>
+      </c>
+      <c r="L11">
+        <v>2.189012146670507</v>
       </c>
       <c r="M11">
-        <v>1389.095930873534</v>
+        <v>0.42724312422121</v>
       </c>
       <c r="N11">
-        <v>1053.548406454446</v>
-      </c>
-      <c r="O11">
-        <v>1389.095880871034</v>
+        <v>1.343525740908285</v>
+      </c>
+      <c r="O11" t="s">
+        <v>65</v>
       </c>
       <c r="P11">
-        <v>1598.007126714926</v>
-      </c>
-      <c r="Q11">
-        <v>0.6296106906376087</v>
+        <v>1389.095914929872</v>
+      </c>
+      <c r="R11">
+        <v>1053.51652988304</v>
       </c>
       <c r="S11">
-        <v>2.400674788376821</v>
+        <v>1389.095864927372</v>
       </c>
       <c r="T11">
-        <v>0.3608681155529354</v>
+        <v>1597.663543641772</v>
       </c>
       <c r="U11">
-        <v>1.259221381275217</v>
-      </c>
-      <c r="V11" t="s">
-        <v>61</v>
+        <v>0.6296501864179226</v>
       </c>
       <c r="W11">
-        <v>1265.996708530521</v>
+        <v>2.22146759175629</v>
       </c>
       <c r="X11">
-        <v>117.7062374841545</v>
+        <v>0.3602035285787062</v>
       </c>
       <c r="Y11">
-        <v>0.8482814863614945</v>
-      </c>
-      <c r="Z11">
-        <v>1410.374922741191</v>
+        <v>1.259300372835845</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>65</v>
       </c>
       <c r="AA11">
-        <v>135.001251504146</v>
+        <v>1265.996708561338</v>
       </c>
       <c r="AB11">
-        <v>0.7110369532550208</v>
+        <v>117.7062467835221</v>
       </c>
       <c r="AC11">
-        <v>1369.2415188996</v>
+        <v>0.8482816117999092</v>
       </c>
       <c r="AD11">
-        <v>6.35468549849708</v>
+        <v>1410.374920951534</v>
       </c>
       <c r="AE11">
-        <v>0.3146811627985963</v>
+        <v>134.9246893742745</v>
+      </c>
+      <c r="AF11">
+        <v>0.7110825690567238</v>
+      </c>
+      <c r="AG11">
+        <v>1370.762660851905</v>
+      </c>
+      <c r="AH11">
+        <v>23.88565134091537</v>
+      </c>
+      <c r="AI11">
+        <v>0.3146811624156554</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:41">
       <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <v>102.8799710801579</v>
+        <v>102.8799708250515</v>
       </c>
       <c r="D12">
-        <v>1286.38482758847</v>
+        <v>0.00516</v>
       </c>
       <c r="E12">
-        <v>698.6658507658452</v>
+        <v>0.003832831851255674</v>
       </c>
       <c r="F12">
-        <v>1286.38487759097</v>
+        <v>1286.384827687597</v>
       </c>
       <c r="G12">
-        <v>1132.089049622668</v>
+        <v>0.00341</v>
       </c>
       <c r="H12">
-        <v>0.673675643316465</v>
+        <v>698.6658121509895</v>
       </c>
       <c r="I12">
-        <v>3.323831515944308</v>
+        <v>1286.384877690097</v>
       </c>
       <c r="J12">
-        <v>0.3567173681449545</v>
+        <v>1132.089003958096</v>
       </c>
       <c r="K12">
-        <v>1.34735128663293</v>
-      </c>
-      <c r="L12" t="s">
-        <v>61</v>
+        <v>0.6736757215706247</v>
+      </c>
+      <c r="L12">
+        <v>3.323831567386825</v>
       </c>
       <c r="M12">
-        <v>1389.264898673628</v>
+        <v>0.3567170903060659</v>
       </c>
       <c r="N12">
-        <v>1089.0249876526</v>
-      </c>
-      <c r="O12">
-        <v>1389.264848671128</v>
+        <v>1.347351443141249</v>
+      </c>
+      <c r="O12" t="s">
+        <v>65</v>
       </c>
       <c r="P12">
-        <v>1628.648714158959</v>
+        <v>1389.264898517649</v>
       </c>
       <c r="Q12">
-        <v>0.622979350967543</v>
+        <v>0.00175</v>
+      </c>
+      <c r="R12">
+        <v>1089.025033494374</v>
       </c>
       <c r="S12">
-        <v>3.198926052527487</v>
+        <v>1389.264848515149</v>
       </c>
       <c r="T12">
-        <v>0.3511172911610337</v>
+        <v>1628.649055545497</v>
       </c>
       <c r="U12">
-        <v>1.245958701935086</v>
-      </c>
-      <c r="V12" t="s">
-        <v>61</v>
+        <v>0.6229793032490016</v>
       </c>
       <c r="W12">
-        <v>1266.153692399769</v>
+        <v>3.198961169222632</v>
       </c>
       <c r="X12">
-        <v>141.0612932153125</v>
+        <v>0.3511179524706031</v>
       </c>
       <c r="Y12">
-        <v>0.8177399303614363</v>
-      </c>
-      <c r="Z12">
-        <v>1410.54467637421</v>
+        <v>1.245958606498003</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>65</v>
       </c>
       <c r="AA12">
-        <v>143.4327210778297</v>
+        <v>1266.153692425157</v>
       </c>
       <c r="AB12">
-        <v>0.7089605195535773</v>
+        <v>141.0613064727752</v>
       </c>
       <c r="AC12">
-        <v>1370.813214155514</v>
+        <v>0.8177401423805134</v>
       </c>
       <c r="AD12">
-        <v>25.46985585367214</v>
+        <v>1410.544676416127</v>
       </c>
       <c r="AE12">
-        <v>0.3112640983253521</v>
+        <v>143.4328292823186</v>
+      </c>
+      <c r="AF12">
+        <v>0.7089602174971477</v>
+      </c>
+      <c r="AG12">
+        <v>1370.813354629604</v>
+      </c>
+      <c r="AH12">
+        <v>25.45474842591003</v>
+      </c>
+      <c r="AI12">
+        <v>0.3112643244689797</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:41">
       <c r="A13" s="1">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C13">
-        <v>103.2406692169659</v>
-      </c>
-      <c r="D13">
-        <v>1285.256591935198</v>
-      </c>
-      <c r="E13">
-        <v>1317.575522605646</v>
+        <v>103.2407526560826</v>
       </c>
       <c r="F13">
-        <v>1285.256641937698</v>
+        <v>1285.256507639644</v>
       </c>
       <c r="G13">
-        <v>3642.838089784352</v>
+        <v>0.00434</v>
       </c>
       <c r="H13">
-        <v>1.0694979229737</v>
+        <v>1317.567856374078</v>
       </c>
       <c r="I13">
-        <v>5.158550895200162</v>
+        <v>1285.256557642145</v>
       </c>
       <c r="J13">
-        <v>0.5487646670347111</v>
+        <v>3642.827329522499</v>
       </c>
       <c r="K13">
-        <v>2.138995845947399</v>
-      </c>
-      <c r="L13" t="s">
-        <v>61</v>
+        <v>1.06951148804293</v>
+      </c>
+      <c r="L13">
+        <v>5.158473685529163</v>
       </c>
       <c r="M13">
-        <v>1388.497361157164</v>
+        <v>0.5487396165936755</v>
       </c>
       <c r="N13">
-        <v>2614.346905430794</v>
-      </c>
-      <c r="O13">
-        <v>1388.497311154664</v>
+        <v>2.139022976085859</v>
+      </c>
+      <c r="O13" t="s">
+        <v>65</v>
       </c>
       <c r="P13">
-        <v>5703.342590015319</v>
-      </c>
-      <c r="Q13">
-        <v>0.8345507893169486</v>
+        <v>1388.497360300727</v>
+      </c>
+      <c r="R13">
+        <v>2614.346866297241</v>
       </c>
       <c r="S13">
-        <v>6.039980641260808</v>
+        <v>1388.497310298227</v>
       </c>
       <c r="T13">
-        <v>0.5763104057455379</v>
+        <v>5703.342282620076</v>
       </c>
       <c r="U13">
-        <v>1.669101578633897</v>
-      </c>
-      <c r="V13" t="s">
-        <v>61</v>
+        <v>0.8345508183546948</v>
       </c>
       <c r="W13">
-        <v>1265.210433171389</v>
+        <v>6.039937505589244</v>
       </c>
       <c r="X13">
-        <v>598.5778457300114</v>
+        <v>0.5763102206370844</v>
       </c>
       <c r="Y13">
-        <v>1.408322822543904</v>
-      </c>
-      <c r="Z13">
-        <v>1409.876605525325</v>
+        <v>1.66910163670939</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>65</v>
       </c>
       <c r="AA13">
-        <v>827.4070384789757</v>
+        <v>1265.210426991729</v>
       </c>
       <c r="AB13">
-        <v>1.024648589655742</v>
+        <v>598.5785755265007</v>
       </c>
       <c r="AC13">
-        <v>1370.333924172893</v>
+        <v>1.408326862653552</v>
       </c>
       <c r="AD13">
-        <v>69.89268595640088</v>
+        <v>1409.87660779709</v>
       </c>
       <c r="AE13">
-        <v>0.416561547477587</v>
+        <v>827.4069615449235</v>
+      </c>
+      <c r="AF13">
+        <v>1.024648521935259</v>
+      </c>
+      <c r="AG13">
+        <v>1370.334358037827</v>
+      </c>
+      <c r="AH13">
+        <v>69.89269560545142</v>
+      </c>
+      <c r="AI13">
+        <v>0.4165638369873404</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:41">
       <c r="A14" s="1">
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C14">
-        <v>103.4175684588245</v>
+        <v>103.4175759084455</v>
       </c>
       <c r="D14">
-        <v>1284.884331500116</v>
+        <v>0.00622</v>
       </c>
       <c r="E14">
-        <v>548.8707047473686</v>
+        <v>0.004679529890918531</v>
       </c>
       <c r="F14">
-        <v>1284.884381502616</v>
+        <v>1284.884324022997</v>
       </c>
       <c r="G14">
-        <v>1568.727857456917</v>
+        <v>0.00424</v>
       </c>
       <c r="H14">
-        <v>1.079876048017075</v>
+        <v>548.870592428805</v>
       </c>
       <c r="I14">
-        <v>2.266667123825623</v>
+        <v>1284.884374025497</v>
       </c>
       <c r="J14">
-        <v>0.6081752765575441</v>
+        <v>1568.727855624164</v>
       </c>
       <c r="K14">
-        <v>2.159752096034151</v>
-      </c>
-      <c r="L14" t="s">
-        <v>61</v>
+        <v>1.079876553958562</v>
+      </c>
+      <c r="L14">
+        <v>2.266668620956077</v>
       </c>
       <c r="M14">
-        <v>1388.30199996394</v>
+        <v>0.6081745976606566</v>
       </c>
       <c r="N14">
-        <v>1107.908305849883</v>
-      </c>
-      <c r="O14">
-        <v>1388.30194996144</v>
+        <v>2.159753107917125</v>
+      </c>
+      <c r="O14" t="s">
+        <v>65</v>
       </c>
       <c r="P14">
-        <v>2483.438687129107</v>
+        <v>1388.301999936442</v>
       </c>
       <c r="Q14">
-        <v>0.8460227503622403</v>
+        <v>0.00198</v>
+      </c>
+      <c r="R14">
+        <v>1107.908324311775</v>
       </c>
       <c r="S14">
-        <v>2.626234881019077</v>
+        <v>1388.301949933942</v>
       </c>
       <c r="T14">
-        <v>0.6100577212331293</v>
+        <v>2483.438817489297</v>
       </c>
       <c r="U14">
-        <v>1.692045500724481</v>
-      </c>
-      <c r="V14" t="s">
-        <v>61</v>
+        <v>0.8460227222768254</v>
       </c>
       <c r="W14">
-        <v>1264.775061888523</v>
+        <v>2.62623483381322</v>
       </c>
       <c r="X14">
-        <v>205.7976823870244</v>
+        <v>0.6100578820840227</v>
       </c>
       <c r="Y14">
-        <v>1.756105138080783</v>
-      </c>
-      <c r="Z14">
-        <v>1409.712217150915</v>
+        <v>1.692045444553651</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>65</v>
       </c>
       <c r="AA14">
-        <v>252.3621494109725</v>
+        <v>1264.775060447557</v>
       </c>
       <c r="AB14">
-        <v>1.207142153883158</v>
+        <v>205.7965588732365</v>
       </c>
       <c r="AC14">
-        <v>1370.308160135203</v>
+        <v>1.756088685001467</v>
       </c>
       <c r="AD14">
-        <v>29.23932244692024</v>
+        <v>1409.712217537225</v>
       </c>
       <c r="AE14">
-        <v>0.4223651982848688</v>
+        <v>252.3622326523478</v>
+      </c>
+      <c r="AF14">
+        <v>1.207142695238841</v>
+      </c>
+      <c r="AG14">
+        <v>1370.308094073177</v>
+      </c>
+      <c r="AH14">
+        <v>29.23932648474871</v>
+      </c>
+      <c r="AI14">
+        <v>0.42236519750809</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:41">
       <c r="A15" s="1">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C15">
-        <v>102.8075424291264</v>
-      </c>
-      <c r="D15">
-        <v>1286.514202372594</v>
-      </c>
-      <c r="E15">
-        <v>2008.914188789368</v>
+        <v>102.8075406705368</v>
       </c>
       <c r="F15">
-        <v>1286.514252375094</v>
-      </c>
-      <c r="G15">
-        <v>3122.915530897227</v>
+        <v>1286.514204893072</v>
       </c>
       <c r="H15">
-        <v>0.6526553125753735</v>
+        <v>2008.914260598205</v>
       </c>
       <c r="I15">
-        <v>4.204885189637687</v>
+        <v>1286.514254895572</v>
       </c>
       <c r="J15">
-        <v>0.3296168494902199</v>
+        <v>3122.915991113221</v>
       </c>
       <c r="K15">
-        <v>1.305310625150747</v>
-      </c>
-      <c r="L15" t="s">
-        <v>61</v>
+        <v>0.6526552905147924</v>
+      </c>
+      <c r="L15">
+        <v>4.204919401373114</v>
       </c>
       <c r="M15">
-        <v>1389.321844806721</v>
+        <v>0.3296172528337404</v>
       </c>
       <c r="N15">
-        <v>3159.984267854009</v>
-      </c>
-      <c r="O15">
-        <v>1389.321794804221</v>
+        <v>1.305310581029585</v>
+      </c>
+      <c r="O15" t="s">
+        <v>65</v>
       </c>
       <c r="P15">
-        <v>4531.586008247516</v>
-      </c>
-      <c r="Q15">
-        <v>0.6011757372061404</v>
+        <v>1389.321845568609</v>
+      </c>
+      <c r="R15">
+        <v>3159.984454362522</v>
       </c>
       <c r="S15">
-        <v>4.632487450509042</v>
+        <v>1389.321795566109</v>
       </c>
       <c r="T15">
-        <v>0.3336840784003293</v>
+        <v>4531.58641780378</v>
       </c>
       <c r="U15">
-        <v>1.202351474412281</v>
-      </c>
-      <c r="V15" t="s">
-        <v>61</v>
+        <v>0.6011756771285541</v>
       </c>
       <c r="W15">
-        <v>1266.227159769334</v>
+        <v>4.632487688301636</v>
       </c>
       <c r="X15">
-        <v>333.6948851000019</v>
+        <v>0.3336844422104223</v>
       </c>
       <c r="Y15">
-        <v>0.7485086536045773</v>
-      </c>
-      <c r="Z15">
-        <v>1410.567798754558</v>
+        <v>1.202351354257108</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>65</v>
       </c>
       <c r="AA15">
-        <v>476.5993037731722</v>
+        <v>1266.227159805614</v>
       </c>
       <c r="AB15">
-        <v>0.6422316532294743</v>
+        <v>333.6949377337923</v>
       </c>
       <c r="AC15">
-        <v>1370.780209890175</v>
+        <v>0.7485084566007645</v>
       </c>
       <c r="AD15">
-        <v>68.78520245812336</v>
+        <v>1410.567798852632</v>
       </c>
       <c r="AE15">
-        <v>0.3002648921484626</v>
+        <v>476.5994927890397</v>
+      </c>
+      <c r="AF15">
+        <v>0.6422314048185552</v>
+      </c>
+      <c r="AG15">
+        <v>1370.780209677061</v>
+      </c>
+      <c r="AH15">
+        <v>68.78535831796582</v>
+      </c>
+      <c r="AI15">
+        <v>0.3002648916955102</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:41">
       <c r="A16" s="1">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C16">
-        <v>102.8040687849593</v>
+        <v>102.8040676989845</v>
       </c>
       <c r="D16">
-        <v>1286.536040982289</v>
+        <v>0.00379</v>
       </c>
       <c r="E16">
-        <v>1867.371704238277</v>
+        <v>0.00293429719012918</v>
       </c>
       <c r="F16">
-        <v>1286.53609098479</v>
+        <v>1286.536041903987</v>
       </c>
       <c r="G16">
-        <v>2830.026406221277</v>
+        <v>0.00274</v>
       </c>
       <c r="H16">
-        <v>0.6441903631154997</v>
+        <v>1867.37187256253</v>
       </c>
       <c r="I16">
-        <v>4.130815138498445</v>
+        <v>1286.536091906487</v>
       </c>
       <c r="J16">
-        <v>0.2951314203376115</v>
+        <v>2830.026805143377</v>
       </c>
       <c r="K16">
-        <v>1.288380726230999</v>
-      </c>
-      <c r="L16" t="s">
-        <v>61</v>
+        <v>0.6441902574101334</v>
+      </c>
+      <c r="L16">
+        <v>4.130827135001509</v>
       </c>
       <c r="M16">
-        <v>1389.340209772249</v>
+        <v>0.2951320235928219</v>
       </c>
       <c r="N16">
-        <v>2912.80160817891</v>
-      </c>
-      <c r="O16">
-        <v>1389.340159769749</v>
+        <v>1.288380514820267</v>
+      </c>
+      <c r="O16" t="s">
+        <v>65</v>
       </c>
       <c r="P16">
-        <v>4097.731265394501</v>
+        <v>1389.340209607972</v>
       </c>
       <c r="Q16">
-        <v>0.5956978185123104</v>
+        <v>0.00105</v>
+      </c>
+      <c r="R16">
+        <v>2912.801363331351</v>
       </c>
       <c r="S16">
-        <v>3.718900419888892</v>
+        <v>1389.340159605472</v>
       </c>
       <c r="T16">
-        <v>0.3057330776527357</v>
+        <v>4097.729640104473</v>
       </c>
       <c r="U16">
-        <v>1.191395637024621</v>
-      </c>
-      <c r="V16" t="s">
-        <v>61</v>
+        <v>0.5956978871889227</v>
       </c>
       <c r="W16">
-        <v>1266.272922900488</v>
+        <v>3.677807083267532</v>
       </c>
       <c r="X16">
-        <v>313.8405626846372</v>
+        <v>0.3057320108676663</v>
       </c>
       <c r="Y16">
-        <v>0.6966488070303702</v>
-      </c>
-      <c r="Z16">
-        <v>1410.586485816279</v>
+        <v>1.191395774377845</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>65</v>
       </c>
       <c r="AA16">
-        <v>420.0203640868002</v>
+        <v>1266.272922893443</v>
       </c>
       <c r="AB16">
-        <v>0.6301520475950164</v>
+        <v>313.8405554472529</v>
       </c>
       <c r="AC16">
-        <v>1371.16500531966</v>
+        <v>0.6966487610176202</v>
       </c>
       <c r="AD16">
-        <v>54.51303954161853</v>
+        <v>1410.586485956184</v>
       </c>
       <c r="AE16">
-        <v>0.2975393577618558</v>
+        <v>420.0147821785297</v>
+      </c>
+      <c r="AF16">
+        <v>0.6301561964836089</v>
+      </c>
+      <c r="AG16">
+        <v>1370.800342653851</v>
+      </c>
+      <c r="AH16">
+        <v>57.24326914478986</v>
+      </c>
+      <c r="AI16">
+        <v>0.297539635039088</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:35">
       <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C17">
-        <v>102.7772218473824</v>
-      </c>
-      <c r="D17">
-        <v>1286.565613266467</v>
-      </c>
-      <c r="E17">
-        <v>1583.911911110886</v>
+        <v>102.7772240230677</v>
       </c>
       <c r="F17">
-        <v>1286.565663268967</v>
+        <v>1286.565613961279</v>
       </c>
       <c r="G17">
-        <v>2353.181203222683</v>
+        <v>0.00178</v>
       </c>
       <c r="H17">
-        <v>0.6309336987531149</v>
+        <v>1583.912019479877</v>
       </c>
       <c r="I17">
-        <v>3.409029861299755</v>
+        <v>1286.565663963779</v>
       </c>
       <c r="J17">
-        <v>0.2976720022875365</v>
+        <v>2353.181434212452</v>
       </c>
       <c r="K17">
-        <v>1.26186739750623</v>
-      </c>
-      <c r="L17" t="s">
-        <v>61</v>
+        <v>0.6309336198132111</v>
+      </c>
+      <c r="L17">
+        <v>3.409027440891033</v>
       </c>
       <c r="M17">
-        <v>1389.34293511885</v>
+        <v>0.2976724365878834</v>
       </c>
       <c r="N17">
-        <v>2496.623466795795</v>
-      </c>
-      <c r="O17">
-        <v>1389.34288511635</v>
+        <v>1.261867239626422</v>
+      </c>
+      <c r="O17" t="s">
+        <v>65</v>
       </c>
       <c r="P17">
-        <v>3480.000482950097</v>
-      </c>
-      <c r="Q17">
-        <v>0.5867467380322553</v>
+        <v>1389.342937989346</v>
+      </c>
+      <c r="R17">
+        <v>2496.634724744991</v>
       </c>
       <c r="S17">
-        <v>4.139836476519936</v>
+        <v>1389.342887986846</v>
       </c>
       <c r="T17">
-        <v>0.322256919060992</v>
+        <v>3480.050696420718</v>
       </c>
       <c r="U17">
-        <v>1.173493476064511</v>
-      </c>
-      <c r="V17" t="s">
-        <v>61</v>
+        <v>0.586742003609601</v>
       </c>
       <c r="W17">
-        <v>1266.288326959437</v>
+        <v>4.155197464541771</v>
       </c>
       <c r="X17">
-        <v>260.4092697107822</v>
+        <v>0.3223060693312403</v>
       </c>
       <c r="Y17">
-        <v>0.6834611758830685</v>
-      </c>
-      <c r="Z17">
-        <v>1410.617128272411</v>
+        <v>1.173484007219202</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>65</v>
       </c>
       <c r="AA17">
-        <v>364.0254055943382</v>
+        <v>1266.288326968617</v>
       </c>
       <c r="AB17">
-        <v>0.6193297955147703</v>
+        <v>260.4092680589347</v>
       </c>
       <c r="AC17">
-        <v>1371.183976082243</v>
+        <v>0.6834611580882213</v>
       </c>
       <c r="AD17">
-        <v>45.37457197127005</v>
+        <v>1410.617128229772</v>
       </c>
       <c r="AE17">
-        <v>0.2930389977176356</v>
+        <v>364.0307205016263</v>
+      </c>
+      <c r="AF17">
+        <v>0.6193241887705594</v>
+      </c>
+      <c r="AG17">
+        <v>1370.813596456425</v>
+      </c>
+      <c r="AH17">
+        <v>44.37567273108929</v>
+      </c>
+      <c r="AI17">
+        <v>0.2930389992530438</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:35">
       <c r="A18" s="1">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C18">
-        <v>102.7813471400002</v>
-      </c>
-      <c r="D18">
-        <v>1286.58435078831</v>
-      </c>
-      <c r="E18">
-        <v>1310.047056858942</v>
+        <v>102.7813471705254</v>
       </c>
       <c r="F18">
-        <v>1286.58440079081</v>
+        <v>1286.58434964045</v>
       </c>
       <c r="G18">
-        <v>1945.264480109814</v>
+        <v>0.00137</v>
       </c>
       <c r="H18">
-        <v>0.6381555658175554</v>
+        <v>1310.046538675736</v>
       </c>
       <c r="I18">
-        <v>2.870300897608056</v>
+        <v>1286.58439964295</v>
       </c>
       <c r="J18">
-        <v>0.263966951917444</v>
+        <v>1945.264508270439</v>
       </c>
       <c r="K18">
-        <v>1.276311131635111</v>
-      </c>
-      <c r="L18" t="s">
-        <v>61</v>
+        <v>0.638156057461966</v>
+      </c>
+      <c r="L18">
+        <v>2.870289284049282</v>
       </c>
       <c r="M18">
-        <v>1389.36579793331</v>
+        <v>0.2639659338727581</v>
       </c>
       <c r="N18">
-        <v>2068.595541968048</v>
-      </c>
-      <c r="O18">
-        <v>1389.36574793081</v>
+        <v>1.276312114923932</v>
+      </c>
+      <c r="O18" t="s">
+        <v>65</v>
       </c>
       <c r="P18">
-        <v>2858.975286166056</v>
-      </c>
-      <c r="Q18">
-        <v>0.5896169171331563</v>
+        <v>1389.365796815976</v>
+      </c>
+      <c r="R18">
+        <v>2068.595834111156</v>
       </c>
       <c r="S18">
-        <v>2.925517558456856</v>
+        <v>1389.365746813475</v>
       </c>
       <c r="T18">
-        <v>0.2847908263597263</v>
+        <v>2858.976195189386</v>
       </c>
       <c r="U18">
-        <v>1.179233834266313</v>
-      </c>
-      <c r="V18" t="s">
-        <v>61</v>
+        <v>0.5896167585703433</v>
       </c>
       <c r="W18">
-        <v>1266.315190837879</v>
+        <v>2.925351511344183</v>
       </c>
       <c r="X18">
-        <v>191.0186028790901</v>
+        <v>0.2847920672120289</v>
       </c>
       <c r="Y18">
-        <v>0.7148754909714494</v>
-      </c>
-      <c r="Z18">
-        <v>1410.613490104828</v>
+        <v>1.179233517140687</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>65</v>
       </c>
       <c r="AA18">
-        <v>292.4900649944389</v>
+        <v>1266.315190607358</v>
       </c>
       <c r="AB18">
-        <v>0.60493833714416</v>
+        <v>191.0197512725757</v>
       </c>
       <c r="AC18">
-        <v>1371.186183182088</v>
+        <v>0.7148731489816416</v>
       </c>
       <c r="AD18">
-        <v>42.4114884035527</v>
+        <v>1410.61349017381</v>
       </c>
       <c r="AE18">
-        <v>0.2944795008153289</v>
+        <v>292.4890936308656</v>
+      </c>
+      <c r="AF18">
+        <v>0.6049404630671454</v>
+      </c>
+      <c r="AG18">
+        <v>1371.186065479649</v>
+      </c>
+      <c r="AH18">
+        <v>42.38028606710211</v>
+      </c>
+      <c r="AI18">
+        <v>0.2944792148548661</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:35">
       <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C19">
-        <v>102.7713338218564</v>
-      </c>
-      <c r="D19">
-        <v>1286.598046835405</v>
-      </c>
-      <c r="E19">
-        <v>1088.256839476351</v>
+        <v>102.7713274842895</v>
       </c>
       <c r="F19">
-        <v>1286.598096837905</v>
+        <v>1286.598044746033</v>
       </c>
       <c r="G19">
-        <v>1595.734431024726</v>
+        <v>0.00239</v>
       </c>
       <c r="H19">
-        <v>0.6327014046224994</v>
+        <v>1088.256533143961</v>
       </c>
       <c r="I19">
-        <v>2.77101170607455</v>
+        <v>1286.598094748533</v>
       </c>
       <c r="J19">
-        <v>0.252602454038599</v>
+        <v>1595.734031515814</v>
       </c>
       <c r="K19">
-        <v>1.265402809244999</v>
-      </c>
-      <c r="L19" t="s">
-        <v>61</v>
+        <v>0.6327017632761961</v>
+      </c>
+      <c r="L19">
+        <v>2.771016323568558</v>
       </c>
       <c r="M19">
-        <v>1389.369480662261</v>
+        <v>0.252600928266034</v>
       </c>
       <c r="N19">
-        <v>1733.906898980159</v>
-      </c>
-      <c r="O19">
-        <v>1389.369430659761</v>
+        <v>1.265403526552392</v>
+      </c>
+      <c r="O19" t="s">
+        <v>65</v>
       </c>
       <c r="P19">
-        <v>2393.651718885077</v>
-      </c>
-      <c r="Q19">
-        <v>0.5952996901732406</v>
+        <v>1389.369472235323</v>
+      </c>
+      <c r="R19">
+        <v>1734.069664924798</v>
       </c>
       <c r="S19">
-        <v>2.802381365123558</v>
+        <v>1389.369422232823</v>
       </c>
       <c r="T19">
-        <v>0.2543481489192311</v>
+        <v>2394.394673795377</v>
       </c>
       <c r="U19">
-        <v>1.190599380346481</v>
-      </c>
-      <c r="V19" t="s">
-        <v>61</v>
+        <v>0.5951991800405249</v>
       </c>
       <c r="W19">
-        <v>1266.305772354336</v>
+        <v>3.081093746093225</v>
       </c>
       <c r="X19">
-        <v>159.1157897414787</v>
+        <v>0.2554292567826676</v>
       </c>
       <c r="Y19">
-        <v>0.6917691931164938</v>
-      </c>
-      <c r="Z19">
-        <v>1410.596949001928</v>
+        <v>1.19039836008105</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>65</v>
       </c>
       <c r="AA19">
-        <v>239.8587767954723</v>
+        <v>1266.305772132352</v>
       </c>
       <c r="AB19">
-        <v>0.6032884694454883</v>
+        <v>159.1159683540576</v>
       </c>
       <c r="AC19">
-        <v>1371.198717966375</v>
+        <v>0.6917689508095292</v>
       </c>
       <c r="AD19">
-        <v>37.31738339880147</v>
+        <v>1410.596943087426</v>
       </c>
       <c r="AE19">
-        <v>0.2973297735619808</v>
+        <v>239.9916109260897</v>
+      </c>
+      <c r="AF19">
+        <v>0.6030968802307942</v>
+      </c>
+      <c r="AG19">
+        <v>1372.683385870967</v>
+      </c>
+      <c r="AH19">
+        <v>2.090000749131144</v>
+      </c>
+      <c r="AI19">
+        <v>0.2973297400900483</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:35">
       <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>102.7689794887103</v>
-      </c>
-      <c r="D20">
-        <v>1286.609900273825</v>
-      </c>
-      <c r="E20">
-        <v>1029.2549005618</v>
+        <v>102.7689719120613</v>
       </c>
       <c r="F20">
-        <v>1286.609950276325</v>
+        <v>1286.609900147807</v>
       </c>
       <c r="G20">
-        <v>1500.314132759151</v>
+        <v>0.00143</v>
       </c>
       <c r="H20">
-        <v>0.6237609513586436</v>
+        <v>1029.254437868277</v>
       </c>
       <c r="I20">
-        <v>2.522793502206889</v>
+        <v>1286.609950150307</v>
       </c>
       <c r="J20">
-        <v>0.2762486708982922</v>
+        <v>1500.31350357264</v>
       </c>
       <c r="K20">
-        <v>1.247521902717287</v>
-      </c>
-      <c r="L20" t="s">
-        <v>61</v>
+        <v>0.623761509536745</v>
+      </c>
+      <c r="L20">
+        <v>2.52279136986443</v>
       </c>
       <c r="M20">
-        <v>1389.378979767536</v>
+        <v>0.2762462276161498</v>
       </c>
       <c r="N20">
-        <v>1592.141270224328</v>
-      </c>
-      <c r="O20">
-        <v>1389.378929765036</v>
+        <v>1.24752301907349</v>
+      </c>
+      <c r="O20" t="s">
+        <v>65</v>
       </c>
       <c r="P20">
-        <v>2181.878914922019</v>
-      </c>
-      <c r="Q20">
-        <v>0.5904119010150402</v>
+        <v>1389.378972064869</v>
+      </c>
+      <c r="R20">
+        <v>1592.142017277545</v>
       </c>
       <c r="S20">
-        <v>2.50820168731024</v>
+        <v>1389.378922062369</v>
       </c>
       <c r="T20">
-        <v>0.2568924153925117</v>
+        <v>2181.879939253626</v>
       </c>
       <c r="U20">
-        <v>1.18082380203008</v>
-      </c>
-      <c r="V20" t="s">
-        <v>61</v>
+        <v>0.5904113503049053</v>
       </c>
       <c r="W20">
-        <v>1266.33277255706</v>
+        <v>2.508229900713894</v>
       </c>
       <c r="X20">
-        <v>157.9680420752773</v>
+        <v>0.2568950697193793</v>
       </c>
       <c r="Y20">
-        <v>0.6127682998931486</v>
-      </c>
-      <c r="Z20">
-        <v>1410.623123729524</v>
+        <v>1.180822700609811</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>65</v>
       </c>
       <c r="AA20">
-        <v>200.7081080173188</v>
+        <v>1266.332772569196</v>
       </c>
       <c r="AB20">
-        <v>0.6342350345717293</v>
+        <v>157.9681117429605</v>
       </c>
       <c r="AC20">
-        <v>1371.206423841171</v>
+        <v>0.6127681757915584</v>
       </c>
       <c r="AD20">
-        <v>31.34711414758716</v>
+        <v>1410.623124127106</v>
       </c>
       <c r="AE20">
-        <v>0.2949201312387029</v>
+        <v>200.708113523828</v>
+      </c>
+      <c r="AF20">
+        <v>0.6342349870022564</v>
+      </c>
+      <c r="AG20">
+        <v>1371.206208516615</v>
+      </c>
+      <c r="AH20">
+        <v>31.34689526877638</v>
+      </c>
+      <c r="AI20">
+        <v>0.2949199428794577</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:35">
       <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C21">
-        <v>102.7602549881556</v>
-      </c>
-      <c r="D21">
-        <v>1286.618257176851</v>
-      </c>
-      <c r="E21">
-        <v>869.1146945409023</v>
+        <v>102.7602610841025</v>
       </c>
       <c r="F21">
-        <v>1286.618307179351</v>
+        <v>1286.618255768769</v>
       </c>
       <c r="G21">
-        <v>1250.243120965858</v>
+        <v>0.00183</v>
       </c>
       <c r="H21">
-        <v>0.6332228980569864</v>
+        <v>869.1157430401952</v>
       </c>
       <c r="I21">
-        <v>2.456909289090282</v>
+        <v>1286.618305771269</v>
       </c>
       <c r="J21">
-        <v>0.1951176699802035</v>
+        <v>1250.244634384739</v>
       </c>
       <c r="K21">
-        <v>1.266445796113973</v>
-      </c>
-      <c r="L21" t="s">
-        <v>61</v>
+        <v>0.6332213252611365</v>
+      </c>
+      <c r="L21">
+        <v>2.456918365709782</v>
       </c>
       <c r="M21">
-        <v>1389.378612170007</v>
+        <v>0.1951249024560196</v>
       </c>
       <c r="N21">
-        <v>1391.178885467967</v>
-      </c>
-      <c r="O21">
-        <v>1389.378562167507</v>
+        <v>1.266442650522273</v>
+      </c>
+      <c r="O21" t="s">
+        <v>65</v>
       </c>
       <c r="P21">
-        <v>1895.855508838905</v>
-      </c>
-      <c r="Q21">
-        <v>0.5834379633905648</v>
+        <v>1389.378616857871</v>
+      </c>
+      <c r="R21">
+        <v>1391.178505754601</v>
       </c>
       <c r="S21">
-        <v>2.275626925724155</v>
+        <v>1389.378566855371</v>
       </c>
       <c r="T21">
-        <v>0.2747691552842937</v>
+        <v>1895.855049607739</v>
       </c>
       <c r="U21">
-        <v>1.16687592678113</v>
-      </c>
-      <c r="V21" t="s">
-        <v>61</v>
+        <v>0.5834382813884054</v>
       </c>
       <c r="W21">
-        <v>1266.318666399171</v>
+        <v>2.275619967584088</v>
       </c>
       <c r="X21">
-        <v>122.4809999503466</v>
+        <v>0.2747677007865592</v>
       </c>
       <c r="Y21">
-        <v>0.694902043778967</v>
-      </c>
-      <c r="Z21">
-        <v>1410.617805634818</v>
+        <v>1.166876562776811</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>65</v>
       </c>
       <c r="AA21">
-        <v>185.1406934205082</v>
+        <v>1266.318666461496</v>
       </c>
       <c r="AB21">
-        <v>0.6086691799254328</v>
+        <v>122.4809359100691</v>
       </c>
       <c r="AC21">
-        <v>1371.199691424227</v>
+        <v>0.6949018867091679</v>
       </c>
       <c r="AD21">
-        <v>28.88615436833313</v>
+        <v>1410.617805704099</v>
       </c>
       <c r="AE21">
-        <v>0.2914073760272995</v>
+        <v>185.1406816347607</v>
+      </c>
+      <c r="AF21">
+        <v>0.6086692417715888</v>
+      </c>
+      <c r="AG21">
+        <v>1371.199690057767</v>
+      </c>
+      <c r="AH21">
+        <v>28.88581738337454</v>
+      </c>
+      <c r="AI21">
+        <v>0.2914073765873408</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:35">
       <c r="A22" s="1">
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>102.7518596730088</v>
+        <v>102.7518731468704</v>
       </c>
       <c r="D22">
-        <v>1286.640249307461</v>
+        <v>0.001675</v>
       </c>
       <c r="E22">
-        <v>750.9685694522033</v>
+        <v>0.001218533955210112</v>
       </c>
       <c r="F22">
-        <v>1286.640299309961</v>
+        <v>1286.640248463998</v>
       </c>
       <c r="G22">
-        <v>1062.866568011053</v>
+        <v>0.000635</v>
       </c>
       <c r="H22">
-        <v>0.6157656424782504</v>
+        <v>750.9688354372702</v>
       </c>
       <c r="I22">
-        <v>2.422793194246156</v>
+        <v>1286.640298466498</v>
       </c>
       <c r="J22">
-        <v>0.2288932396982626</v>
+        <v>1062.86707453755</v>
       </c>
       <c r="K22">
-        <v>1.231531284956501</v>
-      </c>
-      <c r="L22" t="s">
-        <v>61</v>
+        <v>0.6157652272220931</v>
+      </c>
+      <c r="L22">
+        <v>2.422797154313316</v>
       </c>
       <c r="M22">
-        <v>1389.39220898547</v>
+        <v>0.2288955292752605</v>
       </c>
       <c r="N22">
-        <v>1184.450729671749</v>
-      </c>
-      <c r="O22">
-        <v>1389.39215898297</v>
+        <v>1.231530454444186</v>
+      </c>
+      <c r="O22" t="s">
+        <v>65</v>
       </c>
       <c r="P22">
-        <v>1601.612550302124</v>
+        <v>1389.392221615869</v>
       </c>
       <c r="Q22">
-        <v>0.5875994247040471</v>
+        <v>0.00104</v>
+      </c>
+      <c r="R22">
+        <v>1184.449414069262</v>
       </c>
       <c r="S22">
-        <v>2.110597926896039</v>
+        <v>1389.392171613369</v>
       </c>
       <c r="T22">
-        <v>0.2323265997385895</v>
+        <v>1601.610566246641</v>
       </c>
       <c r="U22">
-        <v>1.175198849408094</v>
-      </c>
-      <c r="V22" t="s">
-        <v>61</v>
+        <v>0.5876006684207854</v>
       </c>
       <c r="W22">
-        <v>1266.296042546385</v>
+        <v>2.110571388063803</v>
       </c>
       <c r="X22">
-        <v>95.39792720903972</v>
+        <v>0.2323201570047335</v>
       </c>
       <c r="Y22">
-        <v>0.6558147417112382</v>
-      </c>
-      <c r="Z22">
-        <v>1410.639581620821</v>
+        <v>1.175201336841571</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>65</v>
       </c>
       <c r="AA22">
-        <v>152.0123995470733</v>
+        <v>1266.296042570815</v>
       </c>
       <c r="AB22">
-        <v>0.6132423860815234</v>
+        <v>95.39795068665839</v>
       </c>
       <c r="AC22">
-        <v>1370.833542915834</v>
+        <v>0.6558146636274728</v>
       </c>
       <c r="AD22">
-        <v>22.79568893819633</v>
+        <v>1410.639581620845</v>
       </c>
       <c r="AE22">
-        <v>0.2935149673504886</v>
+        <v>152.0124241854188</v>
+      </c>
+      <c r="AF22">
+        <v>0.6132423788131017</v>
+      </c>
+      <c r="AG22">
+        <v>1370.833553059655</v>
+      </c>
+      <c r="AH22">
+        <v>22.79458870662697</v>
+      </c>
+      <c r="AI22">
+        <v>0.2935149611925038</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:35">
       <c r="A23" s="1">
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C23">
-        <v>102.7539165274343</v>
-      </c>
-      <c r="D23">
-        <v>1286.643882296167</v>
-      </c>
-      <c r="E23">
-        <v>644.8888766024328</v>
+        <v>102.7539184948616</v>
       </c>
       <c r="F23">
-        <v>1286.643932298667</v>
-      </c>
-      <c r="G23">
-        <v>903.9231161296987</v>
+        <v>1286.643880416629</v>
       </c>
       <c r="H23">
-        <v>0.6164966184412464</v>
+        <v>644.8889172444638</v>
       </c>
       <c r="I23">
-        <v>2.079445467705545</v>
+        <v>1286.643930419129</v>
       </c>
       <c r="J23">
-        <v>0.1974298408958717</v>
+        <v>903.9230833677728</v>
       </c>
       <c r="K23">
-        <v>1.232993236882493</v>
-      </c>
-      <c r="L23" t="s">
-        <v>61</v>
+        <v>0.6164965214377255</v>
+      </c>
+      <c r="L23">
+        <v>2.079447600751909</v>
       </c>
       <c r="M23">
-        <v>1389.397898828601</v>
+        <v>0.1974300096017826</v>
       </c>
       <c r="N23">
-        <v>1011.989341738323</v>
-      </c>
-      <c r="O23">
-        <v>1389.397848826101</v>
+        <v>1.232993042875451</v>
+      </c>
+      <c r="O23" t="s">
+        <v>65</v>
       </c>
       <c r="P23">
-        <v>1351.286529060383</v>
+        <v>1389.397898916491</v>
       </c>
       <c r="Q23">
-        <v>0.5865561359635105</v>
+        <v>0.00133</v>
+      </c>
+      <c r="R23">
+        <v>1011.988248429066</v>
       </c>
       <c r="S23">
-        <v>2.098082548923337</v>
+        <v>1389.397848913991</v>
       </c>
       <c r="T23">
-        <v>0.2011140350461263</v>
+        <v>1351.285016208558</v>
       </c>
       <c r="U23">
-        <v>1.173112271927021</v>
-      </c>
-      <c r="V23" t="s">
-        <v>61</v>
+        <v>0.5865573610916996</v>
       </c>
       <c r="W23">
-        <v>1266.358352802967</v>
+        <v>2.098068931806045</v>
       </c>
       <c r="X23">
-        <v>76.75604604147149</v>
+        <v>0.2011078611746406</v>
       </c>
       <c r="Y23">
-        <v>0.694146404531003</v>
-      </c>
-      <c r="Z23">
-        <v>1410.613851496023</v>
+        <v>1.173114722183399</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>65</v>
       </c>
       <c r="AA23">
-        <v>129.4427316367816</v>
+        <v>1266.358352835361</v>
       </c>
       <c r="AB23">
-        <v>0.6054108488747055</v>
+        <v>76.75604393487586</v>
+      </c>
+      <c r="AC23">
+        <v>0.6941464113149803</v>
+      </c>
+      <c r="AD23">
+        <v>1410.61385297202</v>
+      </c>
+      <c r="AE23">
+        <v>129.442653492253</v>
+      </c>
+      <c r="AF23">
+        <v>0.6054114123296602</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:35">
       <c r="A24" s="1">
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C24">
-        <v>102.7588379916078</v>
-      </c>
-      <c r="D24">
-        <v>1286.652535302072</v>
-      </c>
-      <c r="E24">
-        <v>516.7397310338679</v>
+        <v>102.7588262154188</v>
       </c>
       <c r="F24">
-        <v>1286.652585304572</v>
-      </c>
-      <c r="G24">
-        <v>708.9233884756954</v>
+        <v>1286.652539124805</v>
       </c>
       <c r="H24">
-        <v>0.6019904320726215</v>
+        <v>516.7400623057168</v>
       </c>
       <c r="I24">
-        <v>1.977680782641692</v>
+        <v>1286.652589127305</v>
       </c>
       <c r="J24">
-        <v>0.2043037577204701</v>
+        <v>708.9240860289054</v>
       </c>
       <c r="K24">
-        <v>1.203980864145243</v>
-      </c>
-      <c r="L24" t="s">
-        <v>61</v>
+        <v>0.6019897191602857</v>
+      </c>
+      <c r="L24">
+        <v>1.977681976479061</v>
       </c>
       <c r="M24">
-        <v>1389.41147329868</v>
+        <v>0.2043081818531133</v>
       </c>
       <c r="N24">
-        <v>792.8748756987965</v>
-      </c>
-      <c r="O24">
-        <v>1389.411423296179</v>
+        <v>1.203979438320571</v>
+      </c>
+      <c r="O24" t="s">
+        <v>65</v>
       </c>
       <c r="P24">
-        <v>1051.576452461019</v>
-      </c>
-      <c r="Q24">
-        <v>0.586914502253468</v>
+        <v>1389.411465345224</v>
+      </c>
+      <c r="R24">
+        <v>792.9448128715991</v>
       </c>
       <c r="S24">
-        <v>1.908213892908063</v>
+        <v>1389.411415342724</v>
       </c>
       <c r="T24">
-        <v>0.179662738072615</v>
+        <v>1051.898793616349</v>
       </c>
       <c r="U24">
-        <v>1.173829004506936</v>
-      </c>
-      <c r="V24" t="s">
-        <v>61</v>
+        <v>0.5868226947242257</v>
       </c>
       <c r="W24">
-        <v>1266.37089393655</v>
+        <v>2.034857871515118</v>
       </c>
       <c r="X24">
-        <v>59.80135293711445</v>
+        <v>0.1807415312027706</v>
       </c>
       <c r="Y24">
-        <v>0.6480678029098932</v>
-      </c>
-      <c r="Z24">
-        <v>1410.642629178318</v>
+        <v>1.173645389448451</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>65</v>
       </c>
       <c r="AA24">
-        <v>100.3219157639923</v>
+        <v>1266.37089434768</v>
       </c>
       <c r="AB24">
-        <v>0.5819477791008685</v>
+        <v>59.80124269598025</v>
       </c>
       <c r="AC24">
-        <v>1371.212343793769</v>
+        <v>0.6480697016290011</v>
       </c>
       <c r="AD24">
-        <v>18.68050255317641</v>
+        <v>1410.642629847099</v>
       </c>
       <c r="AE24">
-        <v>0.2931767077778053</v>
+        <v>100.378243717975</v>
+      </c>
+      <c r="AF24">
+        <v>0.5817608708021854</v>
+      </c>
+      <c r="AG24">
+        <v>1369.437022511488</v>
+      </c>
+      <c r="AH24">
+        <v>3.380230752839193</v>
+      </c>
+      <c r="AI24">
+        <v>0.2931767092253595</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C25">
-        <v>102.7469533834205</v>
-      </c>
-      <c r="D25">
-        <v>1286.664022271742</v>
-      </c>
-      <c r="E25">
-        <v>369.83874808629</v>
+        <v>102.7469606169641</v>
       </c>
       <c r="F25">
-        <v>1286.664022271742</v>
-      </c>
-      <c r="G25">
-        <v>491.8260259938971</v>
+        <v>1286.664017398754</v>
       </c>
       <c r="H25">
-        <v>0.6112789455515807</v>
+        <v>369.8389927018004</v>
       </c>
       <c r="I25">
-        <v>1.970997706427495</v>
+        <v>1286.664017398754</v>
       </c>
       <c r="J25">
-        <v>0.06640829204766546</v>
+        <v>491.8266773563823</v>
       </c>
       <c r="K25">
-        <v>1.222557891103161</v>
-      </c>
-      <c r="L25" t="s">
-        <v>61</v>
+        <v>0.611278174530538</v>
+      </c>
+      <c r="L25">
+        <v>1.971002198859888</v>
       </c>
       <c r="M25">
-        <v>1389.411025657663</v>
+        <v>0.0664141340161612</v>
       </c>
       <c r="N25">
-        <v>579.8559846594546</v>
-      </c>
-      <c r="O25">
-        <v>1389.410975655163</v>
+        <v>1.222556349061076</v>
+      </c>
+      <c r="O25" t="s">
+        <v>65</v>
       </c>
       <c r="P25">
-        <v>766.0534430724414</v>
+        <v>1389.411028018218</v>
       </c>
       <c r="Q25">
-        <v>0.581247090867435</v>
+        <v>0.00228</v>
+      </c>
+      <c r="R25">
+        <v>579.8559416747313</v>
       </c>
       <c r="S25">
-        <v>1.925110071013741</v>
+        <v>1389.410978015718</v>
       </c>
       <c r="T25">
-        <v>0.1965391379775942</v>
+        <v>766.0533195650653</v>
       </c>
       <c r="U25">
-        <v>1.16249418173487</v>
-      </c>
-      <c r="V25" t="s">
-        <v>61</v>
+        <v>0.5812471601064908</v>
       </c>
       <c r="W25">
-        <v>1266.349327929512</v>
+        <v>1.925108776966211</v>
       </c>
       <c r="X25">
-        <v>32.75049024605481</v>
+        <v>0.1965385388217322</v>
       </c>
       <c r="Y25">
-        <v>0.5764999768004097</v>
-      </c>
-      <c r="Z25">
-        <v>1410.633980762814</v>
+        <v>1.162494320212982</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>65</v>
       </c>
       <c r="AA25">
-        <v>74.86176232757536</v>
+        <v>1266.349327948957</v>
       </c>
       <c r="AB25">
-        <v>0.5819798218990326</v>
+        <v>32.75050151801313</v>
+      </c>
+      <c r="AC25">
+        <v>0.576499779564984</v>
+      </c>
+      <c r="AD25">
+        <v>1410.633980810806</v>
+      </c>
+      <c r="AE25">
+        <v>74.86176745341729</v>
+      </c>
+      <c r="AF25">
+        <v>0.5819797521974224</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C26">
-        <v>102.7261001583615</v>
-      </c>
-      <c r="D26">
-        <v>1286.691024491005</v>
-      </c>
-      <c r="E26">
-        <v>254.1733638664989</v>
+        <v>102.7261013957564</v>
       </c>
       <c r="F26">
-        <v>1286.691024491005</v>
-      </c>
-      <c r="G26">
-        <v>328.4211387894678</v>
+        <v>1286.691022302416</v>
       </c>
       <c r="H26">
-        <v>0.6068888449918776</v>
+        <v>254.1738183660939</v>
       </c>
       <c r="I26">
-        <v>1.962700380458444</v>
+        <v>1286.691022302416</v>
       </c>
       <c r="J26">
-        <v>0.0002121733182155472</v>
+        <v>328.4230722390374</v>
       </c>
       <c r="K26">
-        <v>1.213777689983755</v>
-      </c>
-      <c r="L26" t="s">
-        <v>61</v>
+        <v>0.6068868614370199</v>
+      </c>
+      <c r="L26">
+        <v>1.962703469782377</v>
       </c>
       <c r="M26">
-        <v>1389.417174651867</v>
+        <v>0.0002350275441995731</v>
       </c>
       <c r="N26">
-        <v>403.3441408237041</v>
-      </c>
-      <c r="O26">
-        <v>1389.417124649367</v>
+        <v>1.21377372287404</v>
+      </c>
+      <c r="O26" t="s">
+        <v>65</v>
       </c>
       <c r="P26">
-        <v>521.1721290840036</v>
+        <v>1389.417173700672</v>
       </c>
       <c r="Q26">
-        <v>0.5799251971090322</v>
+        <v>0.00251</v>
+      </c>
+      <c r="R26">
+        <v>403.3441591565559</v>
       </c>
       <c r="S26">
-        <v>1.695961085248344</v>
+        <v>1389.417123698172</v>
       </c>
       <c r="T26">
-        <v>0.1380799287791341</v>
+        <v>521.1721870804433</v>
       </c>
       <c r="U26">
-        <v>1.159850394218064</v>
-      </c>
-      <c r="V26" t="s">
-        <v>61</v>
+        <v>0.5799251551644382</v>
       </c>
       <c r="W26">
-        <v>1266.362019140041</v>
+        <v>1.695961527078159</v>
       </c>
       <c r="X26">
-        <v>27.1757614928028</v>
+        <v>0.1380803386491486</v>
       </c>
       <c r="Y26">
-        <v>0.6427439164305394</v>
-      </c>
-      <c r="Z26">
-        <v>1410.682841356761</v>
+        <v>1.159850310328876</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>65</v>
       </c>
       <c r="AA26">
-        <v>49.43144476194074</v>
+        <v>1266.362019146426</v>
       </c>
       <c r="AB26">
-        <v>0.5917361688797748</v>
+        <v>27.17575084310541</v>
+      </c>
+      <c r="AC26">
+        <v>0.6427437398759817</v>
+      </c>
+      <c r="AD26">
+        <v>1410.682841314734</v>
+      </c>
+      <c r="AE26">
+        <v>49.43147424978309</v>
+      </c>
+      <c r="AF26">
+        <v>0.5917359852045998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>